<commit_message>
Chnaged Sheyway name to Folkestone and Hyde
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Alex\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF4C8BE-DAA9-4892-AFDC-48785357C630}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F16C58D3-F5C3-494D-8121-153DFEA1AB12}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="10260" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="10260" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,18 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6093" uniqueCount="4079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6095" uniqueCount="4081">
   <si>
     <t>register</t>
   </si>
@@ -12260,6 +12267,12 @@
   </si>
   <si>
     <t>7000000000029630</t>
+  </si>
+  <si>
+    <t>Folkestone and Hythe District Council</t>
+  </si>
+  <si>
+    <t>Folkestone and Hythe</t>
   </si>
 </sst>
 </file>
@@ -16480,8 +16493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="U409" sqref="U409"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I255" sqref="I255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30076,9 +30089,15 @@
         <v>66</v>
       </c>
       <c r="I259" t="s">
+        <v>4079</v>
+      </c>
+      <c r="J259" t="s">
+        <v>4080</v>
+      </c>
+      <c r="K259" t="s">
         <v>2231</v>
       </c>
-      <c r="J259" t="s">
+      <c r="L259" t="s">
         <v>2232</v>
       </c>
       <c r="M259" t="s">

</xml_diff>

<commit_message>
Adjusted new css codes for Fife and Perth
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Alex\Dropbox\mysociety\uk_local_authority_lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Alex\Dropbox\mysociety\postcode_convert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F16C58D3-F5C3-494D-8121-153DFEA1AB12}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E928CC-E327-4E0C-A900-1723EBD156DE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="10260" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="10260" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6095" uniqueCount="4081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6097" uniqueCount="4083">
   <si>
     <t>register</t>
   </si>
@@ -12273,6 +12273,12 @@
   </si>
   <si>
     <t>Folkestone and Hythe</t>
+  </si>
+  <si>
+    <t>S12000047</t>
+  </si>
+  <si>
+    <t>S12000048</t>
   </si>
 </sst>
 </file>
@@ -16493,8 +16499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y445"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I255" sqref="I255"/>
+    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="P415" sqref="P415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36712,6 +36718,9 @@
         <v>38521</v>
       </c>
       <c r="P406" t="s">
+        <v>4081</v>
+      </c>
+      <c r="Q406" t="s">
         <v>3379</v>
       </c>
       <c r="S406" t="s">
@@ -37072,6 +37081,9 @@
         <v>38521</v>
       </c>
       <c r="P415" t="s">
+        <v>4082</v>
+      </c>
+      <c r="Q415" t="s">
         <v>3453</v>
       </c>
       <c r="S415" t="s">
@@ -38461,5 +38473,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add some missing mapit and wdtk ids
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisecrow/dev/uk_local_authority_names_and_codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3104E7-D09F-4991-946A-DECD79132F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35869CF8-FC1D-6540-90C1-31AAE9C0A22E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">uk_local_authorities!$A$1:$AD$458</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6388" uniqueCount="4315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6393" uniqueCount="4315">
   <si>
     <t>register</t>
   </si>
@@ -12984,7 +12974,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13827,30 +13817,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z378" sqref="Z378"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="56.140625" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="2"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="56.1640625" customWidth="1"/>
+    <col min="24" max="24" width="9.1640625" style="2"/>
+    <col min="25" max="25" width="5.83203125" customWidth="1"/>
+    <col min="26" max="26" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13942,7 +13935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" hidden="1">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -14001,7 +13994,7 @@
         <v>-0.29853079768066898</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" hidden="1">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -14060,7 +14053,7 @@
         <v>-3.24722422689331</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" hidden="1">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -14119,7 +14112,7 @@
         <v>-1.46665873702776</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" hidden="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -14178,7 +14171,7 @@
         <v>-0.56818848880294304</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" hidden="1">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -14237,7 +14230,7 @@
         <v>0.81129819917048196</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" hidden="1">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -14296,7 +14289,7 @@
         <v>-1.2591513419243701</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" hidden="1">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -14355,7 +14348,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" hidden="1">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -14414,7 +14407,7 @@
         <v>0.91533728957657501</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" hidden="1">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -14473,7 +14466,7 @@
         <v>-0.95891662147405199</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" hidden="1">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -14532,7 +14525,7 @@
         <v>0.46629089418242597</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" hidden="1">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -14594,7 +14587,7 @@
         <v>-1.2009435841509399</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" hidden="1">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -14653,7 +14646,7 @@
         <v>-3.2122852055299398</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" hidden="1">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -14721,7 +14714,7 @@
         <v>-2.4752562946031902</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" hidden="1">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -14789,7 +14782,7 @@
         <v>-2.4675476946073398</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" hidden="1">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -14857,7 +14850,7 @@
         <v>-0.47708243486090501</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" hidden="1">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -14919,7 +14912,7 @@
         <v>0.13316440100825999</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" hidden="1">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -14978,7 +14971,7 @@
         <v>-0.26781131950910397</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" hidden="1">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -15037,7 +15030,7 @@
         <v>0.142348001531232</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" hidden="1">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -15102,7 +15095,7 @@
         <v>-1.8748023729485099</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" hidden="1">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -15167,7 +15160,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" hidden="1">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -15226,7 +15219,7 @@
         <v>-1.22196189843978</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" hidden="1">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -15291,7 +15284,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" hidden="1">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -15350,7 +15343,7 @@
         <v>-0.21001736105659499</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" hidden="1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -15418,7 +15411,7 @@
         <v>-0.13313545319187201</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" hidden="1">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -15483,7 +15476,7 @@
         <v>-1.53257458326465</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" hidden="1">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -15548,7 +15541,7 @@
         <v>-2.4669702024590698</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" hidden="1">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -15607,7 +15600,7 @@
         <v>-1.2773246814138699</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" hidden="1">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -15666,7 +15659,7 @@
         <v>-2.2346840889682799E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -15700,11 +15693,17 @@
       <c r="S30" t="s">
         <v>4150</v>
       </c>
+      <c r="Z30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA30">
+        <v>91513</v>
+      </c>
       <c r="AC30">
         <v>-1.8832767543704001</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" hidden="1">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -15772,7 +15771,7 @@
         <v>-3.0355263398194898</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" hidden="1">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -15831,7 +15830,7 @@
         <v>0.58993191534261002</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" hidden="1">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -15899,7 +15898,7 @@
         <v>-0.73973762236580598</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" hidden="1">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -15964,7 +15963,7 @@
         <v>-1.8546713065720899</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" hidden="1">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -16023,7 +16022,7 @@
         <v>0.83727582982422</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" hidden="1">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -16082,7 +16081,7 @@
         <v>-2.0160150229923799</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" hidden="1">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -16141,7 +16140,7 @@
         <v>1.3106131362756599</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" hidden="1">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -16200,7 +16199,7 @@
         <v>-1.26209487685358</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" hidden="1">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -16259,7 +16258,7 @@
         <v>0.31075979004458298</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" hidden="1">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -16318,7 +16317,7 @@
         <v>-4.7375277037571301E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" hidden="1">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -16377,7 +16376,7 @@
         <v>5.1537722669066997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" hidden="1">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -16448,7 +16447,7 @@
         <v>-2.7708323519360398</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" hidden="1">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -16507,7 +16506,7 @@
         <v>-2.2219452917805902</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" hidden="1">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -16572,7 +16571,7 @@
         <v>-2.3125533828838001</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" hidden="1">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -16631,7 +16630,7 @@
         <v>0.13292340916676401</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" hidden="1">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -16687,7 +16686,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" hidden="1">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -16746,7 +16745,7 @@
         <v>-1.9802318640761301</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" hidden="1">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -16805,7 +16804,7 @@
         <v>-2.8092503063009899</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" hidden="1">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -16864,7 +16863,7 @@
         <v>0.59469378383326399</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" hidden="1">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -16923,7 +16922,7 @@
         <v>1.10181619758618</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" hidden="1">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -16991,7 +16990,7 @@
         <v>-0.43629195492780098</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" hidden="1">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -17050,7 +17049,7 @@
         <v>-1.14613584536538</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" hidden="1">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -17109,7 +17108,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" hidden="1">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -17177,7 +17176,7 @@
         <v>-2.34994253283099</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" hidden="1">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -17239,7 +17238,7 @@
         <v>-0.74226375153748902</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" hidden="1">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -17298,7 +17297,7 @@
         <v>0.480915957502693</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" hidden="1">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -17357,7 +17356,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" hidden="1">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -17416,7 +17415,7 @@
         <v>-2.6478813276136002</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" hidden="1">
       <c r="A59" t="s">
         <v>24</v>
       </c>
@@ -17475,7 +17474,7 @@
         <v>-1.27559517385222</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" hidden="1">
       <c r="A60" t="s">
         <v>24</v>
       </c>
@@ -17534,7 +17533,7 @@
         <v>-1.40123094254592</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" hidden="1">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -17593,7 +17592,7 @@
         <v>-2.0740223238436202</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" hidden="1">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -17661,7 +17660,7 @@
         <v>-2.7358562336485499</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" hidden="1">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -17726,7 +17725,7 @@
         <v>-1.9734126331777899</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" hidden="1">
       <c r="A64" t="s">
         <v>24</v>
       </c>
@@ -17782,7 +17781,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" hidden="1">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -17841,7 +17840,7 @@
         <v>-0.157415056241972</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" hidden="1">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -17900,7 +17899,7 @@
         <v>0.86090231976730502</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" hidden="1">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -17968,7 +17967,7 @@
         <v>-4.9482176397012996</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" hidden="1">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -18027,7 +18026,7 @@
         <v>-3.3731363138071</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" hidden="1">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -18086,7 +18085,7 @@
         <v>-0.69591855896418098</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" hidden="1">
       <c r="A70" t="s">
         <v>24</v>
       </c>
@@ -18145,7 +18144,7 @@
         <v>-1.8929521615162299</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" hidden="1">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -18210,7 +18209,7 @@
         <v>-1.5197503068760101</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29">
       <c r="A72" t="s">
         <v>24</v>
       </c>
@@ -18232,8 +18231,11 @@
       <c r="N72" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA72">
+        <v>64630</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" hidden="1">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -18292,7 +18294,7 @@
         <v>-2.1742510400716202</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" hidden="1">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -18354,7 +18356,7 @@
         <v>-0.18203462265567399</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" hidden="1">
       <c r="A75" t="s">
         <v>24</v>
       </c>
@@ -18413,7 +18415,7 @@
         <v>-8.7165024613834005E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" hidden="1">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -18472,7 +18474,7 @@
         <v>-0.54087696974008204</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" hidden="1">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -18540,7 +18542,7 @@
         <v>-1.5525857155965399</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" hidden="1">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -18599,7 +18601,7 @@
         <v>0.25316777724608802</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" hidden="1">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -18658,7 +18660,7 @@
         <v>-1.04824667885277</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" hidden="1">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -18714,7 +18716,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" hidden="1">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -18773,7 +18775,7 @@
         <v>-1.69368006706174</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" hidden="1">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -18841,7 +18843,7 @@
         <v>-1.4683439126002999</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" hidden="1">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -18897,7 +18899,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" hidden="1">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -18962,7 +18964,7 @@
         <v>-1.0957642741408999</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" hidden="1">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -19024,7 +19026,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" hidden="1">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -19083,7 +19085,7 @@
         <v>1.2892144193203501</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -19111,11 +19113,17 @@
       <c r="Q87" t="s">
         <v>4107</v>
       </c>
+      <c r="Z87" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA87">
+        <v>91365</v>
+      </c>
       <c r="AC87">
         <v>-2.3335558746994098</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" hidden="1">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -19180,7 +19188,7 @@
         <v>-2.1087361271354599</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" hidden="1">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -19251,7 +19259,7 @@
         <v>-1.83991172191284</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" hidden="1">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -19310,7 +19318,7 @@
         <v>-0.331018584222806</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" hidden="1">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -19369,7 +19377,7 @@
         <v>0.26622944628692102</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" hidden="1">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -19428,7 +19436,7 @@
         <v>-1.32720068468055</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" hidden="1">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -19487,7 +19495,7 @@
         <v>0.294782697862571</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" hidden="1">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -19546,7 +19554,7 @@
         <v>-3.2243125929424199</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" hidden="1">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -19605,7 +19613,7 @@
         <v>-2.6218219715923099</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" hidden="1">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -19664,7 +19672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29" hidden="1">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -19723,7 +19731,7 @@
         <v>-0.95512420774780105</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" hidden="1">
       <c r="A98" t="s">
         <v>24</v>
       </c>
@@ -19785,7 +19793,7 @@
         <v>-8.2579317821315692E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29" hidden="1">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -19844,7 +19852,7 @@
         <v>3.03338886761347E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29" hidden="1">
       <c r="A100" t="s">
         <v>24</v>
       </c>
@@ -19903,7 +19911,7 @@
         <v>-0.39217250644269003</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29" hidden="1">
       <c r="A101" t="s">
         <v>24</v>
       </c>
@@ -19962,7 +19970,7 @@
         <v>-8.7264502186229706E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29" hidden="1">
       <c r="A102" t="s">
         <v>24</v>
       </c>
@@ -20021,7 +20029,7 @@
         <v>-0.52347974785409601</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29" hidden="1">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -20080,7 +20088,7 @@
         <v>0.14866520769558</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29" hidden="1">
       <c r="A104" t="s">
         <v>24</v>
       </c>
@@ -20142,7 +20150,7 @@
         <v>-0.26144844660503602</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:29" hidden="1">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -20201,7 +20209,7 @@
         <v>-1.3466958468372301</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29" hidden="1">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -20269,7 +20277,7 @@
         <v>-0.48250917149656902</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:29">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -20300,11 +20308,17 @@
       <c r="U107">
         <v>412</v>
       </c>
+      <c r="Z107" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA107">
+        <v>91370</v>
+      </c>
       <c r="AC107">
         <v>1.4614605743951401</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:29" hidden="1">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -20360,7 +20374,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:29" hidden="1">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -20419,7 +20433,7 @@
         <v>-1.81214118182388</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:29" hidden="1">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -20475,7 +20489,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29" hidden="1">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -20534,7 +20548,7 @@
         <v>-3.5101761920371901</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29" hidden="1">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -20593,7 +20607,7 @@
         <v>-1.2246651080011499</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:30" hidden="1">
       <c r="A113" t="s">
         <v>24</v>
       </c>
@@ -20652,7 +20666,7 @@
         <v>6.0771297225044402E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:30" hidden="1">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -20711,7 +20725,7 @@
         <v>-2.4901213839832601</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:30" hidden="1">
       <c r="A115" t="s">
         <v>24</v>
       </c>
@@ -20770,7 +20784,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:30" hidden="1">
       <c r="A116" t="s">
         <v>24</v>
       </c>
@@ -20829,7 +20843,7 @@
         <v>-2.92287972999782</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:30" hidden="1">
       <c r="A117" t="s">
         <v>24</v>
       </c>
@@ -20894,7 +20908,7 @@
         <v>-1.68289087502256</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:30" hidden="1">
       <c r="A118" t="s">
         <v>24</v>
       </c>
@@ -20953,7 +20967,7 @@
         <v>-1.1193100378155301</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:30" hidden="1">
       <c r="A119" t="s">
         <v>24</v>
       </c>
@@ -21003,7 +21017,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:30" hidden="1">
       <c r="A120" t="s">
         <v>24</v>
       </c>
@@ -21062,7 +21076,7 @@
         <v>-2.2402646253741301</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:30" hidden="1">
       <c r="A121" t="s">
         <v>24</v>
       </c>
@@ -21118,7 +21132,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:30">
       <c r="A122" t="s">
         <v>24</v>
       </c>
@@ -21140,8 +21154,11 @@
       <c r="N122" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA122">
+        <v>8211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30" hidden="1">
       <c r="A123" t="s">
         <v>24</v>
       </c>
@@ -21200,7 +21217,7 @@
         <v>-1.1594623667666399</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:30" hidden="1">
       <c r="A124" t="s">
         <v>24</v>
       </c>
@@ -21259,7 +21276,7 @@
         <v>0.39499417091077599</v>
       </c>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:30" hidden="1">
       <c r="A125" t="s">
         <v>24</v>
       </c>
@@ -21318,7 +21335,7 @@
         <v>5.5542716458775301E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" hidden="1">
       <c r="A126" t="s">
         <v>24</v>
       </c>
@@ -21377,7 +21394,7 @@
         <v>-0.56164554240444897</v>
       </c>
     </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:30" hidden="1">
       <c r="A127" t="s">
         <v>24</v>
       </c>
@@ -21436,7 +21453,7 @@
         <v>1.66134793066905</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:30" hidden="1">
       <c r="A128" t="s">
         <v>24</v>
       </c>
@@ -21495,7 +21512,7 @@
         <v>-0.98936169825244902</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29" hidden="1">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -21554,7 +21571,7 @@
         <v>-1.31908778079823</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29" hidden="1">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -21613,7 +21630,7 @@
         <v>-1.59553909500438</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29" hidden="1">
       <c r="A131" t="s">
         <v>24</v>
       </c>
@@ -21681,7 +21698,7 @@
         <v>-2.7187968167260799</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" hidden="1">
       <c r="A132" t="s">
         <v>24</v>
       </c>
@@ -21737,7 +21754,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" hidden="1">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -21796,7 +21813,7 @@
         <v>-1.0081235593811999</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" hidden="1">
       <c r="A134" t="s">
         <v>24</v>
       </c>
@@ -21855,7 +21872,7 @@
         <v>0.108539457994397</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" hidden="1">
       <c r="A135" t="s">
         <v>24</v>
       </c>
@@ -21914,7 +21931,7 @@
         <v>0.57043334791955602</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29" hidden="1">
       <c r="A136" t="s">
         <v>24</v>
       </c>
@@ -21973,7 +21990,7 @@
         <v>-0.89747200545425898</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29" hidden="1">
       <c r="A137" t="s">
         <v>24</v>
       </c>
@@ -22032,7 +22049,7 @@
         <v>0.22042672677428801</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" hidden="1">
       <c r="A138" t="s">
         <v>24</v>
       </c>
@@ -22091,7 +22108,7 @@
         <v>-6.3315272614078294E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" hidden="1">
       <c r="A139" t="s">
         <v>24</v>
       </c>
@@ -22159,7 +22176,7 @@
         <v>-2.7449596144109498</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" hidden="1">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -22218,7 +22235,7 @@
         <v>-0.28109663669281998</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" hidden="1">
       <c r="A141" t="s">
         <v>24</v>
       </c>
@@ -22277,7 +22294,7 @@
         <v>-1.8739385921285301</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" hidden="1">
       <c r="A142" t="s">
         <v>24</v>
       </c>
@@ -22336,7 +22353,7 @@
         <v>-0.44566202430884599</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29" hidden="1">
       <c r="A143" t="s">
         <v>24</v>
       </c>
@@ -22398,7 +22415,7 @@
         <v>-1.3910550818802301</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29" hidden="1">
       <c r="A144" t="s">
         <v>24</v>
       </c>
@@ -22460,7 +22477,7 @@
         <v>-0.220777565101831</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" hidden="1">
       <c r="A145" t="s">
         <v>24</v>
       </c>
@@ -22519,7 +22536,7 @@
         <v>-0.36616172517234102</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" hidden="1">
       <c r="A146" t="s">
         <v>24</v>
       </c>
@@ -22581,7 +22598,7 @@
         <v>-0.36633274976462499</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" hidden="1">
       <c r="A147" t="s">
         <v>24</v>
       </c>
@@ -22649,7 +22666,7 @@
         <v>-1.2556467591787599</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" hidden="1">
       <c r="A148" t="s">
         <v>24</v>
       </c>
@@ -22705,7 +22722,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" hidden="1">
       <c r="A149" t="s">
         <v>24</v>
       </c>
@@ -22764,7 +22781,7 @@
         <v>-0.341274221017002</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" hidden="1">
       <c r="A150" t="s">
         <v>24</v>
       </c>
@@ -22823,7 +22840,7 @@
         <v>-0.10747266739674501</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" hidden="1">
       <c r="A151" t="s">
         <v>24</v>
       </c>
@@ -22882,7 +22899,7 @@
         <v>-0.220773550455199</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" hidden="1">
       <c r="A152" t="s">
         <v>24</v>
       </c>
@@ -22941,7 +22958,7 @@
         <v>-2.3897873278493602</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" hidden="1">
       <c r="A153" t="s">
         <v>24</v>
       </c>
@@ -23006,7 +23023,7 @@
         <v>-6.2987980018748004</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" hidden="1">
       <c r="A154" t="s">
         <v>24</v>
       </c>
@@ -23074,7 +23091,7 @@
         <v>-1.09489649616619</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" hidden="1">
       <c r="A155" t="s">
         <v>24</v>
       </c>
@@ -23133,7 +23150,7 @@
         <v>1.1597791056265001</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" hidden="1">
       <c r="A156" t="s">
         <v>24</v>
       </c>
@@ -23192,7 +23209,7 @@
         <v>-0.110246258249108</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" hidden="1">
       <c r="A157" t="s">
         <v>24</v>
       </c>
@@ -23254,7 +23271,7 @@
         <v>-0.19221075151882699</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" hidden="1">
       <c r="A158" t="s">
         <v>24</v>
       </c>
@@ -23310,7 +23327,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" hidden="1">
       <c r="A159" t="s">
         <v>24</v>
       </c>
@@ -23369,7 +23386,7 @@
         <v>-0.76542910237272799</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" hidden="1">
       <c r="A160" t="s">
         <v>24</v>
       </c>
@@ -23440,7 +23457,7 @@
         <v>-0.33535150963390398</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" hidden="1">
       <c r="A161" t="s">
         <v>24</v>
       </c>
@@ -23505,7 +23522,7 @@
         <v>0.470465345077615</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29" hidden="1">
       <c r="A162" t="s">
         <v>24</v>
       </c>
@@ -23570,7 +23587,7 @@
         <v>-1.76330731290644</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29" hidden="1">
       <c r="A163" t="s">
         <v>24</v>
       </c>
@@ -23629,7 +23646,7 @@
         <v>-0.28691447761787803</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29" hidden="1">
       <c r="A164" t="s">
         <v>24</v>
       </c>
@@ -23694,7 +23711,7 @@
         <v>-2.8340373463497501</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29" hidden="1">
       <c r="A165" t="s">
         <v>24</v>
       </c>
@@ -23753,7 +23770,7 @@
         <v>-2.7147823620064</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29" hidden="1">
       <c r="A166" t="s">
         <v>24</v>
       </c>
@@ -23809,7 +23826,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29" hidden="1">
       <c r="A167" t="s">
         <v>24</v>
       </c>
@@ -23868,7 +23885,7 @@
         <v>-0.118309072522519</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29" hidden="1">
       <c r="A168" t="s">
         <v>24</v>
       </c>
@@ -23939,7 +23956,7 @@
         <v>-1.1284852020846301</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29">
       <c r="A169" t="s">
         <v>24</v>
       </c>
@@ -23961,8 +23978,11 @@
       <c r="N169" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA169">
+        <v>52349</v>
+      </c>
+    </row>
+    <row r="170" spans="1:29" hidden="1">
       <c r="A170" t="s">
         <v>24</v>
       </c>
@@ -24027,7 +24047,7 @@
         <v>-1.50601636692331</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29" hidden="1">
       <c r="A171" t="s">
         <v>24</v>
       </c>
@@ -24083,7 +24103,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29" hidden="1">
       <c r="A172" t="s">
         <v>24</v>
       </c>
@@ -24142,7 +24162,7 @@
         <v>5.0543556228987803E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29" hidden="1">
       <c r="A173" t="s">
         <v>24</v>
       </c>
@@ -24201,7 +24221,7 @@
         <v>-2.0285774043622199E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29" hidden="1">
       <c r="A174" t="s">
         <v>24</v>
       </c>
@@ -24263,7 +24283,7 @@
         <v>-0.55495288760678196</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:29" hidden="1">
       <c r="A175" t="s">
         <v>24</v>
       </c>
@@ -24322,7 +24342,7 @@
         <v>-1.80491531530489</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:29" hidden="1">
       <c r="A176" t="s">
         <v>24</v>
       </c>
@@ -24378,7 +24398,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" hidden="1">
       <c r="A177" t="s">
         <v>24</v>
       </c>
@@ -24443,7 +24463,7 @@
         <v>-2.91700763031041</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" hidden="1">
       <c r="A178" t="s">
         <v>24</v>
       </c>
@@ -24505,7 +24525,7 @@
         <v>-9.2437868622313998E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" hidden="1">
       <c r="A179" t="s">
         <v>24</v>
       </c>
@@ -24573,7 +24593,7 @@
         <v>-0.42559029048565999</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" hidden="1">
       <c r="A180" t="s">
         <v>24</v>
       </c>
@@ -24632,7 +24652,7 @@
         <v>0.58055256446608905</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" hidden="1">
       <c r="A181" t="s">
         <v>24</v>
       </c>
@@ -24691,7 +24711,7 @@
         <v>0.78377739171598204</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:29" hidden="1">
       <c r="A182" t="s">
         <v>24</v>
       </c>
@@ -24756,7 +24776,7 @@
         <v>-2.2325236866808602</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:29" hidden="1">
       <c r="A183" t="s">
         <v>24</v>
       </c>
@@ -24815,7 +24835,7 @@
         <v>-1.1727869589561499</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:29" hidden="1">
       <c r="A184" t="s">
         <v>24</v>
       </c>
@@ -24874,7 +24894,7 @@
         <v>-2.3446652905044201</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" hidden="1">
       <c r="A185" t="s">
         <v>24</v>
       </c>
@@ -24942,7 +24962,7 @@
         <v>-1.2224301962791999</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:29" hidden="1">
       <c r="A186" t="s">
         <v>24</v>
       </c>
@@ -25001,7 +25021,7 @@
         <v>-3.55643798008176</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:29" hidden="1">
       <c r="A187" t="s">
         <v>24</v>
       </c>
@@ -25072,7 +25092,7 @@
         <v>0.56948457324977197</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:29" hidden="1">
       <c r="A188" t="s">
         <v>24</v>
       </c>
@@ -25131,7 +25151,7 @@
         <v>-0.85621855043544903</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:29" hidden="1">
       <c r="A189" t="s">
         <v>24</v>
       </c>
@@ -25190,7 +25210,7 @@
         <v>-2.5446553195065</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:29" hidden="1">
       <c r="A190" t="s">
         <v>24</v>
       </c>
@@ -25258,7 +25278,7 @@
         <v>-0.73354065299243898</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" hidden="1">
       <c r="A191" t="s">
         <v>24</v>
       </c>
@@ -25317,7 +25337,7 @@
         <v>-0.32511597467560699</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" hidden="1">
       <c r="A192" t="s">
         <v>24</v>
       </c>
@@ -25376,7 +25396,7 @@
         <v>-0.19724645978008301</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:29" hidden="1">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -25438,7 +25458,7 @@
         <v>-0.12705176017318801</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:29" hidden="1">
       <c r="A194" t="s">
         <v>24</v>
       </c>
@@ -25497,7 +25517,7 @@
         <v>1.0924171535160601</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:29" hidden="1">
       <c r="A195" t="s">
         <v>24</v>
       </c>
@@ -25565,7 +25585,7 @@
         <v>-2.06647808763908</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:29" hidden="1">
       <c r="A196" t="s">
         <v>24</v>
       </c>
@@ -25624,7 +25644,7 @@
         <v>-3.9145654715471498</v>
       </c>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:29" hidden="1">
       <c r="A197" t="s">
         <v>24</v>
       </c>
@@ -25683,7 +25703,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" hidden="1">
       <c r="A198" t="s">
         <v>24</v>
       </c>
@@ -25745,7 +25765,7 @@
         <v>-0.91974426351731098</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:29" hidden="1">
       <c r="A199" t="s">
         <v>24</v>
       </c>
@@ -25804,7 +25824,7 @@
         <v>-2.3188747363185298</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" hidden="1">
       <c r="A200" t="s">
         <v>24</v>
       </c>
@@ -25863,7 +25883,7 @@
         <v>-1.44828792583317</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" hidden="1">
       <c r="A201" t="s">
         <v>24</v>
       </c>
@@ -25931,7 +25951,7 @@
         <v>-0.133445083693671</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" hidden="1">
       <c r="A202" t="s">
         <v>24</v>
       </c>
@@ -25996,7 +26016,7 @@
         <v>-1.65782010102585</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" hidden="1">
       <c r="A203" t="s">
         <v>24</v>
       </c>
@@ -26055,7 +26075,7 @@
         <v>-1.62474674793517</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" hidden="1">
       <c r="A204" t="s">
         <v>24</v>
       </c>
@@ -26111,7 +26131,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" hidden="1">
       <c r="A205" t="s">
         <v>24</v>
       </c>
@@ -26182,7 +26202,7 @@
         <v>-1.1765203960699999</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:29" hidden="1">
       <c r="A206" t="s">
         <v>24</v>
       </c>
@@ -26241,7 +26261,7 @@
         <v>-0.19270263064394799</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:29" hidden="1">
       <c r="A207" t="s">
         <v>24</v>
       </c>
@@ -26300,7 +26320,7 @@
         <v>-0.44592595094364801</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:29" hidden="1">
       <c r="A208" t="s">
         <v>24</v>
       </c>
@@ -26368,7 +26388,7 @@
         <v>-0.59273094304076102</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29" hidden="1">
       <c r="A209" t="s">
         <v>24</v>
       </c>
@@ -26427,7 +26447,7 @@
         <v>1.1697820098986</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29" hidden="1">
       <c r="A210" t="s">
         <v>24</v>
       </c>
@@ -26486,7 +26506,7 @@
         <v>-0.88691014682261404</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29" hidden="1">
       <c r="A211" t="s">
         <v>24</v>
       </c>
@@ -26545,7 +26565,7 @@
         <v>1.2828005620354599</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29" hidden="1">
       <c r="A212" t="s">
         <v>24</v>
       </c>
@@ -26613,7 +26633,7 @@
         <v>-2.8007412223167498</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29" hidden="1">
       <c r="A213" t="s">
         <v>24</v>
       </c>
@@ -26669,7 +26689,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" hidden="1">
       <c r="A214" t="s">
         <v>24</v>
       </c>
@@ -26725,7 +26745,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29" hidden="1">
       <c r="A215" t="s">
         <v>24</v>
       </c>
@@ -26790,7 +26810,7 @@
         <v>-1.51743967487292</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29" hidden="1">
       <c r="A216" t="s">
         <v>24</v>
       </c>
@@ -26852,7 +26872,7 @@
         <v>-1.47587145083739</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29" hidden="1">
       <c r="A217" t="s">
         <v>24</v>
       </c>
@@ -26911,7 +26931,7 @@
         <v>-1.62805460803472</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" hidden="1">
       <c r="A218" t="s">
         <v>24</v>
       </c>
@@ -26970,7 +26990,7 @@
         <v>-1.4051226189110999</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29" hidden="1">
       <c r="A219" t="s">
         <v>24</v>
       </c>
@@ -27029,7 +27049,7 @@
         <v>3.7542592217240302E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29" hidden="1">
       <c r="A220" t="s">
         <v>24</v>
       </c>
@@ -27085,7 +27105,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29" hidden="1">
       <c r="A221" t="s">
         <v>24</v>
       </c>
@@ -27147,7 +27167,7 @@
         <v>-1.09340729708271</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29" hidden="1">
       <c r="A222" t="s">
         <v>24</v>
       </c>
@@ -27212,7 +27232,7 @@
         <v>-2.0506522949308699</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:29" hidden="1">
       <c r="A223" t="s">
         <v>24</v>
       </c>
@@ -27268,7 +27288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:29" hidden="1">
       <c r="A224" t="s">
         <v>24</v>
       </c>
@@ -27327,7 +27347,7 @@
         <v>-1.2409629445558299</v>
       </c>
     </row>
-    <row r="225" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:29" hidden="1">
       <c r="A225" t="s">
         <v>24</v>
       </c>
@@ -27386,7 +27406,7 @@
         <v>-2.1849303763291501</v>
       </c>
     </row>
-    <row r="226" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:29" hidden="1">
       <c r="A226" t="s">
         <v>24</v>
       </c>
@@ -27454,7 +27474,7 @@
         <v>-4.1198560602811201</v>
       </c>
     </row>
-    <row r="227" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:29" hidden="1">
       <c r="A227" t="s">
         <v>24</v>
       </c>
@@ -27519,7 +27539,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="228" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:29" hidden="1">
       <c r="A228" t="s">
         <v>24</v>
       </c>
@@ -27587,7 +27607,7 @@
         <v>-1.07837299817203</v>
       </c>
     </row>
-    <row r="229" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:29" hidden="1">
       <c r="A229" t="s">
         <v>24</v>
       </c>
@@ -27646,7 +27666,7 @@
         <v>-2.69765172873824</v>
       </c>
     </row>
-    <row r="230" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:29" hidden="1">
       <c r="A230" t="s">
         <v>24</v>
       </c>
@@ -27714,7 +27734,7 @@
         <v>-0.25310869841260603</v>
       </c>
     </row>
-    <row r="231" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:29" hidden="1">
       <c r="A231" t="s">
         <v>24</v>
       </c>
@@ -27773,7 +27793,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="232" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:29" hidden="1">
       <c r="A232" t="s">
         <v>24</v>
       </c>
@@ -27841,7 +27861,7 @@
         <v>-1.02164637989712</v>
       </c>
     </row>
-    <row r="233" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:29" hidden="1">
       <c r="A233" t="s">
         <v>24</v>
       </c>
@@ -27906,7 +27926,7 @@
         <v>-2.1578678631274801</v>
       </c>
     </row>
-    <row r="234" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:29" hidden="1">
       <c r="A234" t="s">
         <v>24</v>
       </c>
@@ -27965,7 +27985,7 @@
         <v>7.5862726477865405E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:29" hidden="1">
       <c r="A235" t="s">
         <v>24</v>
       </c>
@@ -28033,7 +28053,7 @@
         <v>-0.98382499545167101</v>
       </c>
     </row>
-    <row r="236" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:29" hidden="1">
       <c r="A236" t="s">
         <v>24</v>
       </c>
@@ -28092,7 +28112,7 @@
         <v>-1.9518603046110901</v>
       </c>
     </row>
-    <row r="237" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:29" hidden="1">
       <c r="A237" t="s">
         <v>24</v>
       </c>
@@ -28154,7 +28174,7 @@
         <v>-0.19185369982901401</v>
       </c>
     </row>
-    <row r="238" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:29" hidden="1">
       <c r="A238" t="s">
         <v>24</v>
       </c>
@@ -28213,7 +28233,7 @@
         <v>-2.4447560366013001</v>
       </c>
     </row>
-    <row r="239" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:29" hidden="1">
       <c r="A239" t="s">
         <v>24</v>
       </c>
@@ -28272,7 +28292,7 @@
         <v>-0.31237054143348503</v>
       </c>
     </row>
-    <row r="240" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:29" hidden="1">
       <c r="A240" t="s">
         <v>24</v>
       </c>
@@ -28331,7 +28351,7 @@
         <v>-1.9343273352327199</v>
       </c>
     </row>
-    <row r="241" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:29" hidden="1">
       <c r="A241" t="s">
         <v>24</v>
       </c>
@@ -28390,7 +28410,7 @@
         <v>0.80933174827144005</v>
       </c>
     </row>
-    <row r="242" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:29" hidden="1">
       <c r="A242" t="s">
         <v>24</v>
       </c>
@@ -28449,7 +28469,7 @@
         <v>0.53888531091054503</v>
       </c>
     </row>
-    <row r="243" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:29" hidden="1">
       <c r="A243" t="s">
         <v>24</v>
       </c>
@@ -28508,7 +28528,7 @@
         <v>-2.26729943401683</v>
       </c>
     </row>
-    <row r="244" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:29" hidden="1">
       <c r="A244" t="s">
         <v>24</v>
       </c>
@@ -28573,7 +28593,7 @@
         <v>-1.28615064960739</v>
       </c>
     </row>
-    <row r="245" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:29" hidden="1">
       <c r="A245" t="s">
         <v>24</v>
       </c>
@@ -28632,7 +28652,7 @@
         <v>-1.3282942440232499</v>
       </c>
     </row>
-    <row r="246" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:29" hidden="1">
       <c r="A246" t="s">
         <v>24</v>
       </c>
@@ -28691,7 +28711,7 @@
         <v>-0.76748144845213595</v>
       </c>
     </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:29" hidden="1">
       <c r="A247" t="s">
         <v>24</v>
       </c>
@@ -28750,7 +28770,7 @@
         <v>-0.54131029860619295</v>
       </c>
     </row>
-    <row r="248" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:29" hidden="1">
       <c r="A248" t="s">
         <v>24</v>
       </c>
@@ -28809,7 +28829,7 @@
         <v>-1.0377351214797901</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:29" hidden="1">
       <c r="A249" t="s">
         <v>24</v>
       </c>
@@ -28877,7 +28897,7 @@
         <v>-0.65469061550670404</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:29" hidden="1">
       <c r="A250" t="s">
         <v>24</v>
       </c>
@@ -28936,7 +28956,7 @@
         <v>-0.85200756474897199</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:29" hidden="1">
       <c r="A251" t="s">
         <v>24</v>
       </c>
@@ -28998,7 +29018,7 @@
         <v>-0.34249455556367903</v>
       </c>
     </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:29" hidden="1">
       <c r="A252" t="s">
         <v>24</v>
       </c>
@@ -29063,7 +29083,7 @@
         <v>-2.0089727072543599</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" hidden="1">
       <c r="A253" t="s">
         <v>24</v>
       </c>
@@ -29122,7 +29142,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:29" hidden="1">
       <c r="A254" t="s">
         <v>24</v>
       </c>
@@ -29181,7 +29201,7 @@
         <v>8.1300388968336204E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:29" hidden="1">
       <c r="A255" t="s">
         <v>24</v>
       </c>
@@ -29240,7 +29260,7 @@
         <v>-0.63497108623668497</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:29">
       <c r="A256" t="s">
         <v>24</v>
       </c>
@@ -29262,8 +29282,11 @@
       <c r="N256" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA256">
+        <v>52350</v>
+      </c>
+    </row>
+    <row r="257" spans="1:29" hidden="1">
       <c r="A257" t="s">
         <v>24</v>
       </c>
@@ -29322,7 +29345,7 @@
         <v>-1.55954528496134</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:29" hidden="1">
       <c r="A258" t="s">
         <v>24</v>
       </c>
@@ -29381,7 +29404,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:29" hidden="1">
       <c r="A259" t="s">
         <v>24</v>
       </c>
@@ -29440,7 +29463,7 @@
         <v>-2.9528578456735</v>
       </c>
     </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:29" hidden="1">
       <c r="A260" t="s">
         <v>24</v>
       </c>
@@ -29499,7 +29522,7 @@
         <v>-1.1346806822903901</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:29" hidden="1">
       <c r="A261" t="s">
         <v>24</v>
       </c>
@@ -29558,7 +29581,7 @@
         <v>0.17197231930346801</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:29" hidden="1">
       <c r="A262" t="s">
         <v>24</v>
       </c>
@@ -29614,7 +29637,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:29" hidden="1">
       <c r="A263" t="s">
         <v>24</v>
       </c>
@@ -29679,7 +29702,7 @@
         <v>-3.0150520386678501</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:29" hidden="1">
       <c r="A264" t="s">
         <v>24</v>
       </c>
@@ -29747,7 +29770,7 @@
         <v>-2.4704239435040698</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:29" hidden="1">
       <c r="A265" t="s">
         <v>24</v>
       </c>
@@ -29806,7 +29829,7 @@
         <v>-3.8229361944677298</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:29" hidden="1">
       <c r="A266" t="s">
         <v>24</v>
       </c>
@@ -29871,7 +29894,7 @@
         <v>0.99412411332960504</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:29" hidden="1">
       <c r="A267" t="s">
         <v>24</v>
       </c>
@@ -29936,7 +29959,7 @@
         <v>-1.5503791232830799</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:29" hidden="1">
       <c r="A268" t="s">
         <v>24</v>
       </c>
@@ -30004,7 +30027,7 @@
         <v>-2.7236205816115402</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:29" hidden="1">
       <c r="A269" t="s">
         <v>24</v>
       </c>
@@ -30063,7 +30086,7 @@
         <v>-3.2290793457714399E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:29" hidden="1">
       <c r="A270" t="s">
         <v>24</v>
       </c>
@@ -30131,7 +30154,7 @@
         <v>-2.73405297283644</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:29" hidden="1">
       <c r="A271" t="s">
         <v>24</v>
       </c>
@@ -30190,7 +30213,7 @@
         <v>-0.51784258112992498</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:29" hidden="1">
       <c r="A272" t="s">
         <v>24</v>
       </c>
@@ -30255,7 +30278,7 @@
         <v>-2.1281087509678298</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:29" hidden="1">
       <c r="A273" t="s">
         <v>24</v>
       </c>
@@ -30314,7 +30337,7 @@
         <v>-2.85007636867961</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:29" hidden="1">
       <c r="A274" t="s">
         <v>24</v>
       </c>
@@ -30379,7 +30402,7 @@
         <v>-2.3701907477397399</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:29" hidden="1">
       <c r="A275" t="s">
         <v>24</v>
       </c>
@@ -30447,7 +30470,7 @@
         <v>-0.586234662289148</v>
       </c>
     </row>
-    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" hidden="1">
       <c r="A276" t="s">
         <v>24</v>
       </c>
@@ -30512,7 +30535,7 @@
         <v>-1.45195283365534</v>
       </c>
     </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:29" hidden="1">
       <c r="A277" t="s">
         <v>24</v>
       </c>
@@ -30571,7 +30594,7 @@
         <v>1.2759971899167799</v>
       </c>
     </row>
-    <row r="278" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" hidden="1">
       <c r="A278" t="s">
         <v>24</v>
       </c>
@@ -30630,7 +30653,7 @@
         <v>-1.04288891982992</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" hidden="1">
       <c r="A279" t="s">
         <v>24</v>
       </c>
@@ -30695,7 +30718,7 @@
         <v>-1.72707700878563</v>
       </c>
     </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" hidden="1">
       <c r="A280" t="s">
         <v>24</v>
       </c>
@@ -30751,7 +30774,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" hidden="1">
       <c r="A281" t="s">
         <v>24</v>
       </c>
@@ -30822,7 +30845,7 @@
         <v>0.72869135579069699</v>
       </c>
     </row>
-    <row r="282" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:29" hidden="1">
       <c r="A282" t="s">
         <v>24</v>
       </c>
@@ -30881,7 +30904,7 @@
         <v>-1.07140821432959</v>
       </c>
     </row>
-    <row r="283" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:29" hidden="1">
       <c r="A283" t="s">
         <v>24</v>
       </c>
@@ -30940,7 +30963,7 @@
         <v>-0.46798353846267798</v>
       </c>
     </row>
-    <row r="284" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:29" hidden="1">
       <c r="A284" t="s">
         <v>24</v>
       </c>
@@ -30999,7 +31022,7 @@
         <v>-2.7102579722904498</v>
       </c>
     </row>
-    <row r="285" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" hidden="1">
       <c r="A285" t="s">
         <v>24</v>
       </c>
@@ -31055,7 +31078,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="286" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:29" hidden="1">
       <c r="A286" t="s">
         <v>24</v>
       </c>
@@ -31114,7 +31137,7 @@
         <v>-2.70989034157054</v>
       </c>
     </row>
-    <row r="287" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:29" hidden="1">
       <c r="A287" t="s">
         <v>24</v>
       </c>
@@ -31173,7 +31196,7 @@
         <v>-2.1768091357562098</v>
       </c>
     </row>
-    <row r="288" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:29" hidden="1">
       <c r="A288" t="s">
         <v>24</v>
       </c>
@@ -31232,7 +31255,7 @@
         <v>-2.17649681212928</v>
       </c>
     </row>
-    <row r="289" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:29" hidden="1">
       <c r="A289" t="s">
         <v>24</v>
       </c>
@@ -31300,7 +31323,7 @@
         <v>-2.1645283464811702</v>
       </c>
     </row>
-    <row r="290" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:29" hidden="1">
       <c r="A290" t="s">
         <v>24</v>
       </c>
@@ -31359,7 +31382,7 @@
         <v>-1.98125403204151</v>
       </c>
     </row>
-    <row r="291" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:29" hidden="1">
       <c r="A291" t="s">
         <v>24</v>
       </c>
@@ -31427,7 +31450,7 @@
         <v>-1.39871369539267</v>
       </c>
     </row>
-    <row r="292" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:29" hidden="1">
       <c r="A292" t="s">
         <v>24</v>
       </c>
@@ -31486,7 +31509,7 @@
         <v>-0.17757021668369599</v>
       </c>
     </row>
-    <row r="293" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:29" hidden="1">
       <c r="A293" t="s">
         <v>24</v>
       </c>
@@ -31545,7 +31568,7 @@
         <v>-2.3001467834814702</v>
       </c>
     </row>
-    <row r="294" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:29" hidden="1">
       <c r="A294" t="s">
         <v>24</v>
       </c>
@@ -31604,7 +31627,7 @@
         <v>-1.62283893738364</v>
       </c>
     </row>
-    <row r="295" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:29" hidden="1">
       <c r="A295" t="s">
         <v>24</v>
       </c>
@@ -31660,7 +31683,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="296" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:29" hidden="1">
       <c r="A296" t="s">
         <v>24</v>
       </c>
@@ -31731,7 +31754,7 @@
         <v>-1.32897995507878</v>
       </c>
     </row>
-    <row r="297" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:29" hidden="1">
       <c r="A297" t="s">
         <v>24</v>
       </c>
@@ -31793,7 +31816,7 @@
         <v>-0.189332334990787</v>
       </c>
     </row>
-    <row r="298" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:29" hidden="1">
       <c r="A298" t="s">
         <v>24</v>
       </c>
@@ -31858,7 +31881,7 @@
         <v>-1.4442525340164001</v>
       </c>
     </row>
-    <row r="299" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:29" hidden="1">
       <c r="A299" t="s">
         <v>24</v>
       </c>
@@ -31917,7 +31940,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="300" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:29" hidden="1">
       <c r="A300" t="s">
         <v>24</v>
       </c>
@@ -31976,7 +31999,7 @@
         <v>-0.670548578569375</v>
       </c>
     </row>
-    <row r="301" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:29" hidden="1">
       <c r="A301" t="s">
         <v>24</v>
       </c>
@@ -32044,7 +32067,7 @@
         <v>-1.74381282954794</v>
       </c>
     </row>
-    <row r="302" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:29" hidden="1">
       <c r="A302" t="s">
         <v>24</v>
       </c>
@@ -32103,7 +32126,7 @@
         <v>-7.4056169834462102E-2</v>
       </c>
     </row>
-    <row r="303" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:29" hidden="1">
       <c r="A303" t="s">
         <v>24</v>
       </c>
@@ -32162,7 +32185,7 @@
         <v>0.813219656271712</v>
       </c>
     </row>
-    <row r="304" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:29">
       <c r="A304" t="s">
         <v>24</v>
       </c>
@@ -32196,11 +32219,17 @@
       <c r="U304">
         <v>411</v>
       </c>
+      <c r="Z304" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA304">
+        <v>91531</v>
+      </c>
       <c r="AC304">
         <v>-3.3625758803201502</v>
       </c>
     </row>
-    <row r="305" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:29" hidden="1">
       <c r="A305" t="s">
         <v>24</v>
       </c>
@@ -32265,7 +32294,7 @@
         <v>-2.06281384080734</v>
       </c>
     </row>
-    <row r="306" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:29" hidden="1">
       <c r="A306" t="s">
         <v>24</v>
       </c>
@@ -32324,7 +32353,7 @@
         <v>-4.3406638690371799E-2</v>
       </c>
     </row>
-    <row r="307" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:29" hidden="1">
       <c r="A307" t="s">
         <v>24</v>
       </c>
@@ -32383,7 +32412,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="308" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:29" hidden="1">
       <c r="A308" t="s">
         <v>24</v>
       </c>
@@ -32442,7 +32471,7 @@
         <v>-1.6778453301552601</v>
       </c>
     </row>
-    <row r="309" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:29" hidden="1">
       <c r="A309" t="s">
         <v>24</v>
       </c>
@@ -32501,7 +32530,7 @@
         <v>-3.6567559949466601</v>
       </c>
     </row>
-    <row r="310" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:29" hidden="1">
       <c r="A310" t="s">
         <v>24</v>
       </c>
@@ -32560,7 +32589,7 @@
         <v>1.1150094479463799</v>
       </c>
     </row>
-    <row r="311" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:29" hidden="1">
       <c r="A311" t="s">
         <v>24</v>
       </c>
@@ -32619,7 +32648,7 @@
         <v>-1.5106533665965201</v>
       </c>
     </row>
-    <row r="312" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:29" hidden="1">
       <c r="A312" t="s">
         <v>24</v>
       </c>
@@ -32678,7 +32707,7 @@
         <v>-2.08744455338184</v>
       </c>
     </row>
-    <row r="313" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:29" hidden="1">
       <c r="A313" t="s">
         <v>24</v>
       </c>
@@ -32749,7 +32778,7 @@
         <v>-2.4887952473460202</v>
       </c>
     </row>
-    <row r="314" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:29" hidden="1">
       <c r="A314" t="s">
         <v>24</v>
       </c>
@@ -32808,7 +32837,7 @@
         <v>1.3405526779310999</v>
       </c>
     </row>
-    <row r="315" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:29" hidden="1">
       <c r="A315" t="s">
         <v>24</v>
       </c>
@@ -32867,7 +32896,7 @@
         <v>-0.460598678152911</v>
       </c>
     </row>
-    <row r="316" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:29" hidden="1">
       <c r="A316" t="s">
         <v>24</v>
       </c>
@@ -32935,7 +32964,7 @@
         <v>0.373108306637151</v>
       </c>
     </row>
-    <row r="317" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:29" hidden="1">
       <c r="A317" t="s">
         <v>24</v>
       </c>
@@ -33003,7 +33032,7 @@
         <v>-3.53020277442742</v>
       </c>
     </row>
-    <row r="318" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:29" hidden="1">
       <c r="A318" t="s">
         <v>24</v>
       </c>
@@ -33065,7 +33094,7 @@
         <v>0.357837154125004</v>
       </c>
     </row>
-    <row r="319" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:29" hidden="1">
       <c r="A319" t="s">
         <v>24</v>
       </c>
@@ -33124,7 +33153,7 @@
         <v>-4.2488527797753202</v>
       </c>
     </row>
-    <row r="320" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:29" hidden="1">
       <c r="A320" t="s">
         <v>24</v>
       </c>
@@ -33189,7 +33218,7 @@
         <v>-2.3553497197990101</v>
       </c>
     </row>
-    <row r="321" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:29" hidden="1">
       <c r="A321" t="s">
         <v>24</v>
       </c>
@@ -33248,7 +33277,7 @@
         <v>0.43082466120681001</v>
       </c>
     </row>
-    <row r="322" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:29">
       <c r="A322" t="s">
         <v>24</v>
       </c>
@@ -33267,8 +33296,11 @@
       <c r="I322" t="s">
         <v>4114</v>
       </c>
-    </row>
-    <row r="323" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA322">
+        <v>87984</v>
+      </c>
+    </row>
+    <row r="323" spans="1:29" hidden="1">
       <c r="A323" t="s">
         <v>24</v>
       </c>
@@ -33327,7 +33359,7 @@
         <v>-3.4657444542099701E-2</v>
       </c>
     </row>
-    <row r="324" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:29" hidden="1">
       <c r="A324" t="s">
         <v>24</v>
       </c>
@@ -33386,7 +33418,7 @@
         <v>0.279804820777248</v>
       </c>
     </row>
-    <row r="325" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:29" hidden="1">
       <c r="A325" t="s">
         <v>24</v>
       </c>
@@ -33445,7 +33477,7 @@
         <v>-1.4416684895262699</v>
       </c>
     </row>
-    <row r="326" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:29" hidden="1">
       <c r="A326" t="s">
         <v>24</v>
       </c>
@@ -33504,7 +33536,7 @@
         <v>-0.63266617343135401</v>
       </c>
     </row>
-    <row r="327" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:29" hidden="1">
       <c r="A327" t="s">
         <v>24</v>
       </c>
@@ -33560,7 +33592,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="328" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:29" hidden="1">
       <c r="A328" t="s">
         <v>24</v>
       </c>
@@ -33619,7 +33651,7 @@
         <v>-0.40335198756146401</v>
       </c>
     </row>
-    <row r="329" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:29" hidden="1">
       <c r="A329" t="s">
         <v>24</v>
       </c>
@@ -33678,7 +33710,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="330" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:29" hidden="1">
       <c r="A330" t="s">
         <v>24</v>
       </c>
@@ -33737,7 +33769,7 @@
         <v>-1.58466508699511</v>
       </c>
     </row>
-    <row r="331" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:29" hidden="1">
       <c r="A331" t="s">
         <v>24</v>
       </c>
@@ -33805,7 +33837,7 @@
         <v>-1.3044355560511001</v>
       </c>
     </row>
-    <row r="332" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:29" hidden="1">
       <c r="A332" t="s">
         <v>24</v>
       </c>
@@ -33864,7 +33896,7 @@
         <v>-4.0462162110289803</v>
       </c>
     </row>
-    <row r="333" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:29" hidden="1">
       <c r="A333" t="s">
         <v>24</v>
       </c>
@@ -33923,7 +33955,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="334" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:29" hidden="1">
       <c r="A334" t="s">
         <v>24</v>
       </c>
@@ -33982,7 +34014,7 @@
         <v>0.19865335020727201</v>
       </c>
     </row>
-    <row r="335" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:29">
       <c r="A335" t="s">
         <v>24</v>
       </c>
@@ -34004,8 +34036,11 @@
       <c r="N335" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="336" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA335">
+        <v>88002</v>
+      </c>
+    </row>
+    <row r="336" spans="1:29" hidden="1">
       <c r="A336" t="s">
         <v>24</v>
       </c>
@@ -34064,7 +34099,7 @@
         <v>-0.71233980443257905</v>
       </c>
     </row>
-    <row r="337" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:29" hidden="1">
       <c r="A337" t="s">
         <v>24</v>
       </c>
@@ -34126,7 +34161,7 @@
         <v>-0.19408512068214201</v>
       </c>
     </row>
-    <row r="338" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:29" hidden="1">
       <c r="A338" t="s">
         <v>24</v>
       </c>
@@ -34188,7 +34223,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="339" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:29" hidden="1">
       <c r="A339" t="s">
         <v>24</v>
       </c>
@@ -34247,7 +34282,7 @@
         <v>-1.26453221779957E-2</v>
       </c>
     </row>
-    <row r="340" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:29" hidden="1">
       <c r="A340" t="s">
         <v>24</v>
       </c>
@@ -34312,7 +34347,7 @@
         <v>-2.5895088338873</v>
       </c>
     </row>
-    <row r="341" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:29" hidden="1">
       <c r="A341" t="s">
         <v>24</v>
       </c>
@@ -34380,7 +34415,7 @@
         <v>-1.94460788203187</v>
       </c>
     </row>
-    <row r="342" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:29" hidden="1">
       <c r="A342" t="s">
         <v>24</v>
       </c>
@@ -34439,7 +34474,7 @@
         <v>-1.2210742603696001</v>
       </c>
     </row>
-    <row r="343" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:29" hidden="1">
       <c r="A343" t="s">
         <v>24</v>
       </c>
@@ -34504,7 +34539,7 @@
         <v>-1.4118077319906499</v>
       </c>
     </row>
-    <row r="344" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:29" hidden="1">
       <c r="A344" t="s">
         <v>24</v>
       </c>
@@ -34563,7 +34598,7 @@
         <v>-2.8826587441298099</v>
       </c>
     </row>
-    <row r="345" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:29" hidden="1">
       <c r="A345" t="s">
         <v>24</v>
       </c>
@@ -34622,7 +34657,7 @@
         <v>-0.477114657614783</v>
       </c>
     </row>
-    <row r="346" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:29" hidden="1">
       <c r="A346" t="s">
         <v>24</v>
       </c>
@@ -34687,7 +34722,7 @@
         <v>-1.9663478518608499</v>
       </c>
     </row>
-    <row r="347" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:29" hidden="1">
       <c r="A347" t="s">
         <v>24</v>
       </c>
@@ -34752,7 +34787,7 @@
         <v>-2.1209914536093502</v>
       </c>
     </row>
-    <row r="348" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:29">
       <c r="A348" t="s">
         <v>24</v>
       </c>
@@ -34774,8 +34809,11 @@
       <c r="N348" s="1">
         <v>41730</v>
       </c>
-    </row>
-    <row r="349" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA348">
+        <v>64997</v>
+      </c>
+    </row>
+    <row r="349" spans="1:29" hidden="1">
       <c r="A349" t="s">
         <v>24</v>
       </c>
@@ -34834,7 +34872,7 @@
         <v>-0.186190160336486</v>
       </c>
     </row>
-    <row r="350" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:29" hidden="1">
       <c r="A350" t="s">
         <v>24</v>
       </c>
@@ -34902,7 +34940,7 @@
         <v>-0.69947832145465305</v>
       </c>
     </row>
-    <row r="351" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:29" hidden="1">
       <c r="A351" t="s">
         <v>24</v>
       </c>
@@ -34961,7 +34999,7 @@
         <v>-2.2113242238437398</v>
       </c>
     </row>
-    <row r="352" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:29" hidden="1">
       <c r="A352" t="s">
         <v>24</v>
       </c>
@@ -35020,7 +35058,7 @@
         <v>-0.56077011732615101</v>
       </c>
     </row>
-    <row r="353" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:29" hidden="1">
       <c r="A353" t="s">
         <v>24</v>
       </c>
@@ -35088,7 +35126,7 @@
         <v>-0.88384218537428105</v>
       </c>
     </row>
-    <row r="354" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:29" hidden="1">
       <c r="A354" t="s">
         <v>24</v>
       </c>
@@ -35144,7 +35182,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="355" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:29" hidden="1">
       <c r="A355" t="s">
         <v>24</v>
       </c>
@@ -35206,7 +35244,7 @@
         <v>-0.39581200189250598</v>
       </c>
     </row>
-    <row r="356" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:29" hidden="1">
       <c r="A356" t="s">
         <v>24</v>
       </c>
@@ -35265,7 +35303,7 @@
         <v>-1.5069302321045699</v>
       </c>
     </row>
-    <row r="357" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:29" hidden="1">
       <c r="A357" t="s">
         <v>24</v>
       </c>
@@ -35330,7 +35368,7 @@
         <v>-3.09257525015963</v>
       </c>
     </row>
-    <row r="358" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:29" hidden="1">
       <c r="A358" t="s">
         <v>24</v>
       </c>
@@ -35398,7 +35436,7 @@
         <v>-2.56362586747675</v>
       </c>
     </row>
-    <row r="359" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:29">
       <c r="A359" t="s">
         <v>24</v>
       </c>
@@ -35429,11 +35467,17 @@
       <c r="U359">
         <v>410</v>
       </c>
+      <c r="Z359" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA359">
+        <v>91366</v>
+      </c>
       <c r="AC359">
         <v>0.62207831122558699</v>
       </c>
     </row>
-    <row r="360" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:29" hidden="1">
       <c r="A360" t="s">
         <v>24</v>
       </c>
@@ -35492,7 +35536,7 @@
         <v>-0.16045950038840301</v>
       </c>
     </row>
-    <row r="361" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:29" hidden="1">
       <c r="A361" t="s">
         <v>24</v>
       </c>
@@ -35551,7 +35595,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="362" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:29" hidden="1">
       <c r="A362" t="s">
         <v>24</v>
       </c>
@@ -35607,7 +35651,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="363" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:29" hidden="1">
       <c r="A363" t="s">
         <v>24</v>
       </c>
@@ -35666,7 +35710,7 @@
         <v>-2.0508165247066201</v>
       </c>
     </row>
-    <row r="364" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:29" hidden="1">
       <c r="A364" t="s">
         <v>24</v>
       </c>
@@ -35725,7 +35769,7 @@
         <v>-2.2746669467274199</v>
       </c>
     </row>
-    <row r="365" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:29" hidden="1">
       <c r="A365" t="s">
         <v>24</v>
       </c>
@@ -35784,7 +35828,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="366" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:29" hidden="1">
       <c r="A366" t="s">
         <v>24</v>
       </c>
@@ -35843,7 +35887,7 @@
         <v>-2.8538694979818602</v>
       </c>
     </row>
-    <row r="367" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:29" hidden="1">
       <c r="A367" t="s">
         <v>24</v>
       </c>
@@ -35911,7 +35955,7 @@
         <v>-1.0614499339671399</v>
       </c>
     </row>
-    <row r="368" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:29" hidden="1">
       <c r="A368" t="s">
         <v>3053</v>
       </c>
@@ -35946,7 +35990,7 @@
         <v>54906</v>
       </c>
     </row>
-    <row r="369" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:27" hidden="1">
       <c r="A369" t="s">
         <v>3053</v>
       </c>
@@ -35981,7 +36025,7 @@
         <v>54914</v>
       </c>
     </row>
-    <row r="370" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:27" hidden="1">
       <c r="A370" t="s">
         <v>3053</v>
       </c>
@@ -36016,7 +36060,7 @@
         <v>54905</v>
       </c>
     </row>
-    <row r="371" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:27" hidden="1">
       <c r="A371" t="s">
         <v>3053</v>
       </c>
@@ -36054,7 +36098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="372" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:27" hidden="1">
       <c r="A372" t="s">
         <v>3053</v>
       </c>
@@ -36089,7 +36133,7 @@
         <v>54907</v>
       </c>
     </row>
-    <row r="373" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:27" hidden="1">
       <c r="A373" t="s">
         <v>3053</v>
       </c>
@@ -36124,7 +36168,7 @@
         <v>54908</v>
       </c>
     </row>
-    <row r="374" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:27" hidden="1">
       <c r="A374" t="s">
         <v>3053</v>
       </c>
@@ -36159,7 +36203,7 @@
         <v>54909</v>
       </c>
     </row>
-    <row r="375" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:27" hidden="1">
       <c r="A375" t="s">
         <v>3053</v>
       </c>
@@ -36194,7 +36238,7 @@
         <v>54910</v>
       </c>
     </row>
-    <row r="376" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:27" hidden="1">
       <c r="A376" t="s">
         <v>3053</v>
       </c>
@@ -36229,7 +36273,7 @@
         <v>54911</v>
       </c>
     </row>
-    <row r="377" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:27" hidden="1">
       <c r="A377" t="s">
         <v>3053</v>
       </c>
@@ -36267,7 +36311,7 @@
         <v>54912</v>
       </c>
     </row>
-    <row r="378" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:27">
       <c r="A378" t="s">
         <v>3053</v>
       </c>
@@ -36291,7 +36335,7 @@
         <v>3130</v>
       </c>
     </row>
-    <row r="379" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:27">
       <c r="A379" t="s">
         <v>3053</v>
       </c>
@@ -36315,7 +36359,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="380" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:27">
       <c r="A380" t="s">
         <v>3053</v>
       </c>
@@ -36339,7 +36383,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="381" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:27">
       <c r="A381" t="s">
         <v>3053</v>
       </c>
@@ -36363,7 +36407,7 @@
         <v>3145</v>
       </c>
     </row>
-    <row r="382" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:27">
       <c r="A382" t="s">
         <v>3053</v>
       </c>
@@ -36387,7 +36431,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="383" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:27">
       <c r="A383" t="s">
         <v>3053</v>
       </c>
@@ -36411,7 +36455,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="384" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:27">
       <c r="A384" t="s">
         <v>3053</v>
       </c>
@@ -36435,7 +36479,7 @@
         <v>3160</v>
       </c>
     </row>
-    <row r="385" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:23">
       <c r="A385" t="s">
         <v>3053</v>
       </c>
@@ -36459,7 +36503,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="386" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:23">
       <c r="A386" t="s">
         <v>3053</v>
       </c>
@@ -36483,7 +36527,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="387" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:23">
       <c r="A387" t="s">
         <v>3053</v>
       </c>
@@ -36507,7 +36551,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="388" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:23">
       <c r="A388" t="s">
         <v>3053</v>
       </c>
@@ -36531,7 +36575,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="389" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:23">
       <c r="A389" t="s">
         <v>3053</v>
       </c>
@@ -36555,7 +36599,7 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="390" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:23">
       <c r="A390" t="s">
         <v>3053</v>
       </c>
@@ -36579,7 +36623,7 @@
         <v>3190</v>
       </c>
     </row>
-    <row r="391" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:23">
       <c r="A391" t="s">
         <v>3053</v>
       </c>
@@ -36603,7 +36647,7 @@
         <v>3195</v>
       </c>
     </row>
-    <row r="392" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:23">
       <c r="A392" t="s">
         <v>3053</v>
       </c>
@@ -36627,7 +36671,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="393" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:23">
       <c r="A393" t="s">
         <v>3053</v>
       </c>
@@ -36651,7 +36695,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="394" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:23">
       <c r="A394" t="s">
         <v>3053</v>
       </c>
@@ -36675,7 +36719,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="395" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:23">
       <c r="A395" t="s">
         <v>3053</v>
       </c>
@@ -36699,7 +36743,7 @@
         <v>3215</v>
       </c>
     </row>
-    <row r="396" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:23">
       <c r="A396" t="s">
         <v>3053</v>
       </c>
@@ -36723,7 +36767,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="397" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:23">
       <c r="A397" t="s">
         <v>3053</v>
       </c>
@@ -36747,7 +36791,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="398" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:23">
       <c r="A398" t="s">
         <v>3053</v>
       </c>
@@ -36771,7 +36815,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="399" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:23">
       <c r="A399" t="s">
         <v>3053</v>
       </c>
@@ -36795,7 +36839,7 @@
         <v>3235</v>
       </c>
     </row>
-    <row r="400" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:23">
       <c r="A400" t="s">
         <v>3053</v>
       </c>
@@ -36819,7 +36863,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="401" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:29">
       <c r="A401" t="s">
         <v>3053</v>
       </c>
@@ -36843,7 +36887,7 @@
         <v>3245</v>
       </c>
     </row>
-    <row r="402" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:29">
       <c r="A402" t="s">
         <v>3053</v>
       </c>
@@ -36867,7 +36911,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="403" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:29" hidden="1">
       <c r="A403" t="s">
         <v>3053</v>
       </c>
@@ -36902,7 +36946,7 @@
         <v>54913</v>
       </c>
     </row>
-    <row r="404" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:29" hidden="1">
       <c r="A404" t="s">
         <v>3257</v>
       </c>
@@ -36952,7 +36996,7 @@
         <v>-2.6320254568961299</v>
       </c>
     </row>
-    <row r="405" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:29" hidden="1">
       <c r="A405" t="s">
         <v>3257</v>
       </c>
@@ -37002,7 +37046,7 @@
         <v>-2.1736372108922302</v>
       </c>
     </row>
-    <row r="406" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:29" hidden="1">
       <c r="A406" t="s">
         <v>3257</v>
       </c>
@@ -37052,7 +37096,7 @@
         <v>-5.2161559340253296</v>
       </c>
     </row>
-    <row r="407" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:29" hidden="1">
       <c r="A407" t="s">
         <v>3257</v>
       </c>
@@ -37102,7 +37146,7 @@
         <v>-2.9173012654216701</v>
       </c>
     </row>
-    <row r="408" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:29" hidden="1">
       <c r="A408" t="s">
         <v>3257</v>
       </c>
@@ -37152,7 +37196,7 @@
         <v>-3.7422224090000902</v>
       </c>
     </row>
-    <row r="409" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:29" hidden="1">
       <c r="A409" t="s">
         <v>3257</v>
       </c>
@@ -37205,7 +37249,7 @@
         <v>-3.9593418402573399</v>
       </c>
     </row>
-    <row r="410" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:29" hidden="1">
       <c r="A410" t="s">
         <v>3257</v>
       </c>
@@ -37255,7 +37299,7 @@
         <v>-2.9695507392012699</v>
       </c>
     </row>
-    <row r="411" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:29" hidden="1">
       <c r="A411" t="s">
         <v>3257</v>
       </c>
@@ -37305,7 +37349,7 @@
         <v>-4.3142015194398802</v>
       </c>
     </row>
-    <row r="412" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:29" hidden="1">
       <c r="A412" t="s">
         <v>3257</v>
       </c>
@@ -37355,7 +37399,7 @@
         <v>-3.2883920016089001</v>
       </c>
     </row>
-    <row r="413" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:29" hidden="1">
       <c r="A413" t="s">
         <v>3257</v>
       </c>
@@ -37408,7 +37452,7 @@
         <v>-4.2255597323538296</v>
       </c>
     </row>
-    <row r="414" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:29" hidden="1">
       <c r="A414" t="s">
         <v>3257</v>
       </c>
@@ -37458,7 +37502,7 @@
         <v>-2.72088790105995</v>
       </c>
     </row>
-    <row r="415" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:29" hidden="1">
       <c r="A415" t="s">
         <v>3257</v>
       </c>
@@ -37514,7 +37558,7 @@
         <v>-6.6727812366699801</v>
       </c>
     </row>
-    <row r="416" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:29" hidden="1">
       <c r="A416" t="s">
         <v>3257</v>
       </c>
@@ -37564,7 +37608,7 @@
         <v>-4.3595143451574803</v>
       </c>
     </row>
-    <row r="417" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:29" hidden="1">
       <c r="A417" t="s">
         <v>3257</v>
       </c>
@@ -37614,7 +37658,7 @@
         <v>-3.7906415337898101</v>
       </c>
     </row>
-    <row r="418" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:29" hidden="1">
       <c r="A418" t="s">
         <v>3257</v>
       </c>
@@ -37667,7 +37711,7 @@
         <v>-3.1243518319000199</v>
       </c>
     </row>
-    <row r="419" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:29" hidden="1">
       <c r="A419" t="s">
         <v>3257</v>
       </c>
@@ -37720,7 +37764,7 @@
         <v>-4.2531185815445198</v>
       </c>
     </row>
-    <row r="420" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:29" hidden="1">
       <c r="A420" t="s">
         <v>3257</v>
       </c>
@@ -37773,7 +37817,7 @@
         <v>-6.5410206557117796</v>
       </c>
     </row>
-    <row r="421" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:29" hidden="1">
       <c r="A421" t="s">
         <v>3257</v>
       </c>
@@ -37823,7 +37867,7 @@
         <v>-4.7426698710190003</v>
       </c>
     </row>
-    <row r="422" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:29" hidden="1">
       <c r="A422" t="s">
         <v>3257</v>
       </c>
@@ -37873,7 +37917,7 @@
         <v>-3.1104195114441802</v>
       </c>
     </row>
-    <row r="423" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:29" hidden="1">
       <c r="A423" t="s">
         <v>3257</v>
       </c>
@@ -37926,7 +37970,7 @@
         <v>-3.2675085733413902</v>
       </c>
     </row>
-    <row r="424" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:29" hidden="1">
       <c r="A424" t="s">
         <v>3257</v>
       </c>
@@ -37976,7 +38020,7 @@
         <v>-4.7318068826625499</v>
       </c>
     </row>
-    <row r="425" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:29" hidden="1">
       <c r="A425" t="s">
         <v>3257</v>
       </c>
@@ -38029,7 +38073,7 @@
         <v>-3.9482525144777099</v>
       </c>
     </row>
-    <row r="426" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:29" hidden="1">
       <c r="A426" t="s">
         <v>3257</v>
       </c>
@@ -38079,7 +38123,7 @@
         <v>-2.79660744400323</v>
       </c>
     </row>
-    <row r="427" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:29" hidden="1">
       <c r="A427" t="s">
         <v>3257</v>
       </c>
@@ -38132,7 +38176,7 @@
         <v>-3.81895374279111</v>
       </c>
     </row>
-    <row r="428" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:29" hidden="1">
       <c r="A428" t="s">
         <v>3257</v>
       </c>
@@ -38182,7 +38226,7 @@
         <v>-4.5428045875510996</v>
       </c>
     </row>
-    <row r="429" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:29" hidden="1">
       <c r="A429" t="s">
         <v>3257</v>
       </c>
@@ -38232,7 +38276,7 @@
         <v>-4.6889262632352802</v>
       </c>
     </row>
-    <row r="430" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:29" hidden="1">
       <c r="A430" t="s">
         <v>3257</v>
       </c>
@@ -38282,7 +38326,7 @@
         <v>-2.7884684974713201</v>
       </c>
     </row>
-    <row r="431" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:29" hidden="1">
       <c r="A431" t="s">
         <v>3257</v>
       </c>
@@ -38332,7 +38376,7 @@
         <v>-3.8106358553200299</v>
       </c>
     </row>
-    <row r="432" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:29" hidden="1">
       <c r="A432" t="s">
         <v>3257</v>
       </c>
@@ -38382,7 +38426,7 @@
         <v>-4.34034032374697</v>
       </c>
     </row>
-    <row r="433" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:29" hidden="1">
       <c r="A433" t="s">
         <v>3257</v>
       </c>
@@ -38432,7 +38476,7 @@
         <v>-4.5176029554922001</v>
       </c>
     </row>
-    <row r="434" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:29" hidden="1">
       <c r="A434" t="s">
         <v>3257</v>
       </c>
@@ -38482,7 +38526,7 @@
         <v>-3.5737860466933999</v>
       </c>
     </row>
-    <row r="435" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:29" hidden="1">
       <c r="A435" t="s">
         <v>3257</v>
       </c>
@@ -38532,7 +38576,7 @@
         <v>-1.3441674209272401</v>
       </c>
     </row>
-    <row r="436" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:29" hidden="1">
       <c r="A436" t="s">
         <v>3519</v>
       </c>
@@ -38591,7 +38635,7 @@
         <v>-4.3745242143952199</v>
       </c>
     </row>
-    <row r="437" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:29" hidden="1">
       <c r="A437" t="s">
         <v>3519</v>
       </c>
@@ -38650,7 +38694,7 @@
         <v>-3.6003878013017698</v>
       </c>
     </row>
-    <row r="438" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:29" hidden="1">
       <c r="A438" t="s">
         <v>3519</v>
       </c>
@@ -38709,7 +38753,7 @@
         <v>-3.1938186287935002</v>
       </c>
     </row>
-    <row r="439" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:29" hidden="1">
       <c r="A439" t="s">
         <v>3519</v>
       </c>
@@ -38768,7 +38812,7 @@
         <v>-3.2048973242453598</v>
       </c>
     </row>
-    <row r="440" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:29" hidden="1">
       <c r="A440" t="s">
         <v>3519</v>
       </c>
@@ -38827,7 +38871,7 @@
         <v>-4.0731173568071002</v>
       </c>
     </row>
-    <row r="441" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:29" hidden="1">
       <c r="A441" t="s">
         <v>3519</v>
       </c>
@@ -38886,7 +38930,7 @@
         <v>-4.1631820382407696</v>
       </c>
     </row>
-    <row r="442" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:29" hidden="1">
       <c r="A442" t="s">
         <v>3519</v>
       </c>
@@ -38948,7 +38992,7 @@
         <v>-3.1997652808396699</v>
       </c>
     </row>
-    <row r="443" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:29" hidden="1">
       <c r="A443" t="s">
         <v>3519</v>
       </c>
@@ -39007,7 +39051,7 @@
         <v>-3.7364398723286598</v>
       </c>
     </row>
-    <row r="444" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:29" hidden="1">
       <c r="A444" t="s">
         <v>3519</v>
       </c>
@@ -39066,7 +39110,7 @@
         <v>-3.3541041522652799</v>
       </c>
     </row>
-    <row r="445" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:29" hidden="1">
       <c r="A445" t="s">
         <v>3519</v>
       </c>
@@ -39125,7 +39169,7 @@
         <v>-3.1631503565558798</v>
       </c>
     </row>
-    <row r="446" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:29" hidden="1">
       <c r="A446" t="s">
         <v>3519</v>
       </c>
@@ -39184,7 +39228,7 @@
         <v>-4.69786872585005</v>
       </c>
     </row>
-    <row r="447" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:29" hidden="1">
       <c r="A447" t="s">
         <v>3519</v>
       </c>
@@ -39243,7 +39287,7 @@
         <v>-2.86732879213604</v>
       </c>
     </row>
-    <row r="448" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:29" hidden="1">
       <c r="A448" t="s">
         <v>3519</v>
       </c>
@@ -39302,7 +39346,7 @@
         <v>-3.3610566541754499</v>
       </c>
     </row>
-    <row r="449" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:29" hidden="1">
       <c r="A449" t="s">
         <v>3519</v>
       </c>
@@ -39361,7 +39405,7 @@
         <v>-3.7433933101120802</v>
       </c>
     </row>
-    <row r="450" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:29" hidden="1">
       <c r="A450" t="s">
         <v>3519</v>
       </c>
@@ -39420,7 +39464,7 @@
         <v>-2.9617942281162999</v>
       </c>
     </row>
-    <row r="451" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:29" hidden="1">
       <c r="A451" t="s">
         <v>3519</v>
       </c>
@@ -39479,7 +39523,7 @@
         <v>-5.4124349102999698</v>
       </c>
     </row>
-    <row r="452" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:29" hidden="1">
       <c r="A452" t="s">
         <v>3519</v>
       </c>
@@ -39538,7 +39582,7 @@
         <v>-3.4099252669704501</v>
       </c>
     </row>
-    <row r="453" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:29" hidden="1">
       <c r="A453" t="s">
         <v>3519</v>
       </c>
@@ -39594,7 +39638,7 @@
         <v>-3.43554851990443</v>
       </c>
     </row>
-    <row r="454" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:29" hidden="1">
       <c r="A454" t="s">
         <v>3519</v>
       </c>
@@ -39656,7 +39700,7 @@
         <v>-4.0613695499049802</v>
       </c>
     </row>
-    <row r="455" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:29" hidden="1">
       <c r="A455" t="s">
         <v>3519</v>
       </c>
@@ -39715,7 +39759,7 @@
         <v>-3.0534269632451698</v>
       </c>
     </row>
-    <row r="456" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:29" hidden="1">
       <c r="A456" t="s">
         <v>3519</v>
       </c>
@@ -39774,7 +39818,7 @@
         <v>-3.3991644530109499</v>
       </c>
     </row>
-    <row r="457" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:29" hidden="1">
       <c r="A457" t="s">
         <v>3519</v>
       </c>
@@ -39833,7 +39877,7 @@
         <v>-3.0178639598661499</v>
       </c>
     </row>
-    <row r="458" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:29" ht="18" hidden="1">
       <c r="A458" t="s">
         <v>24</v>
       </c>
@@ -39870,7 +39914,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD458" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}"/>
+  <autoFilter ref="A1:AD458" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}">
+    <filterColumn colId="26">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed overlapping authorities that were reversed
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F17987-47E6-4181-AA6B-7619A17D36C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E26AF1-1BD4-4898-B3BB-EB8287EEEFD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13894,9 +13894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20655,7 +20655,7 @@
         <v>24</v>
       </c>
       <c r="F102" t="s">
-        <v>640</v>
+        <v>327</v>
       </c>
       <c r="G102" t="s">
         <v>877</v>

</xml_diff>

<commit_message>
Updated information on combined authorities
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E26AF1-1BD4-4898-B3BB-EB8287EEEFD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41107E2-EE54-4EBA-9F00-3A15F05E59B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">uk_local_authorities!$A$1:$AE$460</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">uk_local_authorities!$A$1:$AE$463</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7248" uniqueCount="4334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7272" uniqueCount="4349">
   <si>
     <t>local-authority-code</t>
   </si>
@@ -13036,6 +13036,51 @@
   </si>
   <si>
     <t>BS-6879</t>
+  </si>
+  <si>
+    <t>NECA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North East Combined Authority	</t>
+  </si>
+  <si>
+    <t>West Yorkshire Combined Authority</t>
+  </si>
+  <si>
+    <t>WYCA</t>
+  </si>
+  <si>
+    <t>North of Tyne Combined Authority</t>
+  </si>
+  <si>
+    <t>NTCA</t>
+  </si>
+  <si>
+    <t>E47000008</t>
+  </si>
+  <si>
+    <t>E47000001</t>
+  </si>
+  <si>
+    <t>E47000006</t>
+  </si>
+  <si>
+    <t>E47000009</t>
+  </si>
+  <si>
+    <t>E47000007</t>
+  </si>
+  <si>
+    <t>E47000010</t>
+  </si>
+  <si>
+    <t>E47000003</t>
+  </si>
+  <si>
+    <t>E47000011</t>
+  </si>
+  <si>
+    <t>Newcastle Upon Tyne, North Tyneside and Northumberland Combined Authority</t>
   </si>
 </sst>
 </file>
@@ -13892,11 +13937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE460"/>
+  <dimension ref="A1:AE463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18725,6 +18770,9 @@
       <c r="L72" s="1">
         <v>41730</v>
       </c>
+      <c r="O72" t="s">
+        <v>4340</v>
+      </c>
       <c r="V72" t="s">
         <v>4116</v>
       </c>
@@ -21936,6 +21984,9 @@
       <c r="L122" s="1">
         <v>41730</v>
       </c>
+      <c r="O122" t="s">
+        <v>4341</v>
+      </c>
       <c r="V122" t="s">
         <v>4118</v>
       </c>
@@ -35245,6 +35296,12 @@
       <c r="G322" t="s">
         <v>4106</v>
       </c>
+      <c r="L322" s="1">
+        <v>41730</v>
+      </c>
+      <c r="O322" t="s">
+        <v>4342</v>
+      </c>
       <c r="V322" t="s">
         <v>4115</v>
       </c>
@@ -36051,6 +36108,9 @@
       <c r="L335" s="1">
         <v>41730</v>
       </c>
+      <c r="O335" t="s">
+        <v>4343</v>
+      </c>
       <c r="V335" t="s">
         <v>4119</v>
       </c>
@@ -36900,7 +36960,10 @@
         <v>4108</v>
       </c>
       <c r="L348" s="1">
-        <v>41730</v>
+        <v>42538</v>
+      </c>
+      <c r="O348" t="s">
+        <v>4344</v>
       </c>
       <c r="V348" t="s">
         <v>4117</v>
@@ -42591,8 +42654,80 @@
         <v>-0.81157084150603698</v>
       </c>
     </row>
+    <row r="461" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>4326</v>
+      </c>
+      <c r="B461" t="s">
+        <v>4334</v>
+      </c>
+      <c r="D461" t="s">
+        <v>4113</v>
+      </c>
+      <c r="E461" t="s">
+        <v>4114</v>
+      </c>
+      <c r="G461" t="s">
+        <v>4335</v>
+      </c>
+      <c r="L461" s="1">
+        <v>41744</v>
+      </c>
+      <c r="O461" t="s">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="462" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>4326</v>
+      </c>
+      <c r="B462" t="s">
+        <v>4337</v>
+      </c>
+      <c r="D462" t="s">
+        <v>4113</v>
+      </c>
+      <c r="E462" t="s">
+        <v>4114</v>
+      </c>
+      <c r="G462" t="s">
+        <v>4336</v>
+      </c>
+      <c r="L462" s="1">
+        <v>41730</v>
+      </c>
+      <c r="O462" t="s">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="463" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>4326</v>
+      </c>
+      <c r="B463" t="s">
+        <v>4339</v>
+      </c>
+      <c r="D463" t="s">
+        <v>4113</v>
+      </c>
+      <c r="E463" t="s">
+        <v>4114</v>
+      </c>
+      <c r="G463" t="s">
+        <v>4338</v>
+      </c>
+      <c r="H463" t="s">
+        <v>4348</v>
+      </c>
+      <c r="L463" s="1">
+        <v>43406</v>
+      </c>
+      <c r="O463" t="s">
+        <v>4347</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AE460" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}"/>
+  <autoFilter ref="A1:AE463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed stray whitespace from gss codes
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC7131-5FB2-4546-9ED0-65B3317AFD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8509D3C8-25E0-4C90-9EFB-E9E71BB74945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12999,18 +12999,12 @@
     <t>North Northamptonshire</t>
   </si>
   <si>
-    <t>E06000061 </t>
-  </si>
-  <si>
     <t>West Northamptonshire Council</t>
   </si>
   <si>
     <t>West Northamptonshire</t>
   </si>
   <si>
-    <t>E06000062 </t>
-  </si>
-  <si>
     <t>nation</t>
   </si>
   <si>
@@ -13081,6 +13075,12 @@
   </si>
   <si>
     <t>Newcastle Upon Tyne, North Tyneside and Northumberland Combined Authority</t>
+  </si>
+  <si>
+    <t>E06000062</t>
+  </si>
+  <si>
+    <t>E06000061</t>
   </si>
 </sst>
 </file>
@@ -13939,9 +13939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE463"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P376" sqref="P376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13967,7 +13967,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4325</v>
+        <v>4323</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -14015,7 +14015,7 @@
         <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>4331</v>
+        <v>4329</v>
       </c>
       <c r="R1" t="s">
         <v>14</v>
@@ -14030,13 +14030,13 @@
         <v>16</v>
       </c>
       <c r="V1" t="s">
-        <v>4333</v>
+        <v>4331</v>
       </c>
       <c r="W1" t="s">
         <v>1</v>
       </c>
       <c r="X1" t="s">
-        <v>4327</v>
+        <v>4325</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>17</v>
@@ -14062,7 +14062,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -14127,7 +14127,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -14192,7 +14192,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -14257,7 +14257,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -14322,7 +14322,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -14387,7 +14387,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
@@ -14452,7 +14452,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -14517,7 +14517,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B9" t="s">
         <v>87</v>
@@ -14582,7 +14582,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B10" t="s">
         <v>96</v>
@@ -14647,7 +14647,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
@@ -14712,7 +14712,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B12" t="s">
         <v>114</v>
@@ -14780,7 +14780,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B13" t="s">
         <v>124</v>
@@ -14845,7 +14845,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B14" t="s">
         <v>132</v>
@@ -14919,7 +14919,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B15" t="s">
         <v>145</v>
@@ -14993,7 +14993,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B16" t="s">
         <v>155</v>
@@ -15067,7 +15067,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B17" t="s">
         <v>165</v>
@@ -15135,7 +15135,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B18" t="s">
         <v>177</v>
@@ -15200,7 +15200,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B19" t="s">
         <v>185</v>
@@ -15265,7 +15265,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B20" t="s">
         <v>193</v>
@@ -15336,7 +15336,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B21" t="s">
         <v>80</v>
@@ -15401,7 +15401,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B22" t="s">
         <v>214</v>
@@ -15466,7 +15466,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B23" t="s">
         <v>223</v>
@@ -15534,7 +15534,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B24" t="s">
         <v>233</v>
@@ -15599,7 +15599,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B25" t="s">
         <v>241</v>
@@ -15673,7 +15673,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B26" t="s">
         <v>251</v>
@@ -15744,7 +15744,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B27" t="s">
         <v>260</v>
@@ -15815,7 +15815,7 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B28" t="s">
         <v>269</v>
@@ -15880,7 +15880,7 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B29" t="s">
         <v>278</v>
@@ -15945,7 +15945,7 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B30" t="s">
         <v>4075</v>
@@ -15995,7 +15995,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B31" t="s">
         <v>287</v>
@@ -16069,7 +16069,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B32" t="s">
         <v>297</v>
@@ -16134,7 +16134,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B33" t="s">
         <v>306</v>
@@ -16208,7 +16208,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B34" t="s">
         <v>316</v>
@@ -16279,7 +16279,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B35" t="s">
         <v>325</v>
@@ -16344,7 +16344,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B36" t="s">
         <v>334</v>
@@ -16409,7 +16409,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B37" t="s">
         <v>342</v>
@@ -16474,7 +16474,7 @@
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B38" t="s">
         <v>351</v>
@@ -16539,7 +16539,7 @@
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B39" t="s">
         <v>359</v>
@@ -16604,7 +16604,7 @@
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B40" t="s">
         <v>367</v>
@@ -16669,7 +16669,7 @@
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B41" t="s">
         <v>375</v>
@@ -16734,7 +16734,7 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B42" t="s">
         <v>383</v>
@@ -16811,7 +16811,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B43" t="s">
         <v>394</v>
@@ -16876,7 +16876,7 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B44" t="s">
         <v>402</v>
@@ -16947,7 +16947,7 @@
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B45" t="s">
         <v>411</v>
@@ -17012,7 +17012,7 @@
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B46" t="s">
         <v>413</v>
@@ -17074,7 +17074,7 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B47" t="s">
         <v>427</v>
@@ -17139,7 +17139,7 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B48" t="s">
         <v>436</v>
@@ -17204,7 +17204,7 @@
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B49" t="s">
         <v>444</v>
@@ -17269,7 +17269,7 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B50" t="s">
         <v>452</v>
@@ -17334,7 +17334,7 @@
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B51" t="s">
         <v>460</v>
@@ -17408,7 +17408,7 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B52" t="s">
         <v>470</v>
@@ -17473,7 +17473,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B53" t="s">
         <v>478</v>
@@ -17535,7 +17535,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B54" t="s">
         <v>487</v>
@@ -17609,7 +17609,7 @@
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B55" t="s">
         <v>497</v>
@@ -17677,7 +17677,7 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B56" t="s">
         <v>505</v>
@@ -17742,7 +17742,7 @@
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B57" t="s">
         <v>513</v>
@@ -17807,7 +17807,7 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B58" t="s">
         <v>521</v>
@@ -17872,7 +17872,7 @@
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B59" t="s">
         <v>529</v>
@@ -17937,7 +17937,7 @@
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B60" t="s">
         <v>537</v>
@@ -18002,7 +18002,7 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B61" t="s">
         <v>545</v>
@@ -18067,7 +18067,7 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B62" t="s">
         <v>553</v>
@@ -18141,7 +18141,7 @@
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B63" t="s">
         <v>563</v>
@@ -18212,7 +18212,7 @@
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B64" t="s">
         <v>35</v>
@@ -18274,7 +18274,7 @@
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B65" t="s">
         <v>579</v>
@@ -18339,7 +18339,7 @@
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B66" t="s">
         <v>587</v>
@@ -18404,7 +18404,7 @@
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B67" t="s">
         <v>595</v>
@@ -18478,7 +18478,7 @@
     </row>
     <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B68" t="s">
         <v>605</v>
@@ -18543,7 +18543,7 @@
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B69" t="s">
         <v>613</v>
@@ -18573,7 +18573,7 @@
         <v>44287</v>
       </c>
       <c r="N69" t="s">
-        <v>4328</v>
+        <v>4326</v>
       </c>
       <c r="O69" t="s">
         <v>618</v>
@@ -18614,7 +18614,7 @@
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B70" t="s">
         <v>621</v>
@@ -18679,7 +18679,7 @@
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B71" t="s">
         <v>629</v>
@@ -18750,7 +18750,7 @@
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B72" t="s">
         <v>4116</v>
@@ -18768,7 +18768,7 @@
         <v>41730</v>
       </c>
       <c r="O72" t="s">
-        <v>4340</v>
+        <v>4338</v>
       </c>
       <c r="V72" t="s">
         <v>4116</v>
@@ -18782,7 +18782,7 @@
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B73" t="s">
         <v>638</v>
@@ -18847,7 +18847,7 @@
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B74" t="s">
         <v>647</v>
@@ -18915,7 +18915,7 @@
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B75" t="s">
         <v>655</v>
@@ -18980,7 +18980,7 @@
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B76" t="s">
         <v>663</v>
@@ -19045,7 +19045,7 @@
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B77" t="s">
         <v>672</v>
@@ -19119,7 +19119,7 @@
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B78" t="s">
         <v>682</v>
@@ -19184,7 +19184,7 @@
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B79" t="s">
         <v>690</v>
@@ -19214,7 +19214,7 @@
         <v>44287</v>
       </c>
       <c r="N79" t="s">
-        <v>4329</v>
+        <v>4327</v>
       </c>
       <c r="O79" t="s">
         <v>695</v>
@@ -19255,7 +19255,7 @@
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B80" t="s">
         <v>44</v>
@@ -19317,7 +19317,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B81" t="s">
         <v>705</v>
@@ -19379,7 +19379,7 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B82" t="s">
         <v>713</v>
@@ -19453,7 +19453,7 @@
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B83" t="s">
         <v>271</v>
@@ -19515,7 +19515,7 @@
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B84" t="s">
         <v>731</v>
@@ -19583,7 +19583,7 @@
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B85" t="s">
         <v>480</v>
@@ -19645,7 +19645,7 @@
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B86" t="s">
         <v>747</v>
@@ -19710,7 +19710,7 @@
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B87" t="s">
         <v>4076</v>
@@ -19757,7 +19757,7 @@
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B88" t="s">
         <v>755</v>
@@ -19828,7 +19828,7 @@
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B89" t="s">
         <v>764</v>
@@ -19905,7 +19905,7 @@
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B90" t="s">
         <v>775</v>
@@ -19970,7 +19970,7 @@
     </row>
     <row r="91" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B91" t="s">
         <v>783</v>
@@ -20035,7 +20035,7 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B92" t="s">
         <v>792</v>
@@ -20100,7 +20100,7 @@
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B93" t="s">
         <v>800</v>
@@ -20165,7 +20165,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B94" t="s">
         <v>808</v>
@@ -20230,7 +20230,7 @@
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B95" t="s">
         <v>816</v>
@@ -20295,7 +20295,7 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B96" t="s">
         <v>824</v>
@@ -20357,7 +20357,7 @@
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B97" t="s">
         <v>832</v>
@@ -20422,7 +20422,7 @@
     </row>
     <row r="98" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B98" t="s">
         <v>841</v>
@@ -20490,7 +20490,7 @@
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B99" t="s">
         <v>850</v>
@@ -20555,7 +20555,7 @@
     </row>
     <row r="100" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B100" t="s">
         <v>858</v>
@@ -20620,7 +20620,7 @@
     </row>
     <row r="101" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B101" t="s">
         <v>867</v>
@@ -20685,7 +20685,7 @@
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B102" t="s">
         <v>875</v>
@@ -20715,7 +20715,7 @@
         <v>44287</v>
       </c>
       <c r="N102" t="s">
-        <v>4328</v>
+        <v>4326</v>
       </c>
       <c r="O102" t="s">
         <v>880</v>
@@ -20756,7 +20756,7 @@
     </row>
     <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B103" t="s">
         <v>883</v>
@@ -20821,7 +20821,7 @@
     </row>
     <row r="104" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B104" t="s">
         <v>891</v>
@@ -20889,7 +20889,7 @@
     </row>
     <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B105" t="s">
         <v>901</v>
@@ -20954,7 +20954,7 @@
     </row>
     <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B106" t="s">
         <v>909</v>
@@ -21028,7 +21028,7 @@
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B107" t="s">
         <v>4079</v>
@@ -21075,7 +21075,7 @@
     </row>
     <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B108" t="s">
         <v>107</v>
@@ -21137,7 +21137,7 @@
     </row>
     <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B109" t="s">
         <v>926</v>
@@ -21202,7 +21202,7 @@
     </row>
     <row r="110" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B110" t="s">
         <v>785</v>
@@ -21264,7 +21264,7 @@
     </row>
     <row r="111" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B111" t="s">
         <v>941</v>
@@ -21326,7 +21326,7 @@
     </row>
     <row r="112" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B112" t="s">
         <v>949</v>
@@ -21391,7 +21391,7 @@
     </row>
     <row r="113" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B113" t="s">
         <v>957</v>
@@ -21456,7 +21456,7 @@
     </row>
     <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B114" t="s">
         <v>965</v>
@@ -21521,7 +21521,7 @@
     </row>
     <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B115" t="s">
         <v>973</v>
@@ -21583,7 +21583,7 @@
     </row>
     <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B116" t="s">
         <v>981</v>
@@ -21648,7 +21648,7 @@
     </row>
     <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B117" t="s">
         <v>989</v>
@@ -21719,7 +21719,7 @@
     </row>
     <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B118" t="s">
         <v>998</v>
@@ -21784,7 +21784,7 @@
     </row>
     <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B119" t="s">
         <v>169</v>
@@ -21837,7 +21837,7 @@
     </row>
     <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B120" t="s">
         <v>1016</v>
@@ -21902,7 +21902,7 @@
     </row>
     <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B121" t="s">
         <v>299</v>
@@ -21964,7 +21964,7 @@
     </row>
     <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B122" t="s">
         <v>4118</v>
@@ -21982,7 +21982,7 @@
         <v>41730</v>
       </c>
       <c r="O122" t="s">
-        <v>4341</v>
+        <v>4339</v>
       </c>
       <c r="V122" t="s">
         <v>4118</v>
@@ -21996,7 +21996,7 @@
     </row>
     <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B123" t="s">
         <v>1031</v>
@@ -22061,7 +22061,7 @@
     </row>
     <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B124" t="s">
         <v>1039</v>
@@ -22126,7 +22126,7 @@
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B125" t="s">
         <v>1047</v>
@@ -22191,7 +22191,7 @@
     </row>
     <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B126" t="s">
         <v>1055</v>
@@ -22256,7 +22256,7 @@
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B127" t="s">
         <v>1063</v>
@@ -22321,7 +22321,7 @@
     </row>
     <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B128" t="s">
         <v>1071</v>
@@ -22386,7 +22386,7 @@
     </row>
     <row r="129" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B129" t="s">
         <v>1079</v>
@@ -22451,7 +22451,7 @@
     </row>
     <row r="130" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B130" t="s">
         <v>1087</v>
@@ -22516,7 +22516,7 @@
     </row>
     <row r="131" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B131" t="s">
         <v>1095</v>
@@ -22590,7 +22590,7 @@
     </row>
     <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B132" t="s">
         <v>834</v>
@@ -22652,7 +22652,7 @@
     </row>
     <row r="133" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B133" t="s">
         <v>1112</v>
@@ -22714,7 +22714,7 @@
     </row>
     <row r="134" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B134" t="s">
         <v>1120</v>
@@ -22779,7 +22779,7 @@
     </row>
     <row r="135" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B135" t="s">
         <v>1128</v>
@@ -22844,7 +22844,7 @@
     </row>
     <row r="136" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B136" t="s">
         <v>1136</v>
@@ -22909,7 +22909,7 @@
     </row>
     <row r="137" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B137" t="s">
         <v>1144</v>
@@ -22974,7 +22974,7 @@
     </row>
     <row r="138" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B138" t="s">
         <v>1152</v>
@@ -23039,7 +23039,7 @@
     </row>
     <row r="139" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B139" t="s">
         <v>1160</v>
@@ -23113,7 +23113,7 @@
     </row>
     <row r="140" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B140" t="s">
         <v>1170</v>
@@ -23178,7 +23178,7 @@
     </row>
     <row r="141" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B141" t="s">
         <v>1178</v>
@@ -23243,7 +23243,7 @@
     </row>
     <row r="142" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B142" t="s">
         <v>1186</v>
@@ -23308,7 +23308,7 @@
     </row>
     <row r="143" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B143" t="s">
         <v>1194</v>
@@ -23376,7 +23376,7 @@
     </row>
     <row r="144" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B144" t="s">
         <v>1203</v>
@@ -23444,7 +23444,7 @@
     </row>
     <row r="145" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B145" t="s">
         <v>1212</v>
@@ -23509,7 +23509,7 @@
     </row>
     <row r="146" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B146" t="s">
         <v>1220</v>
@@ -23577,7 +23577,7 @@
     </row>
     <row r="147" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B147" t="s">
         <v>1228</v>
@@ -23651,7 +23651,7 @@
     </row>
     <row r="148" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B148" t="s">
         <v>116</v>
@@ -23713,7 +23713,7 @@
     </row>
     <row r="149" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B149" t="s">
         <v>1245</v>
@@ -23778,7 +23778,7 @@
     </row>
     <row r="150" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B150" t="s">
         <v>1253</v>
@@ -23843,7 +23843,7 @@
     </row>
     <row r="151" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B151" t="s">
         <v>1261</v>
@@ -23908,7 +23908,7 @@
     </row>
     <row r="152" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B152" t="s">
         <v>1269</v>
@@ -23973,7 +23973,7 @@
     </row>
     <row r="153" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B153" t="s">
         <v>1277</v>
@@ -24044,7 +24044,7 @@
     </row>
     <row r="154" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B154" t="s">
         <v>1287</v>
@@ -24118,7 +24118,7 @@
     </row>
     <row r="155" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B155" t="s">
         <v>1297</v>
@@ -24183,7 +24183,7 @@
     </row>
     <row r="156" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B156" t="s">
         <v>1305</v>
@@ -24248,7 +24248,7 @@
     </row>
     <row r="157" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B157" t="s">
         <v>1313</v>
@@ -24316,7 +24316,7 @@
     </row>
     <row r="158" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B158" t="s">
         <v>665</v>
@@ -24378,7 +24378,7 @@
     </row>
     <row r="159" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B159" t="s">
         <v>1329</v>
@@ -24405,7 +24405,7 @@
         <v>44287</v>
       </c>
       <c r="N159" t="s">
-        <v>4328</v>
+        <v>4326</v>
       </c>
       <c r="O159" t="s">
         <v>1334</v>
@@ -24446,7 +24446,7 @@
     </row>
     <row r="160" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B160" t="s">
         <v>1337</v>
@@ -24523,7 +24523,7 @@
     </row>
     <row r="161" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B161" t="s">
         <v>1348</v>
@@ -24594,7 +24594,7 @@
     </row>
     <row r="162" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B162" t="s">
         <v>1358</v>
@@ -24665,7 +24665,7 @@
     </row>
     <row r="163" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B163" t="s">
         <v>1367</v>
@@ -24730,7 +24730,7 @@
     </row>
     <row r="164" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B164" t="s">
         <v>1375</v>
@@ -24801,7 +24801,7 @@
     </row>
     <row r="165" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B165" t="s">
         <v>1384</v>
@@ -24866,7 +24866,7 @@
     </row>
     <row r="166" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B166" t="s">
         <v>62</v>
@@ -24928,7 +24928,7 @@
     </row>
     <row r="167" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B167" t="s">
         <v>1399</v>
@@ -24990,7 +24990,7 @@
     </row>
     <row r="168" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B168" t="s">
         <v>1407</v>
@@ -25067,7 +25067,7 @@
     </row>
     <row r="169" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B169" t="s">
         <v>4121</v>
@@ -25096,7 +25096,7 @@
     </row>
     <row r="170" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B170" t="s">
         <v>1418</v>
@@ -25167,7 +25167,7 @@
     </row>
     <row r="171" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B171" t="s">
         <v>216</v>
@@ -25229,7 +25229,7 @@
     </row>
     <row r="172" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B172" t="s">
         <v>1434</v>
@@ -25291,7 +25291,7 @@
     </row>
     <row r="173" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B173" t="s">
         <v>1442</v>
@@ -25356,7 +25356,7 @@
     </row>
     <row r="174" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B174" t="s">
         <v>1450</v>
@@ -25424,7 +25424,7 @@
     </row>
     <row r="175" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B175" t="s">
         <v>1459</v>
@@ -25489,7 +25489,7 @@
     </row>
     <row r="176" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B176" t="s">
         <v>280</v>
@@ -25551,7 +25551,7 @@
     </row>
     <row r="177" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B177" t="s">
         <v>1474</v>
@@ -25619,7 +25619,7 @@
     </row>
     <row r="178" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B178" t="s">
         <v>1483</v>
@@ -25687,7 +25687,7 @@
     </row>
     <row r="179" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B179" t="s">
         <v>1493</v>
@@ -25761,7 +25761,7 @@
     </row>
     <row r="180" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B180" t="s">
         <v>1503</v>
@@ -25826,7 +25826,7 @@
     </row>
     <row r="181" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B181" t="s">
         <v>1511</v>
@@ -25891,7 +25891,7 @@
     </row>
     <row r="182" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B182" t="s">
         <v>1519</v>
@@ -25962,7 +25962,7 @@
     </row>
     <row r="183" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B183" t="s">
         <v>1528</v>
@@ -26027,7 +26027,7 @@
     </row>
     <row r="184" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B184" t="s">
         <v>1536</v>
@@ -26092,7 +26092,7 @@
     </row>
     <row r="185" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B185" t="s">
         <v>1544</v>
@@ -26166,7 +26166,7 @@
     </row>
     <row r="186" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B186" t="s">
         <v>1554</v>
@@ -26231,7 +26231,7 @@
     </row>
     <row r="187" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B187" t="s">
         <v>1562</v>
@@ -26308,7 +26308,7 @@
     </row>
     <row r="188" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B188" t="s">
         <v>1573</v>
@@ -26373,7 +26373,7 @@
     </row>
     <row r="189" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B189" t="s">
         <v>1581</v>
@@ -26438,7 +26438,7 @@
     </row>
     <row r="190" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B190" t="s">
         <v>1590</v>
@@ -26512,7 +26512,7 @@
     </row>
     <row r="191" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B191" t="s">
         <v>1600</v>
@@ -26577,7 +26577,7 @@
     </row>
     <row r="192" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B192" t="s">
         <v>1608</v>
@@ -26642,7 +26642,7 @@
     </row>
     <row r="193" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B193" t="s">
         <v>1616</v>
@@ -26710,7 +26710,7 @@
     </row>
     <row r="194" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B194" t="s">
         <v>1624</v>
@@ -26775,7 +26775,7 @@
     </row>
     <row r="195" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B195" t="s">
         <v>1632</v>
@@ -26849,7 +26849,7 @@
     </row>
     <row r="196" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B196" t="s">
         <v>1642</v>
@@ -26914,7 +26914,7 @@
     </row>
     <row r="197" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B197" t="s">
         <v>1650</v>
@@ -26976,7 +26976,7 @@
     </row>
     <row r="198" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B198" t="s">
         <v>1658</v>
@@ -27044,7 +27044,7 @@
     </row>
     <row r="199" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B199" t="s">
         <v>1667</v>
@@ -27109,7 +27109,7 @@
     </row>
     <row r="200" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B200" t="s">
         <v>1675</v>
@@ -27174,7 +27174,7 @@
     </row>
     <row r="201" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B201" t="s">
         <v>1683</v>
@@ -27248,7 +27248,7 @@
     </row>
     <row r="202" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B202" t="s">
         <v>1693</v>
@@ -27319,7 +27319,7 @@
     </row>
     <row r="203" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B203" t="s">
         <v>1702</v>
@@ -27384,7 +27384,7 @@
     </row>
     <row r="204" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B204" t="s">
         <v>344</v>
@@ -27446,7 +27446,7 @@
     </row>
     <row r="205" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B205" t="s">
         <v>1717</v>
@@ -27523,7 +27523,7 @@
     </row>
     <row r="206" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B206" t="s">
         <v>1728</v>
@@ -27588,7 +27588,7 @@
     </row>
     <row r="207" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B207" t="s">
         <v>1736</v>
@@ -27653,7 +27653,7 @@
     </row>
     <row r="208" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B208" t="s">
         <v>1744</v>
@@ -27727,7 +27727,7 @@
     </row>
     <row r="209" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B209" t="s">
         <v>1754</v>
@@ -27792,7 +27792,7 @@
     </row>
     <row r="210" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B210" t="s">
         <v>1762</v>
@@ -27822,7 +27822,7 @@
         <v>44287</v>
       </c>
       <c r="N210" t="s">
-        <v>4329</v>
+        <v>4327</v>
       </c>
       <c r="O210" t="s">
         <v>1767</v>
@@ -27863,7 +27863,7 @@
     </row>
     <row r="211" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B211" t="s">
         <v>1770</v>
@@ -27928,7 +27928,7 @@
     </row>
     <row r="212" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B212" t="s">
         <v>1778</v>
@@ -28002,7 +28002,7 @@
     </row>
     <row r="213" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B213" t="s">
         <v>327</v>
@@ -28029,7 +28029,7 @@
         <v>44287</v>
       </c>
       <c r="N213" t="s">
-        <v>4330</v>
+        <v>4328</v>
       </c>
       <c r="O213" t="s">
         <v>1792</v>
@@ -28070,7 +28070,7 @@
     </row>
     <row r="214" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B214" t="s">
         <v>71</v>
@@ -28132,7 +28132,7 @@
     </row>
     <row r="215" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B215" t="s">
         <v>1802</v>
@@ -28203,7 +28203,7 @@
     </row>
     <row r="216" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B216" t="s">
         <v>1811</v>
@@ -28271,7 +28271,7 @@
     </row>
     <row r="217" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B217" t="s">
         <v>1820</v>
@@ -28336,7 +28336,7 @@
     </row>
     <row r="218" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B218" t="s">
         <v>1828</v>
@@ -28401,7 +28401,7 @@
     </row>
     <row r="219" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B219" t="s">
         <v>1836</v>
@@ -28466,7 +28466,7 @@
     </row>
     <row r="220" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B220" t="s">
         <v>640</v>
@@ -28528,7 +28528,7 @@
     </row>
     <row r="221" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B221" t="s">
         <v>1851</v>
@@ -28593,7 +28593,7 @@
     </row>
     <row r="222" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B222" t="s">
         <v>1860</v>
@@ -28664,7 +28664,7 @@
     </row>
     <row r="223" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B223" t="s">
         <v>98</v>
@@ -28726,7 +28726,7 @@
     </row>
     <row r="224" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B224" t="s">
         <v>1876</v>
@@ -28788,7 +28788,7 @@
     </row>
     <row r="225" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B225" t="s">
         <v>1884</v>
@@ -28853,7 +28853,7 @@
     </row>
     <row r="226" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B226" t="s">
         <v>1892</v>
@@ -28927,7 +28927,7 @@
     </row>
     <row r="227" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B227" t="s">
         <v>1902</v>
@@ -28995,7 +28995,7 @@
     </row>
     <row r="228" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B228" t="s">
         <v>1912</v>
@@ -29069,7 +29069,7 @@
     </row>
     <row r="229" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B229" t="s">
         <v>1922</v>
@@ -29134,7 +29134,7 @@
     </row>
     <row r="230" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B230" t="s">
         <v>1930</v>
@@ -29208,7 +29208,7 @@
     </row>
     <row r="231" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B231" t="s">
         <v>1940</v>
@@ -29270,7 +29270,7 @@
     </row>
     <row r="232" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B232" t="s">
         <v>1948</v>
@@ -29344,7 +29344,7 @@
     </row>
     <row r="233" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B233" t="s">
         <v>1958</v>
@@ -29415,7 +29415,7 @@
     </row>
     <row r="234" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B234" t="s">
         <v>1967</v>
@@ -29480,7 +29480,7 @@
     </row>
     <row r="235" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B235" t="s">
         <v>1975</v>
@@ -29554,7 +29554,7 @@
     </row>
     <row r="236" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B236" t="s">
         <v>1985</v>
@@ -29619,7 +29619,7 @@
     </row>
     <row r="237" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B237" t="s">
         <v>1993</v>
@@ -29687,7 +29687,7 @@
     </row>
     <row r="238" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B238" t="s">
         <v>2002</v>
@@ -29752,7 +29752,7 @@
     </row>
     <row r="239" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B239" t="s">
         <v>2010</v>
@@ -29817,7 +29817,7 @@
     </row>
     <row r="240" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B240" t="s">
         <v>2018</v>
@@ -29882,7 +29882,7 @@
     </row>
     <row r="241" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B241" t="s">
         <v>2026</v>
@@ -29947,7 +29947,7 @@
     </row>
     <row r="242" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B242" t="s">
         <v>2034</v>
@@ -30012,7 +30012,7 @@
     </row>
     <row r="243" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B243" t="s">
         <v>2042</v>
@@ -30077,7 +30077,7 @@
     </row>
     <row r="244" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B244" t="s">
         <v>2050</v>
@@ -30148,7 +30148,7 @@
     </row>
     <row r="245" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B245" t="s">
         <v>2059</v>
@@ -30213,7 +30213,7 @@
     </row>
     <row r="246" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B246" t="s">
         <v>2067</v>
@@ -30278,7 +30278,7 @@
     </row>
     <row r="247" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B247" t="s">
         <v>2075</v>
@@ -30343,7 +30343,7 @@
     </row>
     <row r="248" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B248" t="s">
         <v>2083</v>
@@ -30408,7 +30408,7 @@
     </row>
     <row r="249" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B249" t="s">
         <v>2091</v>
@@ -30482,7 +30482,7 @@
     </row>
     <row r="250" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B250" t="s">
         <v>2101</v>
@@ -30547,7 +30547,7 @@
     </row>
     <row r="251" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B251" t="s">
         <v>2109</v>
@@ -30615,7 +30615,7 @@
     </row>
     <row r="252" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B252" t="s">
         <v>2118</v>
@@ -30686,7 +30686,7 @@
     </row>
     <row r="253" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B253" t="s">
         <v>2127</v>
@@ -30751,7 +30751,7 @@
     </row>
     <row r="254" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B254" t="s">
         <v>2135</v>
@@ -30816,7 +30816,7 @@
     </row>
     <row r="255" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B255" t="s">
         <v>2143</v>
@@ -30881,7 +30881,7 @@
     </row>
     <row r="256" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B256" t="s">
         <v>4120</v>
@@ -30910,7 +30910,7 @@
     </row>
     <row r="257" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B257" t="s">
         <v>2151</v>
@@ -30975,7 +30975,7 @@
     </row>
     <row r="258" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B258" t="s">
         <v>2159</v>
@@ -31037,7 +31037,7 @@
     </row>
     <row r="259" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B259" t="s">
         <v>2167</v>
@@ -31102,7 +31102,7 @@
     </row>
     <row r="260" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B260" t="s">
         <v>2175</v>
@@ -31167,7 +31167,7 @@
     </row>
     <row r="261" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B261" t="s">
         <v>2183</v>
@@ -31232,7 +31232,7 @@
     </row>
     <row r="262" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B262" t="s">
         <v>89</v>
@@ -31294,7 +31294,7 @@
     </row>
     <row r="263" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B263" t="s">
         <v>2198</v>
@@ -31365,7 +31365,7 @@
     </row>
     <row r="264" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B264" t="s">
         <v>2207</v>
@@ -31439,7 +31439,7 @@
     </row>
     <row r="265" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B265" t="s">
         <v>2217</v>
@@ -31504,7 +31504,7 @@
     </row>
     <row r="266" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B266" t="s">
         <v>2225</v>
@@ -31575,7 +31575,7 @@
     </row>
     <row r="267" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B267" t="s">
         <v>2233</v>
@@ -31646,7 +31646,7 @@
     </row>
     <row r="268" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B268" t="s">
         <v>2242</v>
@@ -31720,7 +31720,7 @@
     </row>
     <row r="269" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B269" t="s">
         <v>2252</v>
@@ -31785,7 +31785,7 @@
     </row>
     <row r="270" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B270" t="s">
         <v>2260</v>
@@ -31859,7 +31859,7 @@
     </row>
     <row r="271" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B271" t="s">
         <v>2270</v>
@@ -31924,7 +31924,7 @@
     </row>
     <row r="272" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B272" t="s">
         <v>2278</v>
@@ -31995,7 +31995,7 @@
     </row>
     <row r="273" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B273" t="s">
         <v>2287</v>
@@ -32060,7 +32060,7 @@
     </row>
     <row r="274" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B274" t="s">
         <v>2295</v>
@@ -32131,7 +32131,7 @@
     </row>
     <row r="275" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B275" t="s">
         <v>2304</v>
@@ -32205,7 +32205,7 @@
     </row>
     <row r="276" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B276" t="s">
         <v>2314</v>
@@ -32276,7 +32276,7 @@
     </row>
     <row r="277" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B277" t="s">
         <v>2323</v>
@@ -32341,7 +32341,7 @@
     </row>
     <row r="278" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B278" t="s">
         <v>2331</v>
@@ -32371,7 +32371,7 @@
         <v>44287</v>
       </c>
       <c r="N278" t="s">
-        <v>4329</v>
+        <v>4327</v>
       </c>
       <c r="O278" t="s">
         <v>2336</v>
@@ -32412,7 +32412,7 @@
     </row>
     <row r="279" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B279" t="s">
         <v>2339</v>
@@ -32483,7 +32483,7 @@
     </row>
     <row r="280" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B280" t="s">
         <v>1583</v>
@@ -32545,7 +32545,7 @@
     </row>
     <row r="281" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B281" t="s">
         <v>2355</v>
@@ -32619,7 +32619,7 @@
     </row>
     <row r="282" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B282" t="s">
         <v>2366</v>
@@ -32684,7 +32684,7 @@
     </row>
     <row r="283" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B283" t="s">
         <v>2374</v>
@@ -32749,7 +32749,7 @@
     </row>
     <row r="284" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B284" t="s">
         <v>2382</v>
@@ -32814,7 +32814,7 @@
     </row>
     <row r="285" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B285" t="s">
         <v>860</v>
@@ -32876,7 +32876,7 @@
     </row>
     <row r="286" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B286" t="s">
         <v>2397</v>
@@ -32938,7 +32938,7 @@
     </row>
     <row r="287" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B287" t="s">
         <v>2405</v>
@@ -33003,7 +33003,7 @@
     </row>
     <row r="288" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B288" t="s">
         <v>2413</v>
@@ -33068,7 +33068,7 @@
     </row>
     <row r="289" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B289" t="s">
         <v>2421</v>
@@ -33142,7 +33142,7 @@
     </row>
     <row r="290" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B290" t="s">
         <v>2431</v>
@@ -33207,7 +33207,7 @@
     </row>
     <row r="291" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B291" t="s">
         <v>2439</v>
@@ -33281,7 +33281,7 @@
     </row>
     <row r="292" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B292" t="s">
         <v>2449</v>
@@ -33346,7 +33346,7 @@
     </row>
     <row r="293" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B293" t="s">
         <v>2457</v>
@@ -33411,7 +33411,7 @@
     </row>
     <row r="294" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B294" t="s">
         <v>2465</v>
@@ -33476,7 +33476,7 @@
     </row>
     <row r="295" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B295" t="s">
         <v>429</v>
@@ -33538,7 +33538,7 @@
     </row>
     <row r="296" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B296" t="s">
         <v>2480</v>
@@ -33612,7 +33612,7 @@
     </row>
     <row r="297" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B297" t="s">
         <v>2491</v>
@@ -33680,7 +33680,7 @@
     </row>
     <row r="298" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B298" t="s">
         <v>2500</v>
@@ -33751,7 +33751,7 @@
     </row>
     <row r="299" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B299" t="s">
         <v>2509</v>
@@ -33813,7 +33813,7 @@
     </row>
     <row r="300" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B300" t="s">
         <v>2517</v>
@@ -33878,7 +33878,7 @@
     </row>
     <row r="301" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B301" t="s">
         <v>2525</v>
@@ -33952,7 +33952,7 @@
     </row>
     <row r="302" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B302" t="s">
         <v>2535</v>
@@ -34017,7 +34017,7 @@
     </row>
     <row r="303" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B303" t="s">
         <v>2543</v>
@@ -34082,7 +34082,7 @@
     </row>
     <row r="304" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B304" t="s">
         <v>4077</v>
@@ -34132,7 +34132,7 @@
     </row>
     <row r="305" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B305" t="s">
         <v>2551</v>
@@ -34203,7 +34203,7 @@
     </row>
     <row r="306" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B306" t="s">
         <v>2560</v>
@@ -34268,7 +34268,7 @@
     </row>
     <row r="307" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B307" t="s">
         <v>2568</v>
@@ -34330,7 +34330,7 @@
     </row>
     <row r="308" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B308" t="s">
         <v>2576</v>
@@ -34395,7 +34395,7 @@
     </row>
     <row r="309" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B309" t="s">
         <v>2584</v>
@@ -34460,7 +34460,7 @@
     </row>
     <row r="310" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B310" t="s">
         <v>2592</v>
@@ -34525,7 +34525,7 @@
     </row>
     <row r="311" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B311" t="s">
         <v>2600</v>
@@ -34590,7 +34590,7 @@
     </row>
     <row r="312" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B312" t="s">
         <v>2608</v>
@@ -34655,7 +34655,7 @@
     </row>
     <row r="313" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B313" t="s">
         <v>2616</v>
@@ -34732,7 +34732,7 @@
     </row>
     <row r="314" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B314" t="s">
         <v>2627</v>
@@ -34797,7 +34797,7 @@
     </row>
     <row r="315" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B315" t="s">
         <v>2635</v>
@@ -34862,7 +34862,7 @@
     </row>
     <row r="316" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B316" t="s">
         <v>2643</v>
@@ -34936,7 +34936,7 @@
     </row>
     <row r="317" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B317" t="s">
         <v>2653</v>
@@ -35010,7 +35010,7 @@
     </row>
     <row r="318" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B318" t="s">
         <v>2663</v>
@@ -35078,7 +35078,7 @@
     </row>
     <row r="319" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B319" t="s">
         <v>2672</v>
@@ -35143,7 +35143,7 @@
     </row>
     <row r="320" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B320" t="s">
         <v>2680</v>
@@ -35214,7 +35214,7 @@
     </row>
     <row r="321" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B321" t="s">
         <v>2689</v>
@@ -35279,7 +35279,7 @@
     </row>
     <row r="322" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B322" t="s">
         <v>4115</v>
@@ -35297,7 +35297,7 @@
         <v>41730</v>
       </c>
       <c r="O322" t="s">
-        <v>4342</v>
+        <v>4340</v>
       </c>
       <c r="V322" t="s">
         <v>4115</v>
@@ -35311,7 +35311,7 @@
     </row>
     <row r="323" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B323" t="s">
         <v>2697</v>
@@ -35376,7 +35376,7 @@
     </row>
     <row r="324" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B324" t="s">
         <v>2705</v>
@@ -35441,7 +35441,7 @@
     </row>
     <row r="325" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B325" t="s">
         <v>2713</v>
@@ -35506,7 +35506,7 @@
     </row>
     <row r="326" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B326" t="s">
         <v>2721</v>
@@ -35571,7 +35571,7 @@
     </row>
     <row r="327" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B327" t="s">
         <v>893</v>
@@ -35633,7 +35633,7 @@
     </row>
     <row r="328" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B328" t="s">
         <v>2736</v>
@@ -35695,7 +35695,7 @@
     </row>
     <row r="329" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B329" t="s">
         <v>2744</v>
@@ -35757,7 +35757,7 @@
     </row>
     <row r="330" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B330" t="s">
         <v>2752</v>
@@ -35822,7 +35822,7 @@
     </row>
     <row r="331" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B331" t="s">
         <v>2760</v>
@@ -35896,7 +35896,7 @@
     </row>
     <row r="332" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B332" t="s">
         <v>2770</v>
@@ -35961,7 +35961,7 @@
     </row>
     <row r="333" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B333" t="s">
         <v>2778</v>
@@ -36023,7 +36023,7 @@
     </row>
     <row r="334" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B334" t="s">
         <v>2786</v>
@@ -36088,7 +36088,7 @@
     </row>
     <row r="335" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B335" t="s">
         <v>4119</v>
@@ -36106,7 +36106,7 @@
         <v>41730</v>
       </c>
       <c r="O335" t="s">
-        <v>4343</v>
+        <v>4341</v>
       </c>
       <c r="V335" t="s">
         <v>4119</v>
@@ -36120,7 +36120,7 @@
     </row>
     <row r="336" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B336" t="s">
         <v>2794</v>
@@ -36150,7 +36150,7 @@
         <v>44287</v>
       </c>
       <c r="N336" t="s">
-        <v>4328</v>
+        <v>4326</v>
       </c>
       <c r="O336" t="s">
         <v>2799</v>
@@ -36191,7 +36191,7 @@
     </row>
     <row r="337" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B337" t="s">
         <v>2802</v>
@@ -36259,7 +36259,7 @@
     </row>
     <row r="338" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B338" t="s">
         <v>2811</v>
@@ -36324,7 +36324,7 @@
     </row>
     <row r="339" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B339" t="s">
         <v>2820</v>
@@ -36389,7 +36389,7 @@
     </row>
     <row r="340" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B340" t="s">
         <v>2828</v>
@@ -36460,7 +36460,7 @@
     </row>
     <row r="341" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B341" t="s">
         <v>2837</v>
@@ -36534,7 +36534,7 @@
     </row>
     <row r="342" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B342" t="s">
         <v>2847</v>
@@ -36599,7 +36599,7 @@
     </row>
     <row r="343" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B343" t="s">
         <v>2855</v>
@@ -36670,7 +36670,7 @@
     </row>
     <row r="344" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B344" t="s">
         <v>2864</v>
@@ -36735,7 +36735,7 @@
     </row>
     <row r="345" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B345" t="s">
         <v>2872</v>
@@ -36800,7 +36800,7 @@
     </row>
     <row r="346" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B346" t="s">
         <v>2880</v>
@@ -36871,7 +36871,7 @@
     </row>
     <row r="347" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B347" t="s">
         <v>2889</v>
@@ -36942,7 +36942,7 @@
     </row>
     <row r="348" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B348" t="s">
         <v>4117</v>
@@ -36960,7 +36960,7 @@
         <v>42538</v>
       </c>
       <c r="O348" t="s">
-        <v>4344</v>
+        <v>4342</v>
       </c>
       <c r="V348" t="s">
         <v>4117</v>
@@ -36974,7 +36974,7 @@
     </row>
     <row r="349" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B349" t="s">
         <v>2898</v>
@@ -37039,7 +37039,7 @@
     </row>
     <row r="350" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B350" t="s">
         <v>2906</v>
@@ -37113,7 +37113,7 @@
     </row>
     <row r="351" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B351" t="s">
         <v>2916</v>
@@ -37178,7 +37178,7 @@
     </row>
     <row r="352" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B352" t="s">
         <v>2924</v>
@@ -37243,7 +37243,7 @@
     </row>
     <row r="353" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B353" t="s">
         <v>2932</v>
@@ -37317,7 +37317,7 @@
     </row>
     <row r="354" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B354" t="s">
         <v>25</v>
@@ -37379,7 +37379,7 @@
     </row>
     <row r="355" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B355" t="s">
         <v>2949</v>
@@ -37447,7 +37447,7 @@
     </row>
     <row r="356" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B356" t="s">
         <v>2957</v>
@@ -37512,7 +37512,7 @@
     </row>
     <row r="357" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B357" t="s">
         <v>2965</v>
@@ -37583,7 +37583,7 @@
     </row>
     <row r="358" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B358" t="s">
         <v>2974</v>
@@ -37657,7 +37657,7 @@
     </row>
     <row r="359" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B359" t="s">
         <v>4078</v>
@@ -37704,7 +37704,7 @@
     </row>
     <row r="360" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B360" t="s">
         <v>2984</v>
@@ -37769,7 +37769,7 @@
     </row>
     <row r="361" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B361" t="s">
         <v>2992</v>
@@ -37831,7 +37831,7 @@
     </row>
     <row r="362" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B362" t="s">
         <v>53</v>
@@ -37893,7 +37893,7 @@
     </row>
     <row r="363" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B363" t="s">
         <v>3007</v>
@@ -37955,7 +37955,7 @@
     </row>
     <row r="364" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B364" t="s">
         <v>3015</v>
@@ -38020,7 +38020,7 @@
     </row>
     <row r="365" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B365" t="s">
         <v>3023</v>
@@ -38085,7 +38085,7 @@
     </row>
     <row r="366" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B366" t="s">
         <v>3031</v>
@@ -38150,7 +38150,7 @@
     </row>
     <row r="367" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B367" t="s">
         <v>3039</v>
@@ -38224,10 +38224,10 @@
     </row>
     <row r="368" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
+        <v>4324</v>
+      </c>
+      <c r="B368" t="s">
         <v>4326</v>
-      </c>
-      <c r="B368" t="s">
-        <v>4328</v>
       </c>
       <c r="C368" t="s">
         <v>4309</v>
@@ -38248,19 +38248,19 @@
         <v>44287</v>
       </c>
       <c r="O368" s="4" t="s">
-        <v>4321</v>
+        <v>4348</v>
       </c>
       <c r="Y368"/>
       <c r="AE368" t="s">
-        <v>4332</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="369" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B369" t="s">
-        <v>4329</v>
+        <v>4327</v>
       </c>
       <c r="C369" t="s">
         <v>4309</v>
@@ -38272,20 +38272,20 @@
         <v>135</v>
       </c>
       <c r="G369" t="s">
+        <v>4321</v>
+      </c>
+      <c r="H369" t="s">
         <v>4322</v>
-      </c>
-      <c r="H369" t="s">
-        <v>4323</v>
       </c>
       <c r="L369" s="1">
         <v>44287</v>
       </c>
       <c r="O369" s="4" t="s">
-        <v>4324</v>
+        <v>4347</v>
       </c>
       <c r="Y369"/>
       <c r="AE369" t="s">
-        <v>4332</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="370" spans="1:31" x14ac:dyDescent="0.25">
@@ -42611,7 +42611,7 @@
     </row>
     <row r="460" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B460" t="s">
         <v>4129</v>
@@ -42653,10 +42653,10 @@
     </row>
     <row r="461" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B461" t="s">
-        <v>4334</v>
+        <v>4332</v>
       </c>
       <c r="D461" t="s">
         <v>4113</v>
@@ -42665,21 +42665,21 @@
         <v>4114</v>
       </c>
       <c r="G461" t="s">
-        <v>4335</v>
+        <v>4333</v>
       </c>
       <c r="L461" s="1">
         <v>41744</v>
       </c>
       <c r="O461" t="s">
-        <v>4345</v>
+        <v>4343</v>
       </c>
     </row>
     <row r="462" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B462" t="s">
-        <v>4337</v>
+        <v>4335</v>
       </c>
       <c r="D462" t="s">
         <v>4113</v>
@@ -42688,21 +42688,21 @@
         <v>4114</v>
       </c>
       <c r="G462" t="s">
-        <v>4336</v>
+        <v>4334</v>
       </c>
       <c r="L462" s="1">
         <v>41730</v>
       </c>
       <c r="O462" t="s">
-        <v>4346</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="463" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>4326</v>
+        <v>4324</v>
       </c>
       <c r="B463" t="s">
-        <v>4339</v>
+        <v>4337</v>
       </c>
       <c r="D463" t="s">
         <v>4113</v>
@@ -42711,16 +42711,16 @@
         <v>4114</v>
       </c>
       <c r="G463" t="s">
-        <v>4338</v>
+        <v>4336</v>
       </c>
       <c r="H463" t="s">
-        <v>4348</v>
+        <v>4346</v>
       </c>
       <c r="L463" s="1">
         <v>43406</v>
       </c>
       <c r="O463" t="s">
-        <v>4347</v>
+        <v>4345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more details on combined authorities
And matched to constituent councils
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8509D3C8-25E0-4C90-9EFB-E9E71BB74945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6B13B-D41C-40B6-A396-4F0B255A23AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">uk_local_authorities!$A$1:$AE$463</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7271" uniqueCount="4349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7519" uniqueCount="4358">
   <si>
     <t>local-authority-code</t>
   </si>
@@ -13081,6 +13082,33 @@
   </si>
   <si>
     <t>E06000061</t>
+  </si>
+  <si>
+    <t>SCO</t>
+  </si>
+  <si>
+    <t>WPA</t>
+  </si>
+  <si>
+    <t>NID</t>
+  </si>
+  <si>
+    <t>Welsh Unitary Council</t>
+  </si>
+  <si>
+    <t>NI District Council</t>
+  </si>
+  <si>
+    <t>Scottish Unitary Council</t>
+  </si>
+  <si>
+    <t>E47000004</t>
+  </si>
+  <si>
+    <t>E47000002</t>
+  </si>
+  <si>
+    <t>E47000005</t>
   </si>
 </sst>
 </file>
@@ -13939,9 +13967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P376" sqref="P376"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13949,7 +13977,7 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="19" customWidth="1"/>
@@ -15687,6 +15715,9 @@
       <c r="E26" t="s">
         <v>196</v>
       </c>
+      <c r="F26" t="s">
+        <v>4120</v>
+      </c>
       <c r="G26" t="s">
         <v>253</v>
       </c>
@@ -15758,6 +15789,9 @@
       <c r="E27" t="s">
         <v>196</v>
       </c>
+      <c r="F27" t="s">
+        <v>4118</v>
+      </c>
       <c r="G27" t="s">
         <v>262</v>
       </c>
@@ -16222,6 +16256,9 @@
       <c r="E34" t="s">
         <v>196</v>
       </c>
+      <c r="F34" t="s">
+        <v>4335</v>
+      </c>
       <c r="G34" t="s">
         <v>318</v>
       </c>
@@ -16890,6 +16927,9 @@
       <c r="E44" t="s">
         <v>196</v>
       </c>
+      <c r="F44" t="s">
+        <v>4118</v>
+      </c>
       <c r="G44" t="s">
         <v>404</v>
       </c>
@@ -18155,6 +18195,9 @@
       <c r="E63" t="s">
         <v>196</v>
       </c>
+      <c r="F63" t="s">
+        <v>4335</v>
+      </c>
       <c r="G63" t="s">
         <v>565</v>
       </c>
@@ -19059,6 +19102,9 @@
       <c r="E77" t="s">
         <v>135</v>
       </c>
+      <c r="F77" t="s">
+        <v>4115</v>
+      </c>
       <c r="G77" t="s">
         <v>674</v>
       </c>
@@ -19526,6 +19572,9 @@
       <c r="E84" t="s">
         <v>196</v>
       </c>
+      <c r="F84" t="s">
+        <v>4120</v>
+      </c>
       <c r="G84" t="s">
         <v>733</v>
       </c>
@@ -19842,6 +19891,9 @@
       <c r="E89" t="s">
         <v>135</v>
       </c>
+      <c r="F89" t="s">
+        <v>4332</v>
+      </c>
       <c r="G89" t="s">
         <v>766</v>
       </c>
@@ -21662,6 +21714,9 @@
       <c r="E117" t="s">
         <v>196</v>
       </c>
+      <c r="F117" t="s">
+        <v>4332</v>
+      </c>
       <c r="G117" t="s">
         <v>991</v>
       </c>
@@ -22530,6 +22585,9 @@
       <c r="E131" t="s">
         <v>135</v>
       </c>
+      <c r="F131" t="s">
+        <v>4121</v>
+      </c>
       <c r="G131" t="s">
         <v>1097</v>
       </c>
@@ -23591,6 +23649,9 @@
       <c r="E147" t="s">
         <v>135</v>
       </c>
+      <c r="F147" t="s">
+        <v>4115</v>
+      </c>
       <c r="G147" t="s">
         <v>1230</v>
       </c>
@@ -24608,6 +24669,9 @@
       <c r="E162" t="s">
         <v>196</v>
       </c>
+      <c r="F162" t="s">
+        <v>4335</v>
+      </c>
       <c r="G162" t="s">
         <v>1360</v>
       </c>
@@ -24744,6 +24808,9 @@
       <c r="E164" t="s">
         <v>196</v>
       </c>
+      <c r="F164" t="s">
+        <v>4121</v>
+      </c>
       <c r="G164" t="s">
         <v>1377</v>
       </c>
@@ -25084,6 +25151,9 @@
       <c r="L169" s="1">
         <v>41730</v>
       </c>
+      <c r="O169" t="s">
+        <v>4355</v>
+      </c>
       <c r="V169" t="s">
         <v>4121</v>
       </c>
@@ -25110,6 +25180,9 @@
       <c r="E170" t="s">
         <v>196</v>
       </c>
+      <c r="F170" t="s">
+        <v>4335</v>
+      </c>
       <c r="G170" t="s">
         <v>1420</v>
       </c>
@@ -25562,6 +25635,9 @@
       <c r="E177" t="s">
         <v>196</v>
       </c>
+      <c r="F177" t="s">
+        <v>4121</v>
+      </c>
       <c r="G177" t="s">
         <v>1476</v>
       </c>
@@ -25905,6 +25981,9 @@
       <c r="E182" t="s">
         <v>196</v>
       </c>
+      <c r="F182" t="s">
+        <v>4118</v>
+      </c>
       <c r="G182" t="s">
         <v>1521</v>
       </c>
@@ -26106,6 +26185,9 @@
       <c r="E185" t="s">
         <v>135</v>
       </c>
+      <c r="F185" t="s">
+        <v>4115</v>
+      </c>
       <c r="G185" t="s">
         <v>1546</v>
       </c>
@@ -26789,6 +26871,9 @@
       <c r="E195" t="s">
         <v>135</v>
       </c>
+      <c r="F195" t="s">
+        <v>4337</v>
+      </c>
       <c r="G195" t="s">
         <v>1634</v>
       </c>
@@ -27262,6 +27347,9 @@
       <c r="E202" t="s">
         <v>196</v>
       </c>
+      <c r="F202" t="s">
+        <v>4337</v>
+      </c>
       <c r="G202" t="s">
         <v>1695</v>
       </c>
@@ -28146,6 +28234,9 @@
       <c r="E215" t="s">
         <v>196</v>
       </c>
+      <c r="F215" t="s">
+        <v>4337</v>
+      </c>
       <c r="G215" t="s">
         <v>1804</v>
       </c>
@@ -28607,6 +28698,9 @@
       <c r="E222" t="s">
         <v>196</v>
       </c>
+      <c r="F222" t="s">
+        <v>4118</v>
+      </c>
       <c r="G222" t="s">
         <v>1862</v>
       </c>
@@ -29284,6 +29378,9 @@
       <c r="E232" t="s">
         <v>135</v>
       </c>
+      <c r="F232" t="s">
+        <v>4115</v>
+      </c>
       <c r="G232" t="s">
         <v>1950</v>
       </c>
@@ -29358,6 +29455,9 @@
       <c r="E233" t="s">
         <v>196</v>
       </c>
+      <c r="F233" t="s">
+        <v>4118</v>
+      </c>
       <c r="G233" t="s">
         <v>1960</v>
       </c>
@@ -30091,6 +30191,9 @@
       <c r="E244" t="s">
         <v>196</v>
       </c>
+      <c r="F244" t="s">
+        <v>4120</v>
+      </c>
       <c r="G244" t="s">
         <v>2052</v>
       </c>
@@ -30898,6 +31001,9 @@
       <c r="L256" s="1">
         <v>41730</v>
       </c>
+      <c r="O256" t="s">
+        <v>4356</v>
+      </c>
       <c r="V256" t="s">
         <v>4120</v>
       </c>
@@ -31308,6 +31414,9 @@
       <c r="E263" t="s">
         <v>196</v>
       </c>
+      <c r="F263" t="s">
+        <v>4121</v>
+      </c>
       <c r="G263" t="s">
         <v>2200</v>
       </c>
@@ -31589,6 +31698,9 @@
       <c r="E267" t="s">
         <v>196</v>
       </c>
+      <c r="F267" t="s">
+        <v>4120</v>
+      </c>
       <c r="G267" t="s">
         <v>2235</v>
       </c>
@@ -31660,6 +31772,9 @@
       <c r="E268" t="s">
         <v>196</v>
       </c>
+      <c r="F268" t="s">
+        <v>4121</v>
+      </c>
       <c r="G268" t="s">
         <v>2244</v>
       </c>
@@ -31938,6 +32053,9 @@
       <c r="E272" t="s">
         <v>196</v>
       </c>
+      <c r="F272" t="s">
+        <v>4118</v>
+      </c>
       <c r="G272" t="s">
         <v>2280</v>
       </c>
@@ -32074,6 +32192,9 @@
       <c r="E274" t="s">
         <v>196</v>
       </c>
+      <c r="F274" t="s">
+        <v>4118</v>
+      </c>
       <c r="G274" t="s">
         <v>2297</v>
       </c>
@@ -32219,6 +32340,9 @@
       <c r="E276" t="s">
         <v>196</v>
       </c>
+      <c r="F276" t="s">
+        <v>4332</v>
+      </c>
       <c r="G276" t="s">
         <v>2316</v>
       </c>
@@ -33549,6 +33673,9 @@
       <c r="E296" t="s">
         <v>135</v>
       </c>
+      <c r="F296" t="s">
+        <v>4115</v>
+      </c>
       <c r="G296" t="s">
         <v>2482</v>
       </c>
@@ -33694,6 +33821,9 @@
       <c r="E298" t="s">
         <v>196</v>
       </c>
+      <c r="F298" t="s">
+        <v>4332</v>
+      </c>
       <c r="G298" t="s">
         <v>2502</v>
       </c>
@@ -34146,6 +34276,9 @@
       <c r="E305" t="s">
         <v>196</v>
       </c>
+      <c r="F305" t="s">
+        <v>4118</v>
+      </c>
       <c r="G305" t="s">
         <v>2553</v>
       </c>
@@ -35157,6 +35290,9 @@
       <c r="E320" t="s">
         <v>196</v>
       </c>
+      <c r="F320" t="s">
+        <v>4118</v>
+      </c>
       <c r="G320" t="s">
         <v>2682</v>
       </c>
@@ -36403,6 +36539,9 @@
       <c r="E340" t="s">
         <v>196</v>
       </c>
+      <c r="F340" t="s">
+        <v>4118</v>
+      </c>
       <c r="G340" t="s">
         <v>2830</v>
       </c>
@@ -36613,6 +36752,9 @@
       <c r="E343" t="s">
         <v>196</v>
       </c>
+      <c r="F343" t="s">
+        <v>4335</v>
+      </c>
       <c r="G343" t="s">
         <v>2857</v>
       </c>
@@ -37013,7 +37155,7 @@
         <v>2904</v>
       </c>
       <c r="V349" t="s">
-        <v>2898</v>
+        <v>4332</v>
       </c>
       <c r="W349" t="s">
         <v>2899</v>
@@ -37087,7 +37229,7 @@
         <v>2914</v>
       </c>
       <c r="V350" t="s">
-        <v>2906</v>
+        <v>4335</v>
       </c>
       <c r="W350" t="s">
         <v>2907</v>
@@ -37152,7 +37294,7 @@
         <v>2922</v>
       </c>
       <c r="V351" t="s">
-        <v>2916</v>
+        <v>4337</v>
       </c>
       <c r="W351" t="s">
         <v>2917</v>
@@ -37526,6 +37668,9 @@
       <c r="E357" t="s">
         <v>196</v>
       </c>
+      <c r="F357" t="s">
+        <v>4121</v>
+      </c>
       <c r="G357" t="s">
         <v>2967</v>
       </c>
@@ -38298,6 +38443,12 @@
       <c r="C370" t="s">
         <v>4316</v>
       </c>
+      <c r="D370" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E370" t="s">
+        <v>4353</v>
+      </c>
       <c r="G370" t="s">
         <v>3051</v>
       </c>
@@ -38339,6 +38490,12 @@
       <c r="C371" t="s">
         <v>4316</v>
       </c>
+      <c r="D371" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E371" t="s">
+        <v>4353</v>
+      </c>
       <c r="G371" t="s">
         <v>3058</v>
       </c>
@@ -38380,6 +38537,12 @@
       <c r="C372" t="s">
         <v>4316</v>
       </c>
+      <c r="D372" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E372" t="s">
+        <v>4353</v>
+      </c>
       <c r="G372" t="s">
         <v>3065</v>
       </c>
@@ -38421,6 +38584,12 @@
       <c r="C373" t="s">
         <v>4316</v>
       </c>
+      <c r="D373" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E373" t="s">
+        <v>4353</v>
+      </c>
       <c r="G373" t="s">
         <v>3072</v>
       </c>
@@ -38465,6 +38634,12 @@
       <c r="C374" t="s">
         <v>4316</v>
       </c>
+      <c r="D374" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E374" t="s">
+        <v>4353</v>
+      </c>
       <c r="G374" t="s">
         <v>3080</v>
       </c>
@@ -38506,6 +38681,12 @@
       <c r="C375" t="s">
         <v>4316</v>
       </c>
+      <c r="D375" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E375" t="s">
+        <v>4353</v>
+      </c>
       <c r="G375" t="s">
         <v>3087</v>
       </c>
@@ -38547,6 +38728,12 @@
       <c r="C376" t="s">
         <v>4316</v>
       </c>
+      <c r="D376" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E376" t="s">
+        <v>4353</v>
+      </c>
       <c r="G376" t="s">
         <v>3094</v>
       </c>
@@ -38588,6 +38775,12 @@
       <c r="C377" t="s">
         <v>4316</v>
       </c>
+      <c r="D377" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E377" t="s">
+        <v>4353</v>
+      </c>
       <c r="G377" t="s">
         <v>3101</v>
       </c>
@@ -38629,6 +38822,12 @@
       <c r="C378" t="s">
         <v>4316</v>
       </c>
+      <c r="D378" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E378" t="s">
+        <v>4353</v>
+      </c>
       <c r="G378" t="s">
         <v>3108</v>
       </c>
@@ -38670,6 +38869,12 @@
       <c r="C379" t="s">
         <v>4316</v>
       </c>
+      <c r="D379" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E379" t="s">
+        <v>4353</v>
+      </c>
       <c r="G379" t="s">
         <v>3115</v>
       </c>
@@ -38711,6 +38916,15 @@
       <c r="B380" t="s">
         <v>3121</v>
       </c>
+      <c r="C380" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D380" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E380" t="s">
+        <v>4353</v>
+      </c>
       <c r="G380" t="s">
         <v>3123</v>
       </c>
@@ -38738,6 +38952,15 @@
       <c r="B381" t="s">
         <v>3126</v>
       </c>
+      <c r="C381" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D381" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E381" t="s">
+        <v>4353</v>
+      </c>
       <c r="G381" t="s">
         <v>3128</v>
       </c>
@@ -38765,6 +38988,15 @@
       <c r="B382" t="s">
         <v>3131</v>
       </c>
+      <c r="C382" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D382" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E382" t="s">
+        <v>4353</v>
+      </c>
       <c r="G382" t="s">
         <v>3133</v>
       </c>
@@ -38792,6 +39024,15 @@
       <c r="B383" t="s">
         <v>3136</v>
       </c>
+      <c r="C383" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D383" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E383" t="s">
+        <v>4353</v>
+      </c>
       <c r="G383" t="s">
         <v>3138</v>
       </c>
@@ -38819,6 +39060,15 @@
       <c r="B384" t="s">
         <v>3141</v>
       </c>
+      <c r="C384" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D384" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E384" t="s">
+        <v>4353</v>
+      </c>
       <c r="G384" t="s">
         <v>3143</v>
       </c>
@@ -38846,6 +39096,15 @@
       <c r="B385" t="s">
         <v>3146</v>
       </c>
+      <c r="C385" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D385" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E385" t="s">
+        <v>4353</v>
+      </c>
       <c r="G385" t="s">
         <v>3148</v>
       </c>
@@ -38873,6 +39132,15 @@
       <c r="B386" t="s">
         <v>3151</v>
       </c>
+      <c r="C386" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D386" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E386" t="s">
+        <v>4353</v>
+      </c>
       <c r="G386" t="s">
         <v>3153</v>
       </c>
@@ -38900,6 +39168,15 @@
       <c r="B387" t="s">
         <v>3156</v>
       </c>
+      <c r="C387" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D387" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E387" t="s">
+        <v>4353</v>
+      </c>
       <c r="G387" t="s">
         <v>3158</v>
       </c>
@@ -38927,6 +39204,15 @@
       <c r="B388" t="s">
         <v>3161</v>
       </c>
+      <c r="C388" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D388" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E388" t="s">
+        <v>4353</v>
+      </c>
       <c r="G388" t="s">
         <v>3163</v>
       </c>
@@ -38954,6 +39240,15 @@
       <c r="B389" t="s">
         <v>3166</v>
       </c>
+      <c r="C389" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D389" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E389" t="s">
+        <v>4353</v>
+      </c>
       <c r="G389" t="s">
         <v>3168</v>
       </c>
@@ -38981,6 +39276,15 @@
       <c r="B390" t="s">
         <v>3171</v>
       </c>
+      <c r="C390" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D390" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E390" t="s">
+        <v>4353</v>
+      </c>
       <c r="G390" t="s">
         <v>3173</v>
       </c>
@@ -39008,6 +39312,15 @@
       <c r="B391" t="s">
         <v>3176</v>
       </c>
+      <c r="C391" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D391" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E391" t="s">
+        <v>4353</v>
+      </c>
       <c r="G391" t="s">
         <v>3178</v>
       </c>
@@ -39035,6 +39348,15 @@
       <c r="B392" t="s">
         <v>3181</v>
       </c>
+      <c r="C392" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D392" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E392" t="s">
+        <v>4353</v>
+      </c>
       <c r="G392" t="s">
         <v>3183</v>
       </c>
@@ -39062,6 +39384,15 @@
       <c r="B393" t="s">
         <v>3186</v>
       </c>
+      <c r="C393" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D393" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E393" t="s">
+        <v>4353</v>
+      </c>
       <c r="G393" t="s">
         <v>3188</v>
       </c>
@@ -39089,6 +39420,15 @@
       <c r="B394" t="s">
         <v>3191</v>
       </c>
+      <c r="C394" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D394" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E394" t="s">
+        <v>4353</v>
+      </c>
       <c r="G394" t="s">
         <v>3193</v>
       </c>
@@ -39116,6 +39456,15 @@
       <c r="B395" t="s">
         <v>3196</v>
       </c>
+      <c r="C395" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D395" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E395" t="s">
+        <v>4353</v>
+      </c>
       <c r="G395" t="s">
         <v>3198</v>
       </c>
@@ -39143,6 +39492,15 @@
       <c r="B396" t="s">
         <v>3201</v>
       </c>
+      <c r="C396" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D396" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E396" t="s">
+        <v>4353</v>
+      </c>
       <c r="G396" t="s">
         <v>3203</v>
       </c>
@@ -39170,6 +39528,15 @@
       <c r="B397" t="s">
         <v>3206</v>
       </c>
+      <c r="C397" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D397" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E397" t="s">
+        <v>4353</v>
+      </c>
       <c r="G397" t="s">
         <v>3208</v>
       </c>
@@ -39197,6 +39564,15 @@
       <c r="B398" t="s">
         <v>3211</v>
       </c>
+      <c r="C398" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D398" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E398" t="s">
+        <v>4353</v>
+      </c>
       <c r="G398" t="s">
         <v>3213</v>
       </c>
@@ -39224,6 +39600,15 @@
       <c r="B399" t="s">
         <v>3216</v>
       </c>
+      <c r="C399" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D399" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E399" t="s">
+        <v>4353</v>
+      </c>
       <c r="G399" t="s">
         <v>3218</v>
       </c>
@@ -39251,6 +39636,15 @@
       <c r="B400" t="s">
         <v>3221</v>
       </c>
+      <c r="C400" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D400" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E400" t="s">
+        <v>4353</v>
+      </c>
       <c r="G400" t="s">
         <v>3223</v>
       </c>
@@ -39278,6 +39672,15 @@
       <c r="B401" t="s">
         <v>3226</v>
       </c>
+      <c r="C401" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D401" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E401" t="s">
+        <v>4353</v>
+      </c>
       <c r="G401" t="s">
         <v>3228</v>
       </c>
@@ -39305,6 +39708,15 @@
       <c r="B402" t="s">
         <v>3231</v>
       </c>
+      <c r="C402" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D402" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E402" t="s">
+        <v>4353</v>
+      </c>
       <c r="G402" t="s">
         <v>3233</v>
       </c>
@@ -39332,6 +39744,15 @@
       <c r="B403" t="s">
         <v>3236</v>
       </c>
+      <c r="C403" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D403" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E403" t="s">
+        <v>4353</v>
+      </c>
       <c r="G403" t="s">
         <v>3238</v>
       </c>
@@ -39359,6 +39780,15 @@
       <c r="B404" t="s">
         <v>3241</v>
       </c>
+      <c r="C404" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D404" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E404" t="s">
+        <v>4353</v>
+      </c>
       <c r="G404" t="s">
         <v>3243</v>
       </c>
@@ -39389,6 +39819,12 @@
       <c r="C405" t="s">
         <v>4316</v>
       </c>
+      <c r="D405" t="s">
+        <v>4351</v>
+      </c>
+      <c r="E405" t="s">
+        <v>4353</v>
+      </c>
       <c r="G405" t="s">
         <v>3247</v>
       </c>
@@ -39430,6 +39866,12 @@
       <c r="C406" t="s">
         <v>4317</v>
       </c>
+      <c r="D406" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E406" t="s">
+        <v>4354</v>
+      </c>
       <c r="G406" t="s">
         <v>3254</v>
       </c>
@@ -39486,6 +39928,12 @@
       <c r="C407" t="s">
         <v>4317</v>
       </c>
+      <c r="D407" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E407" t="s">
+        <v>4354</v>
+      </c>
       <c r="G407" t="s">
         <v>3262</v>
       </c>
@@ -39542,6 +39990,12 @@
       <c r="C408" t="s">
         <v>4317</v>
       </c>
+      <c r="D408" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E408" t="s">
+        <v>4354</v>
+      </c>
       <c r="G408" t="s">
         <v>3270</v>
       </c>
@@ -39598,6 +40052,12 @@
       <c r="C409" t="s">
         <v>4317</v>
       </c>
+      <c r="D409" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E409" t="s">
+        <v>4354</v>
+      </c>
       <c r="G409" t="s">
         <v>3278</v>
       </c>
@@ -39654,6 +40114,12 @@
       <c r="C410" t="s">
         <v>4317</v>
       </c>
+      <c r="D410" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E410" t="s">
+        <v>4354</v>
+      </c>
       <c r="G410" t="s">
         <v>3286</v>
       </c>
@@ -39710,6 +40176,12 @@
       <c r="C411" t="s">
         <v>4317</v>
       </c>
+      <c r="D411" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E411" t="s">
+        <v>4354</v>
+      </c>
       <c r="G411" t="s">
         <v>3294</v>
       </c>
@@ -39769,6 +40241,12 @@
       <c r="C412" t="s">
         <v>4317</v>
       </c>
+      <c r="D412" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E412" t="s">
+        <v>4354</v>
+      </c>
       <c r="G412" t="s">
         <v>3303</v>
       </c>
@@ -39825,6 +40303,12 @@
       <c r="C413" t="s">
         <v>4317</v>
       </c>
+      <c r="D413" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E413" t="s">
+        <v>4354</v>
+      </c>
       <c r="G413" t="s">
         <v>3311</v>
       </c>
@@ -39881,6 +40365,12 @@
       <c r="C414" t="s">
         <v>4317</v>
       </c>
+      <c r="D414" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E414" t="s">
+        <v>4354</v>
+      </c>
       <c r="G414" t="s">
         <v>3319</v>
       </c>
@@ -39937,6 +40427,12 @@
       <c r="C415" t="s">
         <v>4317</v>
       </c>
+      <c r="D415" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E415" t="s">
+        <v>4354</v>
+      </c>
       <c r="G415" t="s">
         <v>3327</v>
       </c>
@@ -39996,6 +40492,12 @@
       <c r="C416" t="s">
         <v>4317</v>
       </c>
+      <c r="D416" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E416" t="s">
+        <v>4354</v>
+      </c>
       <c r="G416" t="s">
         <v>3336</v>
       </c>
@@ -40052,6 +40554,12 @@
       <c r="C417" t="s">
         <v>4317</v>
       </c>
+      <c r="D417" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E417" t="s">
+        <v>4354</v>
+      </c>
       <c r="G417" t="s">
         <v>3344</v>
       </c>
@@ -40114,6 +40622,12 @@
       <c r="C418" t="s">
         <v>4317</v>
       </c>
+      <c r="D418" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E418" t="s">
+        <v>4354</v>
+      </c>
       <c r="G418" t="s">
         <v>3354</v>
       </c>
@@ -40170,6 +40684,12 @@
       <c r="C419" t="s">
         <v>4317</v>
       </c>
+      <c r="D419" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E419" t="s">
+        <v>4354</v>
+      </c>
       <c r="G419" t="s">
         <v>3362</v>
       </c>
@@ -40226,6 +40746,12 @@
       <c r="C420" t="s">
         <v>4317</v>
       </c>
+      <c r="D420" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E420" t="s">
+        <v>4354</v>
+      </c>
       <c r="G420" t="s">
         <v>3370</v>
       </c>
@@ -40285,6 +40811,12 @@
       <c r="C421" t="s">
         <v>4317</v>
       </c>
+      <c r="D421" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E421" t="s">
+        <v>4354</v>
+      </c>
       <c r="G421" t="s">
         <v>3378</v>
       </c>
@@ -40344,6 +40876,12 @@
       <c r="C422" t="s">
         <v>4317</v>
       </c>
+      <c r="D422" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E422" t="s">
+        <v>4354</v>
+      </c>
       <c r="G422" t="s">
         <v>3385</v>
       </c>
@@ -40403,6 +40941,12 @@
       <c r="C423" t="s">
         <v>4317</v>
       </c>
+      <c r="D423" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E423" t="s">
+        <v>4354</v>
+      </c>
       <c r="G423" t="s">
         <v>3394</v>
       </c>
@@ -40459,6 +41003,12 @@
       <c r="C424" t="s">
         <v>4317</v>
       </c>
+      <c r="D424" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E424" t="s">
+        <v>4354</v>
+      </c>
       <c r="G424" t="s">
         <v>3402</v>
       </c>
@@ -40515,6 +41065,12 @@
       <c r="C425" t="s">
         <v>4317</v>
       </c>
+      <c r="D425" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E425" t="s">
+        <v>4354</v>
+      </c>
       <c r="G425" t="s">
         <v>3410</v>
       </c>
@@ -40574,6 +41130,12 @@
       <c r="C426" t="s">
         <v>4317</v>
       </c>
+      <c r="D426" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E426" t="s">
+        <v>4354</v>
+      </c>
       <c r="G426" t="s">
         <v>3419</v>
       </c>
@@ -40630,6 +41192,12 @@
       <c r="C427" t="s">
         <v>4317</v>
       </c>
+      <c r="D427" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E427" t="s">
+        <v>4354</v>
+      </c>
       <c r="G427" t="s">
         <v>3427</v>
       </c>
@@ -40689,6 +41257,12 @@
       <c r="C428" t="s">
         <v>4317</v>
       </c>
+      <c r="D428" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E428" t="s">
+        <v>4354</v>
+      </c>
       <c r="G428" t="s">
         <v>3435</v>
       </c>
@@ -40745,6 +41319,12 @@
       <c r="C429" t="s">
         <v>4317</v>
       </c>
+      <c r="D429" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E429" t="s">
+        <v>4354</v>
+      </c>
       <c r="G429" t="s">
         <v>3443</v>
       </c>
@@ -40804,6 +41384,12 @@
       <c r="C430" t="s">
         <v>4317</v>
       </c>
+      <c r="D430" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E430" t="s">
+        <v>4354</v>
+      </c>
       <c r="G430" t="s">
         <v>3451</v>
       </c>
@@ -40860,6 +41446,12 @@
       <c r="C431" t="s">
         <v>4317</v>
       </c>
+      <c r="D431" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E431" t="s">
+        <v>4354</v>
+      </c>
       <c r="G431" t="s">
         <v>3459</v>
       </c>
@@ -40916,6 +41508,12 @@
       <c r="C432" t="s">
         <v>4317</v>
       </c>
+      <c r="D432" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E432" t="s">
+        <v>4354</v>
+      </c>
       <c r="G432" t="s">
         <v>3467</v>
       </c>
@@ -40972,6 +41570,12 @@
       <c r="C433" t="s">
         <v>4317</v>
       </c>
+      <c r="D433" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E433" t="s">
+        <v>4354</v>
+      </c>
       <c r="G433" t="s">
         <v>3475</v>
       </c>
@@ -41028,6 +41632,12 @@
       <c r="C434" t="s">
         <v>4317</v>
       </c>
+      <c r="D434" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E434" t="s">
+        <v>4354</v>
+      </c>
       <c r="G434" t="s">
         <v>3483</v>
       </c>
@@ -41084,6 +41694,12 @@
       <c r="C435" t="s">
         <v>4317</v>
       </c>
+      <c r="D435" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E435" t="s">
+        <v>4354</v>
+      </c>
       <c r="G435" t="s">
         <v>3491</v>
       </c>
@@ -41140,6 +41756,12 @@
       <c r="C436" t="s">
         <v>4317</v>
       </c>
+      <c r="D436" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E436" t="s">
+        <v>4354</v>
+      </c>
       <c r="G436" t="s">
         <v>3499</v>
       </c>
@@ -41196,6 +41818,12 @@
       <c r="C437" t="s">
         <v>4317</v>
       </c>
+      <c r="D437" t="s">
+        <v>4349</v>
+      </c>
+      <c r="E437" t="s">
+        <v>4354</v>
+      </c>
       <c r="G437" t="s">
         <v>3507</v>
       </c>
@@ -41252,6 +41880,12 @@
       <c r="C438" t="s">
         <v>4318</v>
       </c>
+      <c r="D438" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E438" t="s">
+        <v>4352</v>
+      </c>
       <c r="G438" t="s">
         <v>3516</v>
       </c>
@@ -41314,6 +41948,12 @@
       <c r="C439" t="s">
         <v>4318</v>
       </c>
+      <c r="D439" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E439" t="s">
+        <v>4352</v>
+      </c>
       <c r="G439" t="s">
         <v>3526</v>
       </c>
@@ -41376,6 +42016,12 @@
       <c r="C440" t="s">
         <v>4318</v>
       </c>
+      <c r="D440" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E440" t="s">
+        <v>4352</v>
+      </c>
       <c r="G440" t="s">
         <v>3536</v>
       </c>
@@ -41438,6 +42084,12 @@
       <c r="C441" t="s">
         <v>4318</v>
       </c>
+      <c r="D441" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E441" t="s">
+        <v>4352</v>
+      </c>
       <c r="G441" t="s">
         <v>3545</v>
       </c>
@@ -41500,6 +42152,12 @@
       <c r="C442" t="s">
         <v>4318</v>
       </c>
+      <c r="D442" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E442" t="s">
+        <v>4352</v>
+      </c>
       <c r="G442" t="s">
         <v>3555</v>
       </c>
@@ -41562,6 +42220,12 @@
       <c r="C443" t="s">
         <v>4318</v>
       </c>
+      <c r="D443" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E443" t="s">
+        <v>4352</v>
+      </c>
       <c r="G443" t="s">
         <v>3564</v>
       </c>
@@ -41624,6 +42288,12 @@
       <c r="C444" t="s">
         <v>4318</v>
       </c>
+      <c r="D444" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E444" t="s">
+        <v>4352</v>
+      </c>
       <c r="G444" t="s">
         <v>3574</v>
       </c>
@@ -41689,6 +42359,12 @@
       <c r="C445" t="s">
         <v>4318</v>
       </c>
+      <c r="D445" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E445" t="s">
+        <v>4352</v>
+      </c>
       <c r="G445" t="s">
         <v>3585</v>
       </c>
@@ -41751,6 +42427,12 @@
       <c r="C446" t="s">
         <v>4318</v>
       </c>
+      <c r="D446" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E446" t="s">
+        <v>4352</v>
+      </c>
       <c r="G446" t="s">
         <v>3594</v>
       </c>
@@ -41813,6 +42495,12 @@
       <c r="C447" t="s">
         <v>4318</v>
       </c>
+      <c r="D447" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E447" t="s">
+        <v>4352</v>
+      </c>
       <c r="G447" t="s">
         <v>3604</v>
       </c>
@@ -41875,6 +42563,12 @@
       <c r="C448" t="s">
         <v>4318</v>
       </c>
+      <c r="D448" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E448" t="s">
+        <v>4352</v>
+      </c>
       <c r="G448" t="s">
         <v>3614</v>
       </c>
@@ -41937,6 +42631,12 @@
       <c r="C449" t="s">
         <v>4318</v>
       </c>
+      <c r="D449" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E449" t="s">
+        <v>4352</v>
+      </c>
       <c r="G449" t="s">
         <v>3623</v>
       </c>
@@ -41999,6 +42699,12 @@
       <c r="C450" t="s">
         <v>4318</v>
       </c>
+      <c r="D450" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E450" t="s">
+        <v>4352</v>
+      </c>
       <c r="G450" t="s">
         <v>3633</v>
       </c>
@@ -42061,6 +42767,12 @@
       <c r="C451" t="s">
         <v>4318</v>
       </c>
+      <c r="D451" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E451" t="s">
+        <v>4352</v>
+      </c>
       <c r="G451" t="s">
         <v>3643</v>
       </c>
@@ -42123,6 +42835,12 @@
       <c r="C452" t="s">
         <v>4318</v>
       </c>
+      <c r="D452" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E452" t="s">
+        <v>4352</v>
+      </c>
       <c r="G452" t="s">
         <v>3653</v>
       </c>
@@ -42185,6 +42903,12 @@
       <c r="C453" t="s">
         <v>4318</v>
       </c>
+      <c r="D453" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E453" t="s">
+        <v>4352</v>
+      </c>
       <c r="G453" t="s">
         <v>3663</v>
       </c>
@@ -42247,6 +42971,12 @@
       <c r="C454" t="s">
         <v>4318</v>
       </c>
+      <c r="D454" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E454" t="s">
+        <v>4352</v>
+      </c>
       <c r="G454" t="s">
         <v>3673</v>
       </c>
@@ -42309,6 +43039,12 @@
       <c r="C455" t="s">
         <v>4318</v>
       </c>
+      <c r="D455" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E455" t="s">
+        <v>4352</v>
+      </c>
       <c r="G455" t="s">
         <v>3682</v>
       </c>
@@ -42368,6 +43104,12 @@
       <c r="C456" t="s">
         <v>4318</v>
       </c>
+      <c r="D456" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E456" t="s">
+        <v>4352</v>
+      </c>
       <c r="G456" t="s">
         <v>3691</v>
       </c>
@@ -42433,6 +43175,12 @@
       <c r="C457" t="s">
         <v>4318</v>
       </c>
+      <c r="D457" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E457" t="s">
+        <v>4352</v>
+      </c>
       <c r="G457" t="s">
         <v>3702</v>
       </c>
@@ -42495,6 +43243,12 @@
       <c r="C458" t="s">
         <v>4318</v>
       </c>
+      <c r="D458" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E458" t="s">
+        <v>4352</v>
+      </c>
       <c r="G458" t="s">
         <v>3712</v>
       </c>
@@ -42557,6 +43311,12 @@
       <c r="C459" t="s">
         <v>4318</v>
       </c>
+      <c r="D459" t="s">
+        <v>4350</v>
+      </c>
+      <c r="E459" t="s">
+        <v>4352</v>
+      </c>
       <c r="G459" t="s">
         <v>3722</v>
       </c>
@@ -42673,6 +43433,12 @@
       <c r="O461" t="s">
         <v>4343</v>
       </c>
+      <c r="P461" t="s">
+        <v>4357</v>
+      </c>
+      <c r="V461" t="s">
+        <v>4332</v>
+      </c>
     </row>
     <row r="462" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
@@ -42696,6 +43462,9 @@
       <c r="O462" t="s">
         <v>4344</v>
       </c>
+      <c r="V462" t="s">
+        <v>4335</v>
+      </c>
     </row>
     <row r="463" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
@@ -42721,6 +43490,9 @@
       </c>
       <c r="O463" t="s">
         <v>4345</v>
+      </c>
+      <c r="V463" t="s">
+        <v>4337</v>
       </c>
     </row>
   </sheetData>
@@ -42728,4 +43500,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFF461D-2AE5-44E4-B500-5FA29EC6B45C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added loose regions, made build order output
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33546F8B-B054-4850-BA4A-BEAAAD2D7E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F609D3CF-50A4-4E9D-8FF1-3AA26CB3A6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7517" uniqueCount="4356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7521" uniqueCount="4356">
   <si>
     <t>local-authority-code</t>
   </si>
@@ -13959,11 +13959,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14076,7 +14077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4321</v>
       </c>
@@ -14135,7 +14136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4321</v>
       </c>
@@ -14194,7 +14195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4321</v>
       </c>
@@ -14253,7 +14254,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4321</v>
       </c>
@@ -14312,7 +14313,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4321</v>
       </c>
@@ -14371,7 +14372,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4321</v>
       </c>
@@ -14430,7 +14431,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4321</v>
       </c>
@@ -14495,7 +14496,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4321</v>
       </c>
@@ -14554,7 +14555,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4321</v>
       </c>
@@ -14613,7 +14614,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4321</v>
       </c>
@@ -14672,7 +14673,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4321</v>
       </c>
@@ -14734,7 +14735,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4321</v>
       </c>
@@ -14997,7 +14998,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4321</v>
       </c>
@@ -15059,7 +15060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4321</v>
       </c>
@@ -15118,7 +15119,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4321</v>
       </c>
@@ -15247,67 +15248,31 @@
         <v>4321</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>4334</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>4111</v>
       </c>
       <c r="E21" t="s">
-        <v>207</v>
+        <v>4354</v>
       </c>
       <c r="G21" t="s">
-        <v>208</v>
-      </c>
-      <c r="K21" t="s">
-        <v>210</v>
+        <v>4333</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4343</v>
       </c>
       <c r="L21" s="1">
-        <v>38522</v>
-      </c>
-      <c r="M21" s="1">
-        <v>43921</v>
-      </c>
-      <c r="N21" t="s">
-        <v>4126</v>
+        <v>43406</v>
       </c>
       <c r="O21" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>4134</v>
-      </c>
-      <c r="R21">
-        <v>825</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21" t="s">
-        <v>212</v>
-      </c>
-      <c r="U21">
-        <v>11</v>
+        <v>4342</v>
       </c>
       <c r="V21" t="s">
-        <v>80</v>
-      </c>
-      <c r="W21" t="s">
-        <v>205</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>3736</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>206</v>
-      </c>
-      <c r="AB21">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+        <v>4334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4321</v>
       </c>
@@ -15371,70 +15336,34 @@
         <v>4321</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>4114</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>4111</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>4354</v>
       </c>
       <c r="G23" t="s">
-        <v>225</v>
-      </c>
-      <c r="H23" t="s">
-        <v>226</v>
-      </c>
-      <c r="I23" t="s">
-        <v>227</v>
-      </c>
-      <c r="K23" t="s">
-        <v>228</v>
+        <v>4106</v>
       </c>
       <c r="L23" s="1">
-        <v>38522</v>
-      </c>
-      <c r="M23" s="1">
-        <v>43555</v>
-      </c>
-      <c r="N23" t="s">
-        <v>4073</v>
+        <v>42538</v>
       </c>
       <c r="O23" t="s">
-        <v>229</v>
-      </c>
-      <c r="R23">
-        <v>837</v>
-      </c>
-      <c r="S23">
-        <v>330</v>
-      </c>
-      <c r="T23" t="s">
-        <v>230</v>
-      </c>
-      <c r="U23" t="s">
-        <v>231</v>
+        <v>4339</v>
       </c>
       <c r="V23" t="s">
-        <v>223</v>
+        <v>4114</v>
       </c>
       <c r="W23" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y23" s="2" t="s">
-        <v>3762</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>232</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>144</v>
+        <v>4121</v>
       </c>
       <c r="AB23">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+        <v>64997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4321</v>
       </c>
@@ -15697,7 +15626,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4321</v>
       </c>
@@ -15756,7 +15685,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4321</v>
       </c>
@@ -15930,7 +15859,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4321</v>
       </c>
@@ -16125,7 +16054,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4321</v>
       </c>
@@ -16184,7 +16113,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4321</v>
       </c>
@@ -16243,7 +16172,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4321</v>
       </c>
@@ -16302,7 +16231,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4321</v>
       </c>
@@ -16361,7 +16290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4321</v>
       </c>
@@ -16420,7 +16349,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4321</v>
       </c>
@@ -16479,7 +16408,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4321</v>
       </c>
@@ -16609,7 +16538,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4321</v>
       </c>
@@ -16736,7 +16665,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4321</v>
       </c>
@@ -16795,7 +16724,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4321</v>
       </c>
@@ -16857,7 +16786,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4321</v>
       </c>
@@ -16916,7 +16845,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4321</v>
       </c>
@@ -16975,7 +16904,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4321</v>
       </c>
@@ -17034,7 +16963,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4321</v>
       </c>
@@ -17161,7 +17090,7 @@
         <v>4311</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4321</v>
       </c>
@@ -17220,7 +17149,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4321</v>
       </c>
@@ -17412,7 +17341,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4321</v>
       </c>
@@ -17471,7 +17400,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>4321</v>
       </c>
@@ -17536,7 +17465,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4321</v>
       </c>
@@ -17595,7 +17524,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>4321</v>
       </c>
@@ -17654,7 +17583,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4321</v>
       </c>
@@ -17713,7 +17642,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4321</v>
       </c>
@@ -17908,7 +17837,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4321</v>
       </c>
@@ -17970,7 +17899,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4321</v>
       </c>
@@ -18029,7 +17958,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>4321</v>
       </c>
@@ -18156,7 +18085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>4321</v>
       </c>
@@ -18215,7 +18144,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4321</v>
       </c>
@@ -18280,7 +18209,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>4321</v>
       </c>
@@ -18409,7 +18338,7 @@
         <v>4321</v>
       </c>
       <c r="B72" t="s">
-        <v>4113</v>
+        <v>4329</v>
       </c>
       <c r="D72" t="s">
         <v>4111</v>
@@ -18418,25 +18347,22 @@
         <v>4354</v>
       </c>
       <c r="G72" t="s">
-        <v>4105</v>
+        <v>4330</v>
       </c>
       <c r="L72" s="1">
-        <v>41730</v>
+        <v>41744</v>
       </c>
       <c r="O72" t="s">
-        <v>4335</v>
+        <v>4340</v>
+      </c>
+      <c r="P72" t="s">
+        <v>4351</v>
       </c>
       <c r="V72" t="s">
-        <v>4113</v>
-      </c>
-      <c r="W72" t="s">
-        <v>4120</v>
-      </c>
-      <c r="AB72">
-        <v>64630</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4321</v>
       </c>
@@ -18557,7 +18483,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>4321</v>
       </c>
@@ -18616,7 +18542,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>4321</v>
       </c>
@@ -18746,7 +18672,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>4321</v>
       </c>
@@ -18805,7 +18731,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4321</v>
       </c>
@@ -18870,7 +18796,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4321</v>
       </c>
@@ -18932,7 +18858,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>4321</v>
       </c>
@@ -18988,7 +18914,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4321</v>
       </c>
@@ -19056,7 +18982,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>4321</v>
       </c>
@@ -19123,67 +19049,34 @@
         <v>4321</v>
       </c>
       <c r="B84" t="s">
-        <v>731</v>
+        <v>4113</v>
       </c>
       <c r="D84" t="s">
-        <v>195</v>
+        <v>4111</v>
       </c>
       <c r="E84" t="s">
-        <v>196</v>
-      </c>
-      <c r="F84" t="s">
-        <v>4117</v>
+        <v>4354</v>
       </c>
       <c r="G84" t="s">
-        <v>733</v>
-      </c>
-      <c r="H84" t="s">
-        <v>734</v>
-      </c>
-      <c r="K84" t="s">
-        <v>735</v>
+        <v>4105</v>
       </c>
       <c r="L84" s="1">
-        <v>27120</v>
+        <v>41730</v>
       </c>
       <c r="O84" t="s">
-        <v>736</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>4156</v>
-      </c>
-      <c r="R84">
-        <v>371</v>
-      </c>
-      <c r="S84">
-        <v>260</v>
-      </c>
-      <c r="T84" t="s">
-        <v>737</v>
-      </c>
-      <c r="U84" t="s">
-        <v>738</v>
+        <v>4335</v>
       </c>
       <c r="V84" t="s">
-        <v>731</v>
+        <v>4113</v>
       </c>
       <c r="W84" t="s">
-        <v>732</v>
-      </c>
-      <c r="Y84" s="2" t="s">
-        <v>3929</v>
-      </c>
-      <c r="Z84" t="s">
-        <v>739</v>
-      </c>
-      <c r="AA84" t="s">
-        <v>204</v>
+        <v>4120</v>
       </c>
       <c r="AB84">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+        <v>64630</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4321</v>
       </c>
@@ -19245,7 +19138,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4321</v>
       </c>
@@ -19487,7 +19380,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4321</v>
       </c>
@@ -19546,7 +19439,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>4321</v>
       </c>
@@ -19605,7 +19498,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4321</v>
       </c>
@@ -19664,7 +19557,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>4321</v>
       </c>
@@ -19723,7 +19616,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>4321</v>
       </c>
@@ -19782,7 +19675,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>4321</v>
       </c>
@@ -19841,7 +19734,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>4321</v>
       </c>
@@ -19903,7 +19796,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>4321</v>
       </c>
@@ -19962,7 +19855,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>4321</v>
       </c>
@@ -20024,7 +19917,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>4321</v>
       </c>
@@ -20083,7 +19976,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>4321</v>
       </c>
@@ -20142,7 +20035,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>4321</v>
       </c>
@@ -20201,7 +20094,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4321</v>
       </c>
@@ -20266,7 +20159,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>4321</v>
       </c>
@@ -20325,7 +20218,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>4321</v>
       </c>
@@ -20387,7 +20280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>4321</v>
       </c>
@@ -20558,7 +20451,7 @@
         <v>91370</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>4321</v>
       </c>
@@ -20620,7 +20513,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>4321</v>
       </c>
@@ -20679,7 +20572,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>4321</v>
       </c>
@@ -20741,7 +20634,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>4321</v>
       </c>
@@ -20797,7 +20690,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>4321</v>
       </c>
@@ -20856,7 +20749,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>4321</v>
       </c>
@@ -20915,7 +20808,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>4321</v>
       </c>
@@ -20974,7 +20867,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>4321</v>
       </c>
@@ -21036,7 +20929,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>4321</v>
       </c>
@@ -21095,7 +20988,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>4321</v>
       </c>
@@ -21163,7 +21056,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>4321</v>
       </c>
@@ -21222,60 +21115,39 @@
         <v>196</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>4321</v>
       </c>
       <c r="B119" t="s">
-        <v>169</v>
+        <v>4115</v>
       </c>
       <c r="D119" t="s">
-        <v>1007</v>
+        <v>4111</v>
       </c>
       <c r="E119" t="s">
-        <v>1008</v>
+        <v>4354</v>
       </c>
       <c r="G119" t="s">
-        <v>1009</v>
-      </c>
-      <c r="H119" t="s">
-        <v>1010</v>
+        <v>4107</v>
       </c>
       <c r="L119" s="1">
-        <v>38525</v>
+        <v>41730</v>
       </c>
       <c r="O119" t="s">
-        <v>1011</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>4164</v>
-      </c>
-      <c r="R119" t="s">
-        <v>1012</v>
-      </c>
-      <c r="T119" t="s">
-        <v>1013</v>
+        <v>4336</v>
       </c>
       <c r="V119" t="s">
-        <v>169</v>
+        <v>4115</v>
       </c>
       <c r="W119" t="s">
-        <v>1006</v>
-      </c>
-      <c r="Y119" s="2" t="s">
-        <v>3959</v>
-      </c>
-      <c r="Z119" t="s">
-        <v>1014</v>
+        <v>4122</v>
       </c>
       <c r="AB119">
-        <v>606</v>
-      </c>
-      <c r="AC119" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+        <v>8211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>4321</v>
       </c>
@@ -21334,7 +21206,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>4321</v>
       </c>
@@ -21396,12 +21268,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4321</v>
       </c>
       <c r="B122" t="s">
-        <v>4115</v>
+        <v>4118</v>
       </c>
       <c r="D122" t="s">
         <v>4111</v>
@@ -21410,25 +21282,25 @@
         <v>4354</v>
       </c>
       <c r="G122" t="s">
-        <v>4107</v>
+        <v>4110</v>
       </c>
       <c r="L122" s="1">
         <v>41730</v>
       </c>
       <c r="O122" t="s">
-        <v>4336</v>
+        <v>4349</v>
       </c>
       <c r="V122" t="s">
-        <v>4115</v>
+        <v>4118</v>
       </c>
       <c r="W122" t="s">
-        <v>4122</v>
+        <v>4125</v>
       </c>
       <c r="AB122">
-        <v>8211</v>
-      </c>
-    </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+        <v>52349</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>4321</v>
       </c>
@@ -21487,7 +21359,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>4321</v>
       </c>
@@ -21546,7 +21418,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>4321</v>
       </c>
@@ -21605,7 +21477,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>4321</v>
       </c>
@@ -21664,7 +21536,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>4321</v>
       </c>
@@ -21723,7 +21595,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>4321</v>
       </c>
@@ -21782,7 +21654,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>4321</v>
       </c>
@@ -21841,7 +21713,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>4321</v>
       </c>
@@ -21971,7 +21843,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>4321</v>
       </c>
@@ -22033,7 +21905,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>4321</v>
       </c>
@@ -22089,7 +21961,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>4321</v>
       </c>
@@ -22148,7 +22020,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>4321</v>
       </c>
@@ -22207,7 +22079,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>4321</v>
       </c>
@@ -22266,7 +22138,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>4321</v>
       </c>
@@ -22325,7 +22197,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>4321</v>
       </c>
@@ -22452,7 +22324,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>4321</v>
       </c>
@@ -22511,7 +22383,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>4321</v>
       </c>
@@ -22570,7 +22442,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>4321</v>
       </c>
@@ -22629,7 +22501,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>4321</v>
       </c>
@@ -22691,7 +22563,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>4321</v>
       </c>
@@ -22753,7 +22625,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>4321</v>
       </c>
@@ -22945,7 +22817,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>4321</v>
       </c>
@@ -23007,7 +22879,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>4321</v>
       </c>
@@ -23066,7 +22938,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>4321</v>
       </c>
@@ -23125,7 +22997,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>4321</v>
       </c>
@@ -23184,7 +23056,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>4321</v>
       </c>
@@ -23376,7 +23248,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>4321</v>
       </c>
@@ -23435,7 +23307,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>4321</v>
       </c>
@@ -23494,7 +23366,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>4321</v>
       </c>
@@ -23556,7 +23428,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>4321</v>
       </c>
@@ -23618,7 +23490,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>4321</v>
       </c>
@@ -23751,7 +23623,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>4321</v>
       </c>
@@ -23884,7 +23756,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>4321</v>
       </c>
@@ -24011,7 +23883,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>4321</v>
       </c>
@@ -24070,7 +23942,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>4321</v>
       </c>
@@ -24132,7 +24004,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>4321</v>
       </c>
@@ -24264,7 +24136,7 @@
         <v>4321</v>
       </c>
       <c r="B169" t="s">
-        <v>4118</v>
+        <v>4117</v>
       </c>
       <c r="D169" t="s">
         <v>4111</v>
@@ -24273,22 +24145,22 @@
         <v>4354</v>
       </c>
       <c r="G169" t="s">
-        <v>4110</v>
+        <v>4109</v>
       </c>
       <c r="L169" s="1">
         <v>41730</v>
       </c>
       <c r="O169" t="s">
-        <v>4349</v>
+        <v>4350</v>
       </c>
       <c r="V169" t="s">
-        <v>4118</v>
+        <v>4117</v>
       </c>
       <c r="W169" t="s">
-        <v>4125</v>
+        <v>4124</v>
       </c>
       <c r="AB169">
-        <v>52349</v>
+        <v>52350</v>
       </c>
     </row>
     <row r="170" spans="1:28" x14ac:dyDescent="0.25">
@@ -24359,7 +24231,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>4321</v>
       </c>
@@ -24421,7 +24293,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>4321</v>
       </c>
@@ -24477,7 +24349,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>4321</v>
       </c>
@@ -24536,7 +24408,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>4321</v>
       </c>
@@ -24598,7 +24470,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>4321</v>
       </c>
@@ -24657,7 +24529,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>4321</v>
       </c>
@@ -24724,64 +24596,31 @@
         <v>4321</v>
       </c>
       <c r="B177" t="s">
-        <v>1474</v>
+        <v>4112</v>
       </c>
       <c r="D177" t="s">
-        <v>195</v>
+        <v>4111</v>
       </c>
       <c r="E177" t="s">
-        <v>196</v>
-      </c>
-      <c r="F177" t="s">
-        <v>4118</v>
+        <v>4354</v>
       </c>
       <c r="G177" t="s">
-        <v>1476</v>
-      </c>
-      <c r="H177" t="s">
-        <v>1477</v>
-      </c>
-      <c r="K177" t="s">
-        <v>1478</v>
+        <v>4104</v>
       </c>
       <c r="L177" s="1">
-        <v>38511</v>
+        <v>41730</v>
       </c>
       <c r="O177" t="s">
-        <v>1479</v>
-      </c>
-      <c r="Q177" t="s">
-        <v>4182</v>
-      </c>
-      <c r="R177">
-        <v>341</v>
-      </c>
-      <c r="S177">
-        <v>274</v>
-      </c>
-      <c r="T177" t="s">
-        <v>1480</v>
-      </c>
-      <c r="U177" t="s">
-        <v>1481</v>
+        <v>4337</v>
       </c>
       <c r="V177" t="s">
-        <v>1474</v>
+        <v>4112</v>
       </c>
       <c r="W177" t="s">
-        <v>1475</v>
-      </c>
-      <c r="Y177" s="2" t="s">
-        <v>4034</v>
-      </c>
-      <c r="Z177" t="s">
-        <v>1482</v>
-      </c>
-      <c r="AA177" t="s">
-        <v>204</v>
+        <v>4119</v>
       </c>
       <c r="AB177">
-        <v>3</v>
+        <v>87984</v>
       </c>
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.25">
@@ -24914,7 +24753,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>4321</v>
       </c>
@@ -24973,7 +24812,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>4321</v>
       </c>
@@ -25100,7 +24939,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>4321</v>
       </c>
@@ -25159,7 +24998,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>4321</v>
       </c>
@@ -25289,7 +25128,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>4321</v>
       </c>
@@ -25419,7 +25258,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>4321</v>
       </c>
@@ -25478,7 +25317,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>4321</v>
       </c>
@@ -25605,7 +25444,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>4321</v>
       </c>
@@ -25664,7 +25503,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>4321</v>
       </c>
@@ -25785,7 +25624,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>4321</v>
       </c>
@@ -25915,7 +25754,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>4321</v>
       </c>
@@ -25974,7 +25813,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>4321</v>
       </c>
@@ -26036,7 +25875,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>4321</v>
       </c>
@@ -26098,7 +25937,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>4321</v>
       </c>
@@ -26157,7 +25996,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>4321</v>
       </c>
@@ -26352,7 +26191,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>4321</v>
       </c>
@@ -26411,7 +26250,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>4321</v>
       </c>
@@ -26544,7 +26383,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>4321</v>
       </c>
@@ -26603,7 +26442,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>4321</v>
       </c>
@@ -26730,7 +26569,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="209" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>4321</v>
       </c>
@@ -26789,7 +26628,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="210" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>4321</v>
       </c>
@@ -26854,7 +26693,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="211" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>4321</v>
       </c>
@@ -26981,7 +26820,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="213" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>4321</v>
       </c>
@@ -27049,7 +26888,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="214" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>4321</v>
       </c>
@@ -27179,7 +27018,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="216" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>4321</v>
       </c>
@@ -27241,7 +27080,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="217" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>4321</v>
       </c>
@@ -27300,7 +27139,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="218" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>4321</v>
       </c>
@@ -27359,7 +27198,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="219" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>4321</v>
       </c>
@@ -27418,7 +27257,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="220" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>4321</v>
       </c>
@@ -27480,7 +27319,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="221" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>4321</v>
       </c>
@@ -27607,7 +27446,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="223" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>4321</v>
       </c>
@@ -27669,7 +27508,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="224" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>4321</v>
       </c>
@@ -27725,7 +27564,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="225" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>4321</v>
       </c>
@@ -27857,67 +27696,31 @@
         <v>4321</v>
       </c>
       <c r="B227" t="s">
-        <v>1902</v>
+        <v>4116</v>
       </c>
       <c r="D227" t="s">
-        <v>134</v>
+        <v>4111</v>
       </c>
       <c r="E227" t="s">
-        <v>135</v>
+        <v>4354</v>
       </c>
       <c r="G227" t="s">
-        <v>1904</v>
-      </c>
-      <c r="H227" t="s">
-        <v>1905</v>
-      </c>
-      <c r="I227" t="s">
-        <v>1906</v>
-      </c>
-      <c r="K227" t="s">
-        <v>1907</v>
+        <v>4108</v>
       </c>
       <c r="L227" s="1">
-        <v>35521</v>
-      </c>
-      <c r="M227" s="1">
-        <v>43555</v>
-      </c>
-      <c r="N227" t="s">
-        <v>4073</v>
+        <v>41730</v>
       </c>
       <c r="O227" t="s">
-        <v>1908</v>
-      </c>
-      <c r="R227">
-        <v>836</v>
-      </c>
-      <c r="S227">
-        <v>351</v>
-      </c>
-      <c r="T227" t="s">
-        <v>1909</v>
-      </c>
-      <c r="U227" t="s">
-        <v>1910</v>
+        <v>4338</v>
       </c>
       <c r="V227" t="s">
-        <v>1902</v>
+        <v>4116</v>
       </c>
       <c r="W227" t="s">
-        <v>1903</v>
-      </c>
-      <c r="Y227" s="2" t="s">
-        <v>3901</v>
-      </c>
-      <c r="Z227" t="s">
-        <v>1911</v>
-      </c>
-      <c r="AA227" t="s">
-        <v>144</v>
+        <v>4123</v>
       </c>
       <c r="AB227">
-        <v>305</v>
+        <v>88002</v>
       </c>
     </row>
     <row r="228" spans="1:28" x14ac:dyDescent="0.25">
@@ -27988,7 +27791,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="229" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>4321</v>
       </c>
@@ -28115,7 +27918,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="231" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>4321</v>
       </c>
@@ -28316,7 +28119,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="234" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>4321</v>
       </c>
@@ -28443,7 +28246,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="236" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>4321</v>
       </c>
@@ -28502,7 +28305,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="237" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>4321</v>
       </c>
@@ -28564,7 +28367,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="238" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>4321</v>
       </c>
@@ -28623,7 +28426,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="239" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>4321</v>
       </c>
@@ -28682,7 +28485,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="240" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>4321</v>
       </c>
@@ -28741,7 +28544,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="241" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>4321</v>
       </c>
@@ -28800,7 +28603,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="242" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>4321</v>
       </c>
@@ -28859,7 +28662,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="243" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>4321</v>
       </c>
@@ -28986,7 +28789,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="245" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>4321</v>
       </c>
@@ -29045,7 +28848,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="246" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>4321</v>
       </c>
@@ -29104,7 +28907,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="247" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>4321</v>
       </c>
@@ -29163,7 +28966,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="248" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>4321</v>
       </c>
@@ -29290,7 +29093,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="250" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>4321</v>
       </c>
@@ -29349,7 +29152,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="251" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>4321</v>
       </c>
@@ -29476,7 +29279,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="253" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>4321</v>
       </c>
@@ -29541,7 +29344,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="254" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>4321</v>
       </c>
@@ -29600,7 +29403,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="255" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>4321</v>
       </c>
@@ -29664,7 +29467,7 @@
         <v>4321</v>
       </c>
       <c r="B256" t="s">
-        <v>4117</v>
+        <v>4332</v>
       </c>
       <c r="D256" t="s">
         <v>4111</v>
@@ -29673,25 +29476,19 @@
         <v>4354</v>
       </c>
       <c r="G256" t="s">
-        <v>4109</v>
+        <v>4331</v>
       </c>
       <c r="L256" s="1">
         <v>41730</v>
       </c>
       <c r="O256" t="s">
-        <v>4350</v>
+        <v>4341</v>
       </c>
       <c r="V256" t="s">
-        <v>4117</v>
-      </c>
-      <c r="W256" t="s">
-        <v>4124</v>
-      </c>
-      <c r="AB256">
-        <v>52350</v>
-      </c>
-    </row>
-    <row r="257" spans="1:28" x14ac:dyDescent="0.25">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="257" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>4321</v>
       </c>
@@ -29750,7 +29547,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="258" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>4321</v>
       </c>
@@ -29812,7 +29609,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="259" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>4321</v>
       </c>
@@ -29871,7 +29668,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="260" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>4321</v>
       </c>
@@ -29930,7 +29727,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="261" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>4321</v>
       </c>
@@ -29989,7 +29786,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="262" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>4321</v>
       </c>
@@ -30187,7 +29984,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="265" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>4321</v>
       </c>
@@ -30246,7 +30043,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="266" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>4321</v>
       </c>
@@ -30450,7 +30247,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="269" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>4321</v>
       </c>
@@ -30577,7 +30374,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="271" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>4321</v>
       </c>
@@ -30704,7 +30501,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="273" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>4321</v>
       </c>
@@ -30763,7 +30560,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="274" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>4321</v>
       </c>
@@ -30831,7 +30628,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="275" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>4321</v>
       </c>
@@ -30899,7 +30696,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="276" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>4321</v>
       </c>
@@ -30967,7 +30764,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="277" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>4321</v>
       </c>
@@ -31026,7 +30823,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="278" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>4321</v>
       </c>
@@ -31091,7 +30888,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="279" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>4321</v>
       </c>
@@ -31156,7 +30953,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="280" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>4321</v>
       </c>
@@ -31218,75 +31015,60 @@
         <v>344</v>
       </c>
     </row>
-    <row r="281" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>4321</v>
       </c>
       <c r="B281" t="s">
-        <v>2355</v>
+        <v>169</v>
       </c>
       <c r="D281" t="s">
-        <v>134</v>
+        <v>1007</v>
       </c>
       <c r="E281" t="s">
-        <v>135</v>
+        <v>1008</v>
       </c>
       <c r="G281" t="s">
-        <v>2357</v>
+        <v>1009</v>
       </c>
       <c r="H281" t="s">
-        <v>2358</v>
-      </c>
-      <c r="I281" t="s">
-        <v>2359</v>
-      </c>
-      <c r="J281" t="s">
-        <v>2360</v>
-      </c>
-      <c r="K281" t="s">
-        <v>2361</v>
+        <v>1010</v>
       </c>
       <c r="L281" s="1">
-        <v>38523</v>
+        <v>38525</v>
       </c>
       <c r="O281" t="s">
-        <v>2362</v>
+        <v>1011</v>
       </c>
       <c r="Q281" t="s">
-        <v>4222</v>
-      </c>
-      <c r="R281">
-        <v>882</v>
-      </c>
-      <c r="S281">
-        <v>378</v>
+        <v>4164</v>
+      </c>
+      <c r="R281" t="s">
+        <v>1012</v>
       </c>
       <c r="T281" t="s">
-        <v>2363</v>
-      </c>
-      <c r="U281" t="s">
-        <v>2364</v>
+        <v>1013</v>
       </c>
       <c r="V281" t="s">
-        <v>2355</v>
+        <v>169</v>
       </c>
       <c r="W281" t="s">
-        <v>2356</v>
+        <v>1006</v>
       </c>
       <c r="Y281" s="2" t="s">
-        <v>3882</v>
+        <v>3959</v>
       </c>
       <c r="Z281" t="s">
-        <v>2365</v>
-      </c>
-      <c r="AA281" t="s">
-        <v>144</v>
+        <v>1014</v>
       </c>
       <c r="AB281">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="282" spans="1:28" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+      <c r="AC281" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="282" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>4321</v>
       </c>
@@ -31345,7 +31127,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="283" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>4321</v>
       </c>
@@ -31404,7 +31186,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="284" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>4321</v>
       </c>
@@ -31463,7 +31245,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="285" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>4321</v>
       </c>
@@ -31525,7 +31307,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="286" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>4321</v>
       </c>
@@ -31581,7 +31363,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="287" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>4321</v>
       </c>
@@ -31640,7 +31422,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="288" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>4321</v>
       </c>
@@ -31767,7 +31549,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="290" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>4321</v>
       </c>
@@ -31894,7 +31676,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="292" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>4321</v>
       </c>
@@ -31953,7 +31735,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="293" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>4321</v>
       </c>
@@ -32012,7 +31794,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="294" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>4321</v>
       </c>
@@ -32071,7 +31853,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>4321</v>
       </c>
@@ -32138,7 +31920,10 @@
         <v>4321</v>
       </c>
       <c r="B296" t="s">
-        <v>2480</v>
+        <v>2355</v>
+      </c>
+      <c r="C296" t="s">
+        <v>4307</v>
       </c>
       <c r="D296" t="s">
         <v>134</v>
@@ -32146,65 +31931,62 @@
       <c r="E296" t="s">
         <v>135</v>
       </c>
-      <c r="F296" t="s">
-        <v>4112</v>
-      </c>
       <c r="G296" t="s">
-        <v>2482</v>
+        <v>2357</v>
       </c>
       <c r="H296" t="s">
-        <v>2483</v>
+        <v>2358</v>
       </c>
       <c r="I296" t="s">
-        <v>2484</v>
+        <v>2359</v>
       </c>
       <c r="J296" t="s">
-        <v>2485</v>
+        <v>2360</v>
       </c>
       <c r="K296" t="s">
-        <v>2486</v>
+        <v>2361</v>
       </c>
       <c r="L296" s="1">
-        <v>38521</v>
+        <v>38523</v>
       </c>
       <c r="O296" t="s">
-        <v>2487</v>
+        <v>2362</v>
       </c>
       <c r="Q296" t="s">
-        <v>4227</v>
+        <v>4222</v>
       </c>
       <c r="R296">
-        <v>808</v>
+        <v>882</v>
       </c>
       <c r="S296">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="T296" t="s">
-        <v>2488</v>
+        <v>2363</v>
       </c>
       <c r="U296" t="s">
-        <v>2489</v>
+        <v>2364</v>
       </c>
       <c r="V296" t="s">
-        <v>2480</v>
+        <v>2355</v>
       </c>
       <c r="W296" t="s">
-        <v>2481</v>
+        <v>2356</v>
       </c>
       <c r="Y296" s="2" t="s">
-        <v>3860</v>
+        <v>3882</v>
       </c>
       <c r="Z296" t="s">
-        <v>2490</v>
+        <v>2365</v>
       </c>
       <c r="AA296" t="s">
         <v>144</v>
       </c>
       <c r="AB296">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="297" spans="1:28" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="297" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>4321</v>
       </c>
@@ -32334,7 +32116,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>4321</v>
       </c>
@@ -32396,7 +32178,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="300" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>4321</v>
       </c>
@@ -32523,7 +32305,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="302" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>4321</v>
       </c>
@@ -32582,7 +32364,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="303" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>4321</v>
       </c>
@@ -32756,7 +32538,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="306" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>4321</v>
       </c>
@@ -32815,7 +32597,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="307" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>4321</v>
       </c>
@@ -32877,7 +32659,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="308" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>4321</v>
       </c>
@@ -32936,7 +32718,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="309" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>4321</v>
       </c>
@@ -32995,7 +32777,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="310" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>4321</v>
       </c>
@@ -33054,7 +32836,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="311" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>4321</v>
       </c>
@@ -33113,7 +32895,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="312" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>4321</v>
       </c>
@@ -33243,7 +33025,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="314" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>4321</v>
       </c>
@@ -33302,7 +33084,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="315" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>4321</v>
       </c>
@@ -33497,7 +33279,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="318" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>4321</v>
       </c>
@@ -33559,7 +33341,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="319" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>4321</v>
       </c>
@@ -33686,7 +33468,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>4321</v>
       </c>
@@ -33745,39 +33527,72 @@
         <v>407</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>4321</v>
       </c>
       <c r="B322" t="s">
-        <v>4112</v>
+        <v>80</v>
       </c>
       <c r="D322" t="s">
-        <v>4111</v>
+        <v>206</v>
       </c>
       <c r="E322" t="s">
-        <v>4354</v>
+        <v>207</v>
       </c>
       <c r="G322" t="s">
-        <v>4104</v>
+        <v>208</v>
+      </c>
+      <c r="K322" t="s">
+        <v>210</v>
       </c>
       <c r="L322" s="1">
-        <v>41730</v>
+        <v>38522</v>
+      </c>
+      <c r="M322" s="1">
+        <v>43921</v>
+      </c>
+      <c r="N322" t="s">
+        <v>4126</v>
       </c>
       <c r="O322" t="s">
-        <v>4337</v>
+        <v>211</v>
+      </c>
+      <c r="Q322" t="s">
+        <v>4134</v>
+      </c>
+      <c r="R322">
+        <v>825</v>
+      </c>
+      <c r="S322">
+        <v>1</v>
+      </c>
+      <c r="T322" t="s">
+        <v>212</v>
+      </c>
+      <c r="U322">
+        <v>11</v>
       </c>
       <c r="V322" t="s">
-        <v>4112</v>
+        <v>80</v>
       </c>
       <c r="W322" t="s">
-        <v>4119</v>
+        <v>205</v>
+      </c>
+      <c r="Y322" s="2" t="s">
+        <v>3736</v>
+      </c>
+      <c r="Z322" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA322" t="s">
+        <v>206</v>
       </c>
       <c r="AB322">
-        <v>87984</v>
-      </c>
-    </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="323" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>4321</v>
       </c>
@@ -33836,7 +33651,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>4321</v>
       </c>
@@ -33895,7 +33710,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>4321</v>
       </c>
@@ -33954,7 +33769,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>4321</v>
       </c>
@@ -34013,7 +33828,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>4321</v>
       </c>
@@ -34075,7 +33890,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>4321</v>
       </c>
@@ -34131,7 +33946,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>4321</v>
       </c>
@@ -34193,7 +34008,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>4321</v>
       </c>
@@ -34320,7 +34135,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>4321</v>
       </c>
@@ -34379,7 +34194,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>4321</v>
       </c>
@@ -34441,7 +34256,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>4321</v>
       </c>
@@ -34500,39 +34315,75 @@
         <v>421</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>4321</v>
       </c>
       <c r="B335" t="s">
-        <v>4116</v>
+        <v>223</v>
       </c>
       <c r="D335" t="s">
-        <v>4111</v>
+        <v>134</v>
       </c>
       <c r="E335" t="s">
-        <v>4354</v>
+        <v>135</v>
       </c>
       <c r="G335" t="s">
-        <v>4108</v>
+        <v>225</v>
+      </c>
+      <c r="H335" t="s">
+        <v>226</v>
+      </c>
+      <c r="I335" t="s">
+        <v>227</v>
+      </c>
+      <c r="K335" t="s">
+        <v>228</v>
       </c>
       <c r="L335" s="1">
-        <v>41730</v>
+        <v>38522</v>
+      </c>
+      <c r="M335" s="1">
+        <v>43555</v>
+      </c>
+      <c r="N335" t="s">
+        <v>4073</v>
       </c>
       <c r="O335" t="s">
-        <v>4338</v>
+        <v>229</v>
+      </c>
+      <c r="R335">
+        <v>837</v>
+      </c>
+      <c r="S335">
+        <v>330</v>
+      </c>
+      <c r="T335" t="s">
+        <v>230</v>
+      </c>
+      <c r="U335" t="s">
+        <v>231</v>
       </c>
       <c r="V335" t="s">
-        <v>4116</v>
+        <v>223</v>
       </c>
       <c r="W335" t="s">
-        <v>4123</v>
+        <v>224</v>
+      </c>
+      <c r="Y335" s="2" t="s">
+        <v>3762</v>
+      </c>
+      <c r="Z335" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA335" t="s">
+        <v>144</v>
       </c>
       <c r="AB335">
-        <v>88002</v>
-      </c>
-    </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="336" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>4321</v>
       </c>
@@ -34597,7 +34448,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="337" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>4321</v>
       </c>
@@ -34659,7 +34510,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>4321</v>
       </c>
@@ -34724,7 +34575,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="339" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>4321</v>
       </c>
@@ -34919,7 +34770,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="342" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>4321</v>
       </c>
@@ -35046,7 +34897,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="344" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>4321</v>
       </c>
@@ -35105,7 +34956,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="345" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>4321</v>
       </c>
@@ -35299,34 +35150,76 @@
         <v>4321</v>
       </c>
       <c r="B348" t="s">
-        <v>4114</v>
+        <v>2480</v>
+      </c>
+      <c r="C348" t="s">
+        <v>4312</v>
       </c>
       <c r="D348" t="s">
-        <v>4111</v>
+        <v>134</v>
       </c>
       <c r="E348" t="s">
-        <v>4354</v>
+        <v>135</v>
+      </c>
+      <c r="F348" t="s">
+        <v>4112</v>
       </c>
       <c r="G348" t="s">
-        <v>4106</v>
+        <v>2482</v>
+      </c>
+      <c r="H348" t="s">
+        <v>2483</v>
+      </c>
+      <c r="I348" t="s">
+        <v>2484</v>
+      </c>
+      <c r="J348" t="s">
+        <v>2485</v>
+      </c>
+      <c r="K348" t="s">
+        <v>2486</v>
       </c>
       <c r="L348" s="1">
-        <v>42538</v>
+        <v>38521</v>
       </c>
       <c r="O348" t="s">
-        <v>4339</v>
+        <v>2487</v>
+      </c>
+      <c r="Q348" t="s">
+        <v>4227</v>
+      </c>
+      <c r="R348">
+        <v>808</v>
+      </c>
+      <c r="S348">
+        <v>356</v>
+      </c>
+      <c r="T348" t="s">
+        <v>2488</v>
+      </c>
+      <c r="U348" t="s">
+        <v>2489</v>
       </c>
       <c r="V348" t="s">
-        <v>4114</v>
+        <v>2480</v>
       </c>
       <c r="W348" t="s">
-        <v>4121</v>
+        <v>2481</v>
+      </c>
+      <c r="Y348" s="2" t="s">
+        <v>3860</v>
+      </c>
+      <c r="Z348" t="s">
+        <v>2490</v>
+      </c>
+      <c r="AA348" t="s">
+        <v>144</v>
       </c>
       <c r="AB348">
-        <v>64997</v>
-      </c>
-    </row>
-    <row r="349" spans="1:28" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="349" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>4321</v>
       </c>
@@ -35453,7 +35346,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="351" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>4321</v>
       </c>
@@ -35512,7 +35405,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="352" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>4321</v>
       </c>
@@ -35639,7 +35532,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="354" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>4321</v>
       </c>
@@ -35763,7 +35656,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="356" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>4321</v>
       </c>
@@ -36002,7 +35895,7 @@
         <v>91366</v>
       </c>
     </row>
-    <row r="360" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>4321</v>
       </c>
@@ -36061,7 +35954,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="361" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>4321</v>
       </c>
@@ -36123,7 +36016,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="362" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>4321</v>
       </c>
@@ -36185,7 +36078,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="363" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>4321</v>
       </c>
@@ -36241,7 +36134,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="364" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>4321</v>
       </c>
@@ -36300,7 +36193,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="365" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>4321</v>
       </c>
@@ -36365,7 +36258,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="366" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>4321</v>
       </c>
@@ -37034,7 +36927,7 @@
         <v>54912</v>
       </c>
     </row>
-    <row r="380" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>4313</v>
       </c>
@@ -37070,7 +36963,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="381" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>4313</v>
       </c>
@@ -37106,7 +36999,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="382" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>4313</v>
       </c>
@@ -37142,7 +37035,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="383" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>4313</v>
       </c>
@@ -37178,7 +37071,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="384" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>4313</v>
       </c>
@@ -37214,7 +37107,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="385" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>4313</v>
       </c>
@@ -37250,7 +37143,7 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="386" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>4313</v>
       </c>
@@ -37286,7 +37179,7 @@
         <v>3152</v>
       </c>
     </row>
-    <row r="387" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>4313</v>
       </c>
@@ -37322,7 +37215,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="388" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>4313</v>
       </c>
@@ -37358,7 +37251,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="389" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>4313</v>
       </c>
@@ -37394,7 +37287,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="390" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>4313</v>
       </c>
@@ -37430,7 +37323,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="391" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>4313</v>
       </c>
@@ -37466,7 +37359,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="392" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>4313</v>
       </c>
@@ -37502,7 +37395,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="393" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>4313</v>
       </c>
@@ -37538,7 +37431,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="394" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>4313</v>
       </c>
@@ -37574,7 +37467,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="395" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>4313</v>
       </c>
@@ -37610,7 +37503,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="396" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>4313</v>
       </c>
@@ -37646,7 +37539,7 @@
         <v>3202</v>
       </c>
     </row>
-    <row r="397" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>4313</v>
       </c>
@@ -37682,7 +37575,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="398" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>4313</v>
       </c>
@@ -37718,7 +37611,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="399" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>4313</v>
       </c>
@@ -37754,7 +37647,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="400" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>4313</v>
       </c>
@@ -37790,7 +37683,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="401" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>4313</v>
       </c>
@@ -37826,7 +37719,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="402" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>4313</v>
       </c>
@@ -37862,7 +37755,7 @@
         <v>3232</v>
       </c>
     </row>
-    <row r="403" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>4313</v>
       </c>
@@ -37898,7 +37791,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="404" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>4313</v>
       </c>
@@ -41214,54 +41107,135 @@
         <v>4321</v>
       </c>
       <c r="B461" t="s">
-        <v>4329</v>
+        <v>1474</v>
+      </c>
+      <c r="C461" t="s">
+        <v>4305</v>
       </c>
       <c r="D461" t="s">
-        <v>4111</v>
+        <v>195</v>
       </c>
       <c r="E461" t="s">
-        <v>4354</v>
+        <v>196</v>
+      </c>
+      <c r="F461" t="s">
+        <v>4118</v>
       </c>
       <c r="G461" t="s">
-        <v>4330</v>
+        <v>1476</v>
+      </c>
+      <c r="H461" t="s">
+        <v>1477</v>
+      </c>
+      <c r="K461" t="s">
+        <v>1478</v>
       </c>
       <c r="L461" s="1">
-        <v>41744</v>
+        <v>38511</v>
       </c>
       <c r="O461" t="s">
-        <v>4340</v>
-      </c>
-      <c r="P461" t="s">
-        <v>4351</v>
+        <v>1479</v>
+      </c>
+      <c r="Q461" t="s">
+        <v>4182</v>
+      </c>
+      <c r="R461">
+        <v>341</v>
+      </c>
+      <c r="S461">
+        <v>274</v>
+      </c>
+      <c r="T461" t="s">
+        <v>1480</v>
+      </c>
+      <c r="U461" t="s">
+        <v>1481</v>
       </c>
       <c r="V461" t="s">
-        <v>4329</v>
-      </c>
-    </row>
-    <row r="462" spans="1:28" x14ac:dyDescent="0.25">
+        <v>1474</v>
+      </c>
+      <c r="W461" t="s">
+        <v>1475</v>
+      </c>
+      <c r="Y461" s="2" t="s">
+        <v>4034</v>
+      </c>
+      <c r="Z461" t="s">
+        <v>1482</v>
+      </c>
+      <c r="AA461" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB461">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="462" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>4321</v>
       </c>
       <c r="B462" t="s">
-        <v>4332</v>
+        <v>1902</v>
       </c>
       <c r="D462" t="s">
-        <v>4111</v>
+        <v>134</v>
       </c>
       <c r="E462" t="s">
-        <v>4354</v>
+        <v>135</v>
       </c>
       <c r="G462" t="s">
-        <v>4331</v>
+        <v>1904</v>
+      </c>
+      <c r="H462" t="s">
+        <v>1905</v>
+      </c>
+      <c r="I462" t="s">
+        <v>1906</v>
+      </c>
+      <c r="K462" t="s">
+        <v>1907</v>
       </c>
       <c r="L462" s="1">
-        <v>41730</v>
+        <v>35521</v>
+      </c>
+      <c r="M462" s="1">
+        <v>43555</v>
+      </c>
+      <c r="N462" t="s">
+        <v>4073</v>
       </c>
       <c r="O462" t="s">
-        <v>4341</v>
+        <v>1908</v>
+      </c>
+      <c r="R462">
+        <v>836</v>
+      </c>
+      <c r="S462">
+        <v>351</v>
+      </c>
+      <c r="T462" t="s">
+        <v>1909</v>
+      </c>
+      <c r="U462" t="s">
+        <v>1910</v>
       </c>
       <c r="V462" t="s">
-        <v>4332</v>
+        <v>1902</v>
+      </c>
+      <c r="W462" t="s">
+        <v>1903</v>
+      </c>
+      <c r="Y462" s="2" t="s">
+        <v>3901</v>
+      </c>
+      <c r="Z462" t="s">
+        <v>1911</v>
+      </c>
+      <c r="AA462" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB462">
+        <v>305</v>
       </c>
     </row>
     <row r="463" spans="1:28" x14ac:dyDescent="0.25">
@@ -41269,32 +41243,83 @@
         <v>4321</v>
       </c>
       <c r="B463" t="s">
-        <v>4334</v>
+        <v>731</v>
+      </c>
+      <c r="C463" t="s">
+        <v>4311</v>
       </c>
       <c r="D463" t="s">
-        <v>4111</v>
+        <v>195</v>
       </c>
       <c r="E463" t="s">
-        <v>4354</v>
+        <v>196</v>
+      </c>
+      <c r="F463" t="s">
+        <v>4117</v>
       </c>
       <c r="G463" t="s">
-        <v>4333</v>
+        <v>733</v>
       </c>
       <c r="H463" t="s">
-        <v>4343</v>
+        <v>734</v>
+      </c>
+      <c r="K463" t="s">
+        <v>735</v>
       </c>
       <c r="L463" s="1">
-        <v>43406</v>
+        <v>27120</v>
       </c>
       <c r="O463" t="s">
-        <v>4342</v>
+        <v>736</v>
+      </c>
+      <c r="Q463" t="s">
+        <v>4156</v>
+      </c>
+      <c r="R463">
+        <v>371</v>
+      </c>
+      <c r="S463">
+        <v>260</v>
+      </c>
+      <c r="T463" t="s">
+        <v>737</v>
+      </c>
+      <c r="U463" t="s">
+        <v>738</v>
       </c>
       <c r="V463" t="s">
-        <v>4334</v>
+        <v>731</v>
+      </c>
+      <c r="W463" t="s">
+        <v>732</v>
+      </c>
+      <c r="Y463" s="2" t="s">
+        <v>3929</v>
+      </c>
+      <c r="Z463" t="s">
+        <v>739</v>
+      </c>
+      <c r="AA463" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB463">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}"/>
+  <autoFilter ref="A1:AC463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}">
+    <filterColumn colId="11">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="12">
+      <filters blank="1"/>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:AC463">
+      <sortCondition descending="1" ref="L1:L463"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed dorset > devon error
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53310BF-5F1B-415E-85CF-225B82D5EBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA23C97-9369-462E-AC33-E32A7F188343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13959,12 +13959,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14431,7 +14430,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4321</v>
       </c>
@@ -14794,7 +14793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4321</v>
       </c>
@@ -14862,7 +14861,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4321</v>
       </c>
@@ -14930,7 +14929,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4321</v>
       </c>
@@ -15178,7 +15177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4321</v>
       </c>
@@ -15243,7 +15242,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4321</v>
       </c>
@@ -15331,7 +15330,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4321</v>
       </c>
@@ -15422,7 +15421,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4321</v>
       </c>
@@ -15490,7 +15489,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4321</v>
       </c>
@@ -15558,7 +15557,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4321</v>
       </c>
@@ -15744,7 +15743,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4321</v>
       </c>
@@ -15791,7 +15790,7 @@
         <v>91513</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4321</v>
       </c>
@@ -15918,7 +15917,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4321</v>
       </c>
@@ -15986,7 +15985,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4321</v>
       </c>
@@ -16467,7 +16466,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4321</v>
       </c>
@@ -16597,7 +16596,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4321</v>
       </c>
@@ -16724,7 +16723,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4321</v>
       </c>
@@ -17022,7 +17021,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4321</v>
       </c>
@@ -17149,7 +17148,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4321</v>
       </c>
@@ -17211,7 +17210,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4321</v>
       </c>
@@ -17400,7 +17399,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>4321</v>
       </c>
@@ -17701,7 +17700,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4321</v>
       </c>
@@ -17769,7 +17768,7 @@
         <v>4306</v>
       </c>
     </row>
-    <row r="63" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4321</v>
       </c>
@@ -17837,7 +17836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4321</v>
       </c>
@@ -18017,7 +18016,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>4321</v>
       </c>
@@ -18144,7 +18143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4321</v>
       </c>
@@ -18268,7 +18267,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>4321</v>
       </c>
@@ -18333,7 +18332,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4321</v>
       </c>
@@ -18601,7 +18600,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>4321</v>
       </c>
@@ -18731,7 +18730,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4321</v>
       </c>
@@ -18796,7 +18795,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4321</v>
       </c>
@@ -18917,7 +18916,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4321</v>
       </c>
@@ -18985,7 +18984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>4321</v>
       </c>
@@ -19047,7 +19046,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>4321</v>
       </c>
@@ -19079,7 +19078,7 @@
         <v>64630</v>
       </c>
     </row>
-    <row r="85" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4321</v>
       </c>
@@ -19200,7 +19199,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>4321</v>
       </c>
@@ -19244,7 +19243,7 @@
         <v>91365</v>
       </c>
     </row>
-    <row r="88" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>4321</v>
       </c>
@@ -19309,7 +19308,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4321</v>
       </c>
@@ -19737,7 +19736,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="96" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>4321</v>
       </c>
@@ -20097,7 +20096,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="102" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4321</v>
       </c>
@@ -20342,7 +20341,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>4321</v>
       </c>
@@ -20454,7 +20453,7 @@
         <v>91370</v>
       </c>
     </row>
-    <row r="108" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>4321</v>
       </c>
@@ -20575,7 +20574,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>4321</v>
       </c>
@@ -20873,7 +20872,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="115" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>4321</v>
       </c>
@@ -20994,7 +20993,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>4321</v>
       </c>
@@ -21121,7 +21120,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="119" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>4321</v>
       </c>
@@ -21212,7 +21211,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="121" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>4321</v>
       </c>
@@ -21274,7 +21273,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="122" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4321</v>
       </c>
@@ -21778,7 +21777,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="131" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>4321</v>
       </c>
@@ -21849,7 +21848,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="132" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>4321</v>
       </c>
@@ -22265,7 +22264,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="139" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>4321</v>
       </c>
@@ -22755,7 +22754,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="147" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>4321</v>
       </c>
@@ -22826,7 +22825,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>4321</v>
       </c>
@@ -23124,7 +23123,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="153" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>4321</v>
       </c>
@@ -23189,7 +23188,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="154" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>4321</v>
       </c>
@@ -23437,7 +23436,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="158" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>4321</v>
       </c>
@@ -23499,7 +23498,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="159" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>4321</v>
       </c>
@@ -23561,7 +23560,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="160" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>4321</v>
       </c>
@@ -23697,7 +23696,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="162" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>4321</v>
       </c>
@@ -23824,7 +23823,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="164" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>4321</v>
       </c>
@@ -23951,7 +23950,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>4321</v>
       </c>
@@ -24072,7 +24071,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="168" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>4321</v>
       </c>
@@ -24143,7 +24142,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="169" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>4321</v>
       </c>
@@ -24175,7 +24174,7 @@
         <v>52350</v>
       </c>
     </row>
-    <row r="170" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>4321</v>
       </c>
@@ -24243,7 +24242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>4321</v>
       </c>
@@ -24544,7 +24543,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="176" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>4321</v>
       </c>
@@ -24606,7 +24605,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="177" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>4321</v>
       </c>
@@ -24638,7 +24637,7 @@
         <v>87984</v>
       </c>
     </row>
-    <row r="178" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>4321</v>
       </c>
@@ -24700,7 +24699,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="179" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>4321</v>
       </c>
@@ -24886,7 +24885,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>4321</v>
       </c>
@@ -25072,7 +25071,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="185" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>4321</v>
       </c>
@@ -25202,7 +25201,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="187" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>4321</v>
       </c>
@@ -25391,7 +25390,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="190" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>4321</v>
       </c>
@@ -25698,7 +25697,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="195" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>4321</v>
       </c>
@@ -25828,7 +25827,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="197" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>4321</v>
       </c>
@@ -26070,7 +26069,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="201" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>4321</v>
       </c>
@@ -26138,7 +26137,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="202" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>4321</v>
       </c>
@@ -26265,7 +26264,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="204" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>4321</v>
       </c>
@@ -26327,7 +26326,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="205" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>4321</v>
       </c>
@@ -26516,7 +26515,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="208" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>4321</v>
       </c>
@@ -26643,7 +26642,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="210" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>4321</v>
       </c>
@@ -26767,7 +26766,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="212" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>4321</v>
       </c>
@@ -26835,7 +26834,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="213" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>4321</v>
       </c>
@@ -26903,7 +26902,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="214" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>4321</v>
       </c>
@@ -26965,7 +26964,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="215" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>4321</v>
       </c>
@@ -27272,7 +27271,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="220" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>4321</v>
       </c>
@@ -27396,7 +27395,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="222" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>4321</v>
       </c>
@@ -27464,7 +27463,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="223" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>4321</v>
       </c>
@@ -27644,7 +27643,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="226" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>4321</v>
       </c>
@@ -27712,7 +27711,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="227" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>4321</v>
       </c>
@@ -27744,7 +27743,7 @@
         <v>88002</v>
       </c>
     </row>
-    <row r="228" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>4321</v>
       </c>
@@ -27871,7 +27870,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="230" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>4321</v>
       </c>
@@ -27939,7 +27938,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="231" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>4321</v>
       </c>
@@ -28001,7 +28000,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="232" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>4321</v>
       </c>
@@ -28072,7 +28071,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="233" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>4321</v>
       </c>
@@ -28199,7 +28198,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="235" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>4321</v>
       </c>
@@ -28742,7 +28741,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="244" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>4321</v>
       </c>
@@ -29046,7 +29045,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="249" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>4321</v>
       </c>
@@ -29235,7 +29234,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="252" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>4321</v>
       </c>
@@ -29300,7 +29299,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="253" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>4321</v>
       </c>
@@ -29483,7 +29482,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="256" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>4321</v>
       </c>
@@ -29568,7 +29567,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="258" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>4321</v>
       </c>
@@ -29807,7 +29806,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="262" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>4321</v>
       </c>
@@ -29869,7 +29868,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="263" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>4321</v>
       </c>
@@ -29937,7 +29936,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="264" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>4321</v>
       </c>
@@ -30022,7 +30021,7 @@
         <v>24</v>
       </c>
       <c r="F265" t="s">
-        <v>480</v>
+        <v>271</v>
       </c>
       <c r="G265" t="s">
         <v>2219</v>
@@ -30129,7 +30128,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="267" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>4321</v>
       </c>
@@ -30197,7 +30196,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="268" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>4321</v>
       </c>
@@ -30327,7 +30326,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="270" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>4321</v>
       </c>
@@ -30454,7 +30453,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="272" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>4321</v>
       </c>
@@ -30581,7 +30580,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="274" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>4321</v>
       </c>
@@ -30649,7 +30648,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="275" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>4321</v>
       </c>
@@ -30717,7 +30716,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>4321</v>
       </c>
@@ -30844,7 +30843,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="278" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>4321</v>
       </c>
@@ -30909,7 +30908,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="279" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>4321</v>
       </c>
@@ -30974,7 +30973,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="280" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>4321</v>
       </c>
@@ -31036,7 +31035,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="281" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>4321</v>
       </c>
@@ -31266,7 +31265,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="285" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>4321</v>
       </c>
@@ -31505,7 +31504,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="289" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>4321</v>
       </c>
@@ -31632,7 +31631,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="291" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>4321</v>
       </c>
@@ -31877,7 +31876,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="295" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>4321</v>
       </c>
@@ -31939,7 +31938,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="296" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>4321</v>
       </c>
@@ -32072,7 +32071,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="298" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>4321</v>
       </c>
@@ -32140,7 +32139,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="299" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>4321</v>
       </c>
@@ -32261,7 +32260,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="301" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>4321</v>
       </c>
@@ -32494,7 +32493,7 @@
         <v>91531</v>
       </c>
     </row>
-    <row r="305" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>4321</v>
       </c>
@@ -32621,7 +32620,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="307" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>4321</v>
       </c>
@@ -32759,7 +32758,7 @@
         <v>24</v>
       </c>
       <c r="F309" t="s">
-        <v>480</v>
+        <v>271</v>
       </c>
       <c r="G309" t="s">
         <v>2586</v>
@@ -32978,7 +32977,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="313" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>4321</v>
       </c>
@@ -33167,7 +33166,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="316" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>4321</v>
       </c>
@@ -33235,7 +33234,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="317" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>4321</v>
       </c>
@@ -33424,7 +33423,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="320" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>4321</v>
       </c>
@@ -33551,7 +33550,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="322" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>4321</v>
       </c>
@@ -33852,7 +33851,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="327" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>4321</v>
       </c>
@@ -33973,7 +33972,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="329" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>4321</v>
       </c>
@@ -34094,7 +34093,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="331" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>4321</v>
       </c>
@@ -34221,7 +34220,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="333" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>4321</v>
       </c>
@@ -34342,7 +34341,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="335" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>4321</v>
       </c>
@@ -34410,7 +34409,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="336" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>4321</v>
       </c>
@@ -34537,7 +34536,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="338" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>4321</v>
       </c>
@@ -34661,7 +34660,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="340" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>4321</v>
       </c>
@@ -34729,7 +34728,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="341" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>4321</v>
       </c>
@@ -34856,7 +34855,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="343" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>4321</v>
       </c>
@@ -35042,7 +35041,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="346" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>4321</v>
       </c>
@@ -35107,7 +35106,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="347" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>4321</v>
       </c>
@@ -35172,7 +35171,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="348" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>4321</v>
       </c>
@@ -35305,7 +35304,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="350" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>4321</v>
       </c>
@@ -35491,7 +35490,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="353" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>4321</v>
       </c>
@@ -35559,7 +35558,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="354" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>4321</v>
       </c>
@@ -35742,7 +35741,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="357" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>4321</v>
       </c>
@@ -35810,7 +35809,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="358" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>4321</v>
       </c>
@@ -35981,7 +35980,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="361" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>4321</v>
       </c>
@@ -36043,7 +36042,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="362" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>4321</v>
       </c>
@@ -36223,7 +36222,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="365" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>4321</v>
       </c>
@@ -36347,7 +36346,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="367" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>4321</v>
       </c>
@@ -36415,7 +36414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="368" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>4321</v>
       </c>
@@ -36448,7 +36447,7 @@
         <v>4327</v>
       </c>
     </row>
-    <row r="369" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>4321</v>
       </c>
@@ -36481,7 +36480,7 @@
         <v>4327</v>
       </c>
     </row>
-    <row r="370" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>4313</v>
       </c>
@@ -36528,7 +36527,7 @@
         <v>54906</v>
       </c>
     </row>
-    <row r="371" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>4313</v>
       </c>
@@ -36575,7 +36574,7 @@
         <v>54914</v>
       </c>
     </row>
-    <row r="372" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>4313</v>
       </c>
@@ -36622,7 +36621,7 @@
         <v>54905</v>
       </c>
     </row>
-    <row r="373" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>4313</v>
       </c>
@@ -36672,7 +36671,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="374" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>4313</v>
       </c>
@@ -36719,7 +36718,7 @@
         <v>54907</v>
       </c>
     </row>
-    <row r="375" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>4313</v>
       </c>
@@ -36766,7 +36765,7 @@
         <v>54908</v>
       </c>
     </row>
-    <row r="376" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>4313</v>
       </c>
@@ -36813,7 +36812,7 @@
         <v>54909</v>
       </c>
     </row>
-    <row r="377" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>4313</v>
       </c>
@@ -36860,7 +36859,7 @@
         <v>54910</v>
       </c>
     </row>
-    <row r="378" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>4313</v>
       </c>
@@ -36907,7 +36906,7 @@
         <v>54911</v>
       </c>
     </row>
-    <row r="379" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>4313</v>
       </c>
@@ -36957,7 +36956,7 @@
         <v>54912</v>
       </c>
     </row>
-    <row r="380" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>4313</v>
       </c>
@@ -36993,7 +36992,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="381" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>4313</v>
       </c>
@@ -37029,7 +37028,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="382" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>4313</v>
       </c>
@@ -37065,7 +37064,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="383" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>4313</v>
       </c>
@@ -37101,7 +37100,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="384" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>4313</v>
       </c>
@@ -37137,7 +37136,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="385" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>4313</v>
       </c>
@@ -37173,7 +37172,7 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="386" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>4313</v>
       </c>
@@ -37209,7 +37208,7 @@
         <v>3152</v>
       </c>
     </row>
-    <row r="387" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>4313</v>
       </c>
@@ -37245,7 +37244,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="388" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>4313</v>
       </c>
@@ -37281,7 +37280,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="389" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>4313</v>
       </c>
@@ -37317,7 +37316,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="390" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>4313</v>
       </c>
@@ -37353,7 +37352,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="391" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>4313</v>
       </c>
@@ -37389,7 +37388,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="392" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>4313</v>
       </c>
@@ -37425,7 +37424,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="393" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>4313</v>
       </c>
@@ -37461,7 +37460,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="394" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>4313</v>
       </c>
@@ -37497,7 +37496,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="395" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>4313</v>
       </c>
@@ -37533,7 +37532,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="396" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>4313</v>
       </c>
@@ -37569,7 +37568,7 @@
         <v>3202</v>
       </c>
     </row>
-    <row r="397" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>4313</v>
       </c>
@@ -37605,7 +37604,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="398" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>4313</v>
       </c>
@@ -37641,7 +37640,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="399" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>4313</v>
       </c>
@@ -37677,7 +37676,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="400" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>4313</v>
       </c>
@@ -37713,7 +37712,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="401" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>4313</v>
       </c>
@@ -37749,7 +37748,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="402" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>4313</v>
       </c>
@@ -37785,7 +37784,7 @@
         <v>3232</v>
       </c>
     </row>
-    <row r="403" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>4313</v>
       </c>
@@ -37821,7 +37820,7 @@
         <v>3237</v>
       </c>
     </row>
-    <row r="404" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>4313</v>
       </c>
@@ -37857,7 +37856,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="405" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>4313</v>
       </c>
@@ -37904,7 +37903,7 @@
         <v>54913</v>
       </c>
     </row>
-    <row r="406" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>4314</v>
       </c>
@@ -37960,7 +37959,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="407" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>4314</v>
       </c>
@@ -38016,7 +38015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="408" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>4314</v>
       </c>
@@ -38072,7 +38071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="409" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>4314</v>
       </c>
@@ -38128,7 +38127,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="410" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>4314</v>
       </c>
@@ -38184,7 +38183,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="411" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>4314</v>
       </c>
@@ -38243,7 +38242,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="412" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>4314</v>
       </c>
@@ -38299,7 +38298,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="413" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>4314</v>
       </c>
@@ -38355,7 +38354,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="414" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>4314</v>
       </c>
@@ -38411,7 +38410,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="415" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>4314</v>
       </c>
@@ -38470,7 +38469,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="416" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>4314</v>
       </c>
@@ -38526,7 +38525,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="417" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>4314</v>
       </c>
@@ -38588,7 +38587,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="418" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>4314</v>
       </c>
@@ -38644,7 +38643,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="419" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>4314</v>
       </c>
@@ -38700,7 +38699,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="420" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>4314</v>
       </c>
@@ -38759,7 +38758,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="421" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>4314</v>
       </c>
@@ -38818,7 +38817,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="422" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>4314</v>
       </c>
@@ -38877,7 +38876,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="423" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>4314</v>
       </c>
@@ -38933,7 +38932,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="424" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>4314</v>
       </c>
@@ -38989,7 +38988,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="425" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>4314</v>
       </c>
@@ -39048,7 +39047,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="426" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>4314</v>
       </c>
@@ -39104,7 +39103,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="427" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>4314</v>
       </c>
@@ -39163,7 +39162,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="428" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>4314</v>
       </c>
@@ -39219,7 +39218,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="429" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>4314</v>
       </c>
@@ -39278,7 +39277,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="430" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>4314</v>
       </c>
@@ -39334,7 +39333,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="431" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>4314</v>
       </c>
@@ -39390,7 +39389,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="432" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>4314</v>
       </c>
@@ -39446,7 +39445,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="433" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>4314</v>
       </c>
@@ -39502,7 +39501,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="434" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>4314</v>
       </c>
@@ -39558,7 +39557,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="435" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>4314</v>
       </c>
@@ -39614,7 +39613,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="436" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>4314</v>
       </c>
@@ -39670,7 +39669,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="437" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>4314</v>
       </c>
@@ -39726,7 +39725,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="438" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>4315</v>
       </c>
@@ -39788,7 +39787,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="439" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>4315</v>
       </c>
@@ -39850,7 +39849,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="440" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>4315</v>
       </c>
@@ -39912,7 +39911,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="441" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>4315</v>
       </c>
@@ -39974,7 +39973,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="442" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>4315</v>
       </c>
@@ -40036,7 +40035,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="443" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>4315</v>
       </c>
@@ -40098,7 +40097,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="444" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>4315</v>
       </c>
@@ -40163,7 +40162,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="445" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>4315</v>
       </c>
@@ -40225,7 +40224,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="446" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>4315</v>
       </c>
@@ -40287,7 +40286,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="447" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>4315</v>
       </c>
@@ -40349,7 +40348,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="448" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>4315</v>
       </c>
@@ -40411,7 +40410,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="449" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>4315</v>
       </c>
@@ -40473,7 +40472,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="450" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>4315</v>
       </c>
@@ -40535,7 +40534,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="451" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>4315</v>
       </c>
@@ -40597,7 +40596,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="452" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>4315</v>
       </c>
@@ -40659,7 +40658,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="453" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>4315</v>
       </c>
@@ -40721,7 +40720,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="454" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>4315</v>
       </c>
@@ -40783,7 +40782,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="455" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>4315</v>
       </c>
@@ -40842,7 +40841,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="456" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>4315</v>
       </c>
@@ -40907,7 +40906,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="457" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>4315</v>
       </c>
@@ -40969,7 +40968,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="458" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>4315</v>
       </c>
@@ -41031,7 +41030,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="459" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>4315</v>
       </c>
@@ -41093,7 +41092,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="460" spans="1:28" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>4321</v>
       </c>
@@ -41132,7 +41131,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="461" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>4321</v>
       </c>
@@ -41200,7 +41199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="462" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>4321</v>
       </c>
@@ -41268,7 +41267,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="463" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>4321</v>
       </c>
@@ -41337,17 +41336,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="London borough"/>
-        <filter val="Non-metropolitan district"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="12">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added regions for combined authorities
</commit_message>
<xml_diff>
--- a/uk_local_authorities.xlsx
+++ b/uk_local_authorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexj\Dropbox\mysociety\uk_local_authority_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F8E734-450F-4424-8AC4-6CD703F340AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49494AD7-9449-4F63-8EAB-5292BE4698AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uk_local_authorities" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7549" uniqueCount="4357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7561" uniqueCount="4358">
   <si>
     <t>local-authority-code</t>
   </si>
@@ -13106,6 +13106,9 @@
   </si>
   <si>
     <t>combined-authority</t>
+  </si>
+  <si>
+    <t>East</t>
   </si>
 </sst>
 </file>
@@ -13962,18 +13965,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
@@ -14200,7 +14204,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4320</v>
       </c>
@@ -14959,12 +14963,15 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4320</v>
       </c>
       <c r="B16" t="s">
         <v>2810</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4307</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -15031,6 +15038,9 @@
       <c r="B17" t="s">
         <v>4330</v>
       </c>
+      <c r="C17" t="s">
+        <v>4310</v>
+      </c>
       <c r="D17" t="s">
         <v>4110</v>
       </c>
@@ -15156,7 +15166,7 @@
         <v>91366</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4320</v>
       </c>
@@ -15284,6 +15294,9 @@
       <c r="B22" t="s">
         <v>4115</v>
       </c>
+      <c r="C22" t="s">
+        <v>4307</v>
+      </c>
       <c r="D22" t="s">
         <v>4110</v>
       </c>
@@ -15349,6 +15362,9 @@
       <c r="B24" t="s">
         <v>4113</v>
       </c>
+      <c r="C24" t="s">
+        <v>4309</v>
+      </c>
       <c r="D24" t="s">
         <v>4110</v>
       </c>
@@ -15604,7 +15620,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4320</v>
       </c>
@@ -15855,7 +15871,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4320</v>
       </c>
@@ -16038,7 +16054,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4320</v>
       </c>
@@ -17660,6 +17676,9 @@
       <c r="B62" t="s">
         <v>4111</v>
       </c>
+      <c r="C62" t="s">
+        <v>4311</v>
+      </c>
       <c r="D62" t="s">
         <v>4110</v>
       </c>
@@ -17685,7 +17704,7 @@
         <v>87984</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4320</v>
       </c>
@@ -18311,7 +18330,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4320</v>
       </c>
@@ -18491,7 +18510,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>4312</v>
       </c>
@@ -19106,7 +19125,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4320</v>
       </c>
@@ -19732,7 +19751,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>4320</v>
       </c>
@@ -20340,7 +20359,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>4320</v>
       </c>
@@ -20837,6 +20856,9 @@
       <c r="B114" t="s">
         <v>4116</v>
       </c>
+      <c r="C114" t="s">
+        <v>4310</v>
+      </c>
       <c r="D114" t="s">
         <v>4110</v>
       </c>
@@ -22843,7 +22865,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>4320</v>
       </c>
@@ -23590,7 +23612,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>4312</v>
       </c>
@@ -24081,7 +24103,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="167" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>4320</v>
       </c>
@@ -24149,7 +24171,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="168" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>4320</v>
       </c>
@@ -24537,6 +24559,9 @@
       <c r="B174" t="s">
         <v>4332</v>
       </c>
+      <c r="C174" t="s">
+        <v>4311</v>
+      </c>
       <c r="D174" t="s">
         <v>4110</v>
       </c>
@@ -25030,6 +25055,9 @@
       <c r="B183" t="s">
         <v>4328</v>
       </c>
+      <c r="C183" t="s">
+        <v>4311</v>
+      </c>
       <c r="D183" t="s">
         <v>4110</v>
       </c>
@@ -25052,7 +25080,7 @@
         <v>4328</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>4312</v>
       </c>
@@ -25088,7 +25116,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>4320</v>
       </c>
@@ -25327,7 +25355,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>4312</v>
       </c>
@@ -25410,7 +25438,7 @@
         <v>54913</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>4312</v>
       </c>
@@ -25818,7 +25846,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>4312</v>
       </c>
@@ -27002,7 +27030,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>4312</v>
       </c>
@@ -28771,6 +28799,9 @@
       <c r="B248" t="s">
         <v>4117</v>
       </c>
+      <c r="C248" t="s">
+        <v>4304</v>
+      </c>
       <c r="D248" t="s">
         <v>4110</v>
       </c>
@@ -28864,7 +28895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>4312</v>
       </c>
@@ -29009,7 +29040,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>4312</v>
       </c>
@@ -29364,7 +29395,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>4312</v>
       </c>
@@ -29657,7 +29688,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>4320</v>
       </c>
@@ -31335,6 +31366,9 @@
       <c r="B291" t="s">
         <v>4114</v>
       </c>
+      <c r="C291" t="s">
+        <v>4304</v>
+      </c>
       <c r="D291" t="s">
         <v>4110</v>
       </c>
@@ -31367,6 +31401,9 @@
       <c r="B292" t="s">
         <v>168</v>
       </c>
+      <c r="C292" t="s">
+        <v>4308</v>
+      </c>
       <c r="D292" t="s">
         <v>1006</v>
       </c>
@@ -32015,7 +32052,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="303" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>4320</v>
       </c>
@@ -32263,7 +32300,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="307" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>4312</v>
       </c>
@@ -33349,7 +33386,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="326" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>4320</v>
       </c>
@@ -33709,7 +33746,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="332" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>4320</v>
       </c>
@@ -34022,7 +34059,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="337" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>4312</v>
       </c>
@@ -34241,7 +34278,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="341" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>4312</v>
       </c>
@@ -34336,7 +34373,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="343" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>4320</v>
       </c>
@@ -34572,7 +34609,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="347" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>4312</v>
       </c>
@@ -34906,7 +34943,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="353" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>4320</v>
       </c>
@@ -35343,7 +35380,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="360" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>4312</v>
       </c>
@@ -35639,7 +35676,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="365" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>4320</v>
       </c>
@@ -35763,7 +35800,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="367" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>4312</v>
       </c>
@@ -35923,7 +35960,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="370" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>4312</v>
       </c>
@@ -36647,7 +36684,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="382" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>4320</v>
       </c>
@@ -36768,7 +36805,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="384" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>4320</v>
       </c>
@@ -37503,7 +37540,7 @@
         <v>54907</v>
       </c>
     </row>
-    <row r="396" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>4312</v>
       </c>
@@ -37598,7 +37635,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="398" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>4312</v>
       </c>
@@ -37945,6 +37982,9 @@
       <c r="B404" t="s">
         <v>4112</v>
       </c>
+      <c r="C404" t="s">
+        <v>4357</v>
+      </c>
       <c r="D404" t="s">
         <v>4110</v>
       </c>
@@ -38289,7 +38329,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="410" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>4320</v>
       </c>
@@ -39125,7 +39165,7 @@
         <v>91513</v>
       </c>
     </row>
-    <row r="424" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>4320</v>
       </c>
@@ -39252,7 +39292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="426" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>4320</v>
       </c>
@@ -40333,7 +40373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="443" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>4312</v>
       </c>
@@ -40369,7 +40409,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="444" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>4312</v>
       </c>
@@ -40405,7 +40445,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="445" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>4312</v>
       </c>
@@ -40500,7 +40540,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="447" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>4320</v>
       </c>
@@ -40789,7 +40829,7 @@
         <v>54906</v>
       </c>
     </row>
-    <row r="452" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>4312</v>
       </c>
@@ -40881,7 +40921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="454" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>4312</v>
       </c>
@@ -40964,7 +41004,7 @@
         <v>54914</v>
       </c>
     </row>
-    <row r="456" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>4312</v>
       </c>
@@ -41394,6 +41434,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AD463" xr:uid="{4F3B871C-5D88-4776-ABC1-BB4125ADD1C8}">
+    <filterColumn colId="13">
+      <filters blank="1"/>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD463">
       <sortCondition descending="1" ref="H1:H463"/>
     </sortState>

</xml_diff>